<commit_message>
Add memory index register
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF20433A-22BA-4B19-AF13-810DB6F687F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847151E-6198-4B9B-A65E-53130348C6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="149">
   <si>
     <t>MODE B</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>PC_1</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Stores the most significant 8 bit of the memory address</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="192">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1577,10 +1583,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1606,6 +1608,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1642,44 +1683,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1690,69 +1755,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1771,6 +1773,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2105,10 +2109,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F30110-9AA6-4607-84AE-181659F51D05}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2120,17 +2124,17 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="128" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="135" t="s">
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="131" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="135" t="s">
+      <c r="H2" s="131" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2150,8 +2154,8 @@
       <c r="F3" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="136"/>
-      <c r="H3" s="136"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -2607,6 +2611,14 @@
       </c>
       <c r="H19" s="32" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>147</v>
+      </c>
+      <c r="H21" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2733,73 +2745,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="147"/>
-      <c r="E3" s="147"/>
-      <c r="F3" s="147"/>
-      <c r="G3" s="148"/>
-      <c r="H3" s="143" t="s">
+      <c r="D3" s="156"/>
+      <c r="E3" s="156"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="152" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="144"/>
-      <c r="J3" s="145"/>
-      <c r="K3" s="143" t="s">
+      <c r="I3" s="153"/>
+      <c r="J3" s="154"/>
+      <c r="K3" s="152" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="155" t="s">
+      <c r="L3" s="153"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="156"/>
-      <c r="P3" s="157"/>
+      <c r="O3" s="140"/>
+      <c r="P3" s="141"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="149" t="s">
+      <c r="S3" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="150"/>
-      <c r="U3" s="150"/>
-      <c r="V3" s="150"/>
-      <c r="W3" s="150"/>
-      <c r="X3" s="150"/>
-      <c r="Y3" s="150"/>
-      <c r="Z3" s="151"/>
-      <c r="AA3" s="152" t="s">
+      <c r="T3" s="134"/>
+      <c r="U3" s="134"/>
+      <c r="V3" s="134"/>
+      <c r="W3" s="134"/>
+      <c r="X3" s="134"/>
+      <c r="Y3" s="134"/>
+      <c r="Z3" s="135"/>
+      <c r="AA3" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="153"/>
-      <c r="AC3" s="153"/>
-      <c r="AD3" s="153"/>
-      <c r="AE3" s="153"/>
-      <c r="AF3" s="153"/>
-      <c r="AG3" s="153"/>
-      <c r="AH3" s="154"/>
+      <c r="AB3" s="137"/>
+      <c r="AC3" s="137"/>
+      <c r="AD3" s="137"/>
+      <c r="AE3" s="137"/>
+      <c r="AF3" s="137"/>
+      <c r="AG3" s="137"/>
+      <c r="AH3" s="138"/>
     </row>
     <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="160" t="s">
+      <c r="B5" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="158" t="s">
+      <c r="C5" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="158"/>
-      <c r="E5" s="158"/>
-      <c r="F5" s="158"/>
-      <c r="G5" s="158"/>
-      <c r="H5" s="158"/>
-      <c r="I5" s="158"/>
-      <c r="J5" s="159"/>
+      <c r="D5" s="142"/>
+      <c r="E5" s="142"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
+      <c r="I5" s="142"/>
+      <c r="J5" s="143"/>
     </row>
     <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="161"/>
+      <c r="B6" s="145"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -2829,16 +2841,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="137" t="s">
+      <c r="C7" s="146" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="138"/>
-      <c r="E7" s="138"/>
-      <c r="F7" s="138"/>
-      <c r="G7" s="138"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="138"/>
-      <c r="J7" s="139"/>
+      <c r="D7" s="147"/>
+      <c r="E7" s="147"/>
+      <c r="F7" s="147"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="147"/>
+      <c r="I7" s="147"/>
+      <c r="J7" s="148"/>
     </row>
     <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
@@ -2848,25 +2860,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="140" t="s">
+      <c r="G8" s="149" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="141"/>
-      <c r="I8" s="141"/>
-      <c r="J8" s="142"/>
+      <c r="H8" s="150"/>
+      <c r="I8" s="150"/>
+      <c r="J8" s="151"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2877,8 +2889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B20B11-9266-4E5E-A2B3-3496A1A10C3B}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26:N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,29 +2906,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="135" t="s">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="162" t="s">
+      <c r="J2" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="135" t="s">
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="N2" s="135" t="s">
+      <c r="N2" s="131" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2939,8 +2951,8 @@
       <c r="G3" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
       <c r="J3" s="59" t="s">
         <v>3</v>
       </c>
@@ -2950,8 +2962,8 @@
       <c r="L3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="93">
@@ -2977,7 +2989,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="165" t="s">
+      <c r="H4" s="160" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="79" t="s">
@@ -3023,7 +3035,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="166"/>
+      <c r="H5" s="159"/>
       <c r="I5" s="53" t="s">
         <v>3</v>
       </c>
@@ -3067,25 +3079,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="158" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="76" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="162" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="170" t="s">
+      <c r="K6" s="171" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="172" t="s">
+      <c r="L6" s="168" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="180" t="s">
+      <c r="M6" s="173" t="s">
         <v>118</v>
       </c>
-      <c r="N6" s="174" t="s">
+      <c r="N6" s="176" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3113,15 +3125,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="167"/>
+      <c r="H7" s="158"/>
       <c r="I7" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="168"/>
-      <c r="K7" s="170"/>
-      <c r="L7" s="172"/>
-      <c r="M7" s="181"/>
-      <c r="N7" s="174"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="174"/>
+      <c r="N7" s="176"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="94">
@@ -3147,15 +3159,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="167"/>
+      <c r="H8" s="158"/>
       <c r="I8" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="168"/>
-      <c r="K8" s="170"/>
-      <c r="L8" s="172"/>
-      <c r="M8" s="181"/>
-      <c r="N8" s="174"/>
+      <c r="J8" s="162"/>
+      <c r="K8" s="171"/>
+      <c r="L8" s="168"/>
+      <c r="M8" s="174"/>
+      <c r="N8" s="176"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="94">
@@ -3181,15 +3193,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="167"/>
+      <c r="H9" s="158"/>
       <c r="I9" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="168"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="172"/>
-      <c r="M9" s="181"/>
-      <c r="N9" s="174"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="168"/>
+      <c r="M9" s="174"/>
+      <c r="N9" s="176"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="94">
@@ -3215,15 +3227,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="167"/>
+      <c r="H10" s="158"/>
       <c r="I10" s="104" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="168"/>
-      <c r="K10" s="170"/>
-      <c r="L10" s="172"/>
-      <c r="M10" s="181"/>
-      <c r="N10" s="174"/>
+      <c r="J10" s="162"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="174"/>
+      <c r="N10" s="176"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="95">
@@ -3249,15 +3261,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="166"/>
+      <c r="H11" s="159"/>
       <c r="I11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="169"/>
-      <c r="K11" s="171"/>
-      <c r="L11" s="173"/>
-      <c r="M11" s="182"/>
-      <c r="N11" s="175"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="169"/>
+      <c r="M11" s="175"/>
+      <c r="N11" s="177"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="93">
@@ -3283,25 +3295,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="165" t="s">
+      <c r="H12" s="160" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="176" t="s">
+      <c r="J12" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="177" t="s">
+      <c r="K12" s="170" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="178" t="s">
+      <c r="L12" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="165" t="s">
+      <c r="M12" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="N12" s="179" t="s">
+      <c r="N12" s="178" t="s">
         <v>106</v>
       </c>
     </row>
@@ -3329,15 +3341,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="167"/>
+      <c r="H13" s="158"/>
       <c r="I13" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="168"/>
-      <c r="K13" s="170"/>
-      <c r="L13" s="172"/>
-      <c r="M13" s="167"/>
-      <c r="N13" s="174"/>
+      <c r="J13" s="162"/>
+      <c r="K13" s="171"/>
+      <c r="L13" s="168"/>
+      <c r="M13" s="158"/>
+      <c r="N13" s="176"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="94">
@@ -3363,15 +3375,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="167"/>
+      <c r="H14" s="158"/>
       <c r="I14" s="104" t="s">
         <v>104</v>
       </c>
-      <c r="J14" s="168"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="172"/>
-      <c r="M14" s="167"/>
-      <c r="N14" s="174"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="171"/>
+      <c r="L14" s="168"/>
+      <c r="M14" s="158"/>
+      <c r="N14" s="176"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="95">
@@ -3397,15 +3409,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="166"/>
+      <c r="H15" s="159"/>
       <c r="I15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="169"/>
-      <c r="K15" s="171"/>
-      <c r="L15" s="173"/>
-      <c r="M15" s="166"/>
-      <c r="N15" s="175"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="159"/>
+      <c r="N15" s="177"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="93">
@@ -3431,22 +3443,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="165" t="s">
+      <c r="H16" s="160" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="176" t="s">
+      <c r="J16" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="183" t="s">
+      <c r="K16" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="178" t="s">
+      <c r="L16" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="165" t="s">
+      <c r="M16" s="160" t="s">
         <v>119</v>
       </c>
       <c r="N16" s="87" t="s">
@@ -3477,14 +3489,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="167"/>
+      <c r="H17" s="158"/>
       <c r="I17" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="168"/>
-      <c r="K17" s="184"/>
-      <c r="L17" s="172"/>
-      <c r="M17" s="167"/>
+      <c r="J17" s="162"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="168"/>
+      <c r="M17" s="158"/>
       <c r="N17" s="86" t="s">
         <v>107</v>
       </c>
@@ -3513,14 +3525,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="167"/>
+      <c r="H18" s="158"/>
       <c r="I18" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="168"/>
-      <c r="K18" s="184"/>
-      <c r="L18" s="172"/>
-      <c r="M18" s="167"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="165"/>
+      <c r="L18" s="168"/>
+      <c r="M18" s="158"/>
       <c r="N18" s="86" t="s">
         <v>109</v>
       </c>
@@ -3549,14 +3561,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="166"/>
+      <c r="H19" s="159"/>
       <c r="I19" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="169"/>
-      <c r="K19" s="185"/>
-      <c r="L19" s="173"/>
-      <c r="M19" s="166"/>
+      <c r="J19" s="163"/>
+      <c r="K19" s="166"/>
+      <c r="L19" s="169"/>
+      <c r="M19" s="159"/>
       <c r="N19" s="55" t="s">
         <v>110</v>
       </c>
@@ -3586,22 +3598,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="165" t="s">
+      <c r="H20" s="160" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="176" t="s">
+      <c r="J20" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="177" t="s">
+      <c r="K20" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="178" t="s">
+      <c r="L20" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="180" t="s">
+      <c r="M20" s="173" t="s">
         <v>118</v>
       </c>
       <c r="N20" s="52" t="s">
@@ -3632,14 +3644,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="167"/>
+      <c r="H21" s="158"/>
       <c r="I21" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="168"/>
-      <c r="K21" s="170"/>
-      <c r="L21" s="172"/>
-      <c r="M21" s="181"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="171"/>
+      <c r="L21" s="168"/>
+      <c r="M21" s="174"/>
       <c r="N21" s="86" t="s">
         <v>101</v>
       </c>
@@ -3668,14 +3680,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="167"/>
+      <c r="H22" s="158"/>
       <c r="I22" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="168"/>
-      <c r="K22" s="170"/>
-      <c r="L22" s="172"/>
-      <c r="M22" s="181"/>
+      <c r="J22" s="162"/>
+      <c r="K22" s="171"/>
+      <c r="L22" s="168"/>
+      <c r="M22" s="174"/>
       <c r="N22" s="86" t="s">
         <v>102</v>
       </c>
@@ -3704,14 +3716,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="166"/>
+      <c r="H23" s="159"/>
       <c r="I23" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="169"/>
-      <c r="K23" s="171"/>
-      <c r="L23" s="173"/>
-      <c r="M23" s="182"/>
+      <c r="J23" s="163"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="169"/>
+      <c r="M23" s="175"/>
       <c r="N23" s="52" t="s">
         <v>103</v>
       </c>
@@ -3740,7 +3752,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="165" t="s">
+      <c r="H24" s="160" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="76" t="s">
@@ -3786,14 +3798,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="167"/>
+      <c r="H25" s="158"/>
       <c r="I25" s="82" t="s">
         <v>46</v>
       </c>
       <c r="J25" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="K25" s="126" t="s">
+      <c r="K25" s="122" t="s">
         <v>16</v>
       </c>
       <c r="L25" s="120" t="s">
@@ -3830,15 +3842,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="167"/>
-      <c r="I26" s="127" t="s">
+      <c r="H26" s="158"/>
+      <c r="I26" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="J26" s="128"/>
-      <c r="K26" s="129"/>
-      <c r="L26" s="130"/>
-      <c r="M26" s="131"/>
-      <c r="N26" s="131"/>
+      <c r="J26" s="124"/>
+      <c r="K26" s="125"/>
+      <c r="L26" s="126"/>
+      <c r="M26" s="127"/>
+      <c r="N26" s="127"/>
     </row>
     <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="95">
@@ -3864,15 +3876,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="166"/>
-      <c r="I27" s="114" t="s">
+      <c r="H27" s="159"/>
+      <c r="I27" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="J27" s="122"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="124"/>
-      <c r="M27" s="125"/>
-      <c r="N27" s="125"/>
+      <c r="J27" s="188"/>
+      <c r="K27" s="189"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="55"/>
+      <c r="N27" s="55"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="93">
@@ -3898,7 +3910,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="165" t="s">
+      <c r="H28" s="160" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="46" t="s">
@@ -3944,7 +3956,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="167"/>
+      <c r="H29" s="158"/>
       <c r="I29" s="82" t="s">
         <v>52</v>
       </c>
@@ -3988,7 +4000,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="167"/>
+      <c r="H30" s="158"/>
       <c r="I30" s="82" t="s">
         <v>53</v>
       </c>
@@ -4032,7 +4044,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="166"/>
+      <c r="H31" s="159"/>
       <c r="I31" s="106" t="s">
         <v>125</v>
       </c>
@@ -4066,7 +4078,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="167" t="s">
+      <c r="H32" s="158" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="76" t="s">
@@ -4113,7 +4125,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="167"/>
+      <c r="H33" s="158"/>
       <c r="I33" s="82" t="s">
         <v>24</v>
       </c>
@@ -4158,7 +4170,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="166"/>
+      <c r="H34" s="159"/>
       <c r="I34" s="114" t="s">
         <v>126</v>
       </c>
@@ -4217,11 +4229,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4230,25 +4256,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4270,13 +4282,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="179" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="135" t="s">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="131" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4293,7 +4305,7 @@
       <c r="E3" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="136"/>
+      <c r="F3" s="132"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
@@ -4479,22 +4491,22 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="131" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="188" t="s">
+      <c r="C2" s="184" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="188"/>
-      <c r="G2" s="188"/>
-      <c r="H2" s="188"/>
-      <c r="I2" s="188"/>
-      <c r="J2" s="189"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="185"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="136"/>
+      <c r="B3" s="132"/>
       <c r="C3" s="98">
         <v>7</v>
       </c>
@@ -4533,73 +4545,73 @@
       <c r="E4" s="101" t="s">
         <v>88</v>
       </c>
-      <c r="F4" s="190" t="s">
+      <c r="F4" s="186" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="190"/>
-      <c r="H4" s="190"/>
-      <c r="I4" s="190"/>
-      <c r="J4" s="191"/>
+      <c r="G4" s="186"/>
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="187"/>
     </row>
     <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="186" t="s">
+      <c r="C5" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="D5" s="186"/>
-      <c r="E5" s="186"/>
-      <c r="F5" s="186"/>
-      <c r="G5" s="186"/>
-      <c r="H5" s="186"/>
-      <c r="I5" s="186"/>
-      <c r="J5" s="187"/>
+      <c r="D5" s="182"/>
+      <c r="E5" s="182"/>
+      <c r="F5" s="182"/>
+      <c r="G5" s="182"/>
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="183"/>
     </row>
     <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="186" t="s">
+      <c r="C6" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="186"/>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
-      <c r="I6" s="186"/>
-      <c r="J6" s="187"/>
+      <c r="D6" s="182"/>
+      <c r="E6" s="182"/>
+      <c r="F6" s="182"/>
+      <c r="G6" s="182"/>
+      <c r="H6" s="182"/>
+      <c r="I6" s="182"/>
+      <c r="J6" s="183"/>
     </row>
     <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="102" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="186" t="s">
+      <c r="C7" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="186"/>
-      <c r="E7" s="186"/>
-      <c r="F7" s="186"/>
-      <c r="G7" s="186"/>
-      <c r="H7" s="186"/>
-      <c r="I7" s="186"/>
-      <c r="J7" s="187"/>
+      <c r="D7" s="182"/>
+      <c r="E7" s="182"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="182"/>
+      <c r="H7" s="182"/>
+      <c r="I7" s="182"/>
+      <c r="J7" s="183"/>
     </row>
     <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="186" t="s">
+      <c r="C8" s="182" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="186"/>
-      <c r="E8" s="186"/>
-      <c r="F8" s="186"/>
-      <c r="G8" s="186"/>
-      <c r="H8" s="186"/>
-      <c r="I8" s="186"/>
-      <c r="J8" s="187"/>
+      <c r="D8" s="182"/>
+      <c r="E8" s="182"/>
+      <c r="F8" s="182"/>
+      <c r="G8" s="182"/>
+      <c r="H8" s="182"/>
+      <c r="I8" s="182"/>
+      <c r="J8" s="183"/>
       <c r="K8" t="s">
         <v>93</v>
       </c>
@@ -4723,29 +4735,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="179" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="163"/>
-      <c r="F2" s="163"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="135" t="s">
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="131" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="135" t="s">
+      <c r="I2" s="131" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="162" t="s">
+      <c r="J2" s="179" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="163"/>
-      <c r="L2" s="163"/>
-      <c r="M2" s="135" t="s">
+      <c r="K2" s="180"/>
+      <c r="L2" s="180"/>
+      <c r="M2" s="131" t="s">
         <v>117</v>
       </c>
-      <c r="N2" s="135" t="s">
+      <c r="N2" s="131" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4768,8 +4780,8 @@
       <c r="G3" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="136"/>
-      <c r="I3" s="136"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
       <c r="J3" s="59" t="s">
         <v>3</v>
       </c>
@@ -4779,8 +4791,8 @@
       <c r="L3" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="136"/>
-      <c r="N3" s="136"/>
+      <c r="M3" s="132"/>
+      <c r="N3" s="132"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="93">
@@ -4806,7 +4818,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="165" t="s">
+      <c r="H4" s="160" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="79" t="s">
@@ -4852,7 +4864,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="166"/>
+      <c r="H5" s="159"/>
       <c r="I5" s="53" t="s">
         <v>3</v>
       </c>
@@ -4896,25 +4908,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="158" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="162" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="170" t="s">
+      <c r="K6" s="171" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="172" t="s">
+      <c r="L6" s="168" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="180" t="s">
+      <c r="M6" s="173" t="s">
         <v>118</v>
       </c>
-      <c r="N6" s="174" t="s">
+      <c r="N6" s="176" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4942,15 +4954,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="167"/>
+      <c r="H7" s="158"/>
       <c r="I7" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="168"/>
-      <c r="K7" s="170"/>
-      <c r="L7" s="172"/>
-      <c r="M7" s="181"/>
-      <c r="N7" s="174"/>
+      <c r="J7" s="162"/>
+      <c r="K7" s="171"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="174"/>
+      <c r="N7" s="176"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="94">
@@ -4976,15 +4988,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="167"/>
+      <c r="H8" s="158"/>
       <c r="I8" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="168"/>
-      <c r="K8" s="170"/>
-      <c r="L8" s="172"/>
-      <c r="M8" s="181"/>
-      <c r="N8" s="174"/>
+      <c r="J8" s="162"/>
+      <c r="K8" s="171"/>
+      <c r="L8" s="168"/>
+      <c r="M8" s="174"/>
+      <c r="N8" s="176"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="94">
@@ -5010,15 +5022,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="167"/>
+      <c r="H9" s="158"/>
       <c r="I9" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="168"/>
-      <c r="K9" s="170"/>
-      <c r="L9" s="172"/>
-      <c r="M9" s="181"/>
-      <c r="N9" s="174"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="168"/>
+      <c r="M9" s="174"/>
+      <c r="N9" s="176"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="94">
@@ -5044,15 +5056,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="167"/>
+      <c r="H10" s="158"/>
       <c r="I10" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="168"/>
-      <c r="K10" s="170"/>
-      <c r="L10" s="172"/>
-      <c r="M10" s="181"/>
-      <c r="N10" s="174"/>
+      <c r="J10" s="162"/>
+      <c r="K10" s="171"/>
+      <c r="L10" s="168"/>
+      <c r="M10" s="174"/>
+      <c r="N10" s="176"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="95">
@@ -5078,15 +5090,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="166"/>
+      <c r="H11" s="159"/>
       <c r="I11" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="169"/>
-      <c r="K11" s="171"/>
-      <c r="L11" s="173"/>
-      <c r="M11" s="182"/>
-      <c r="N11" s="175"/>
+      <c r="J11" s="163"/>
+      <c r="K11" s="172"/>
+      <c r="L11" s="169"/>
+      <c r="M11" s="175"/>
+      <c r="N11" s="177"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="93">
@@ -5112,25 +5124,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="165" t="s">
+      <c r="H12" s="160" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="176" t="s">
+      <c r="J12" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="177" t="s">
+      <c r="K12" s="170" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="178" t="s">
+      <c r="L12" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="165" t="s">
+      <c r="M12" s="160" t="s">
         <v>119</v>
       </c>
-      <c r="N12" s="179" t="s">
+      <c r="N12" s="178" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5158,15 +5170,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="167"/>
+      <c r="H13" s="158"/>
       <c r="I13" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="168"/>
-      <c r="K13" s="170"/>
-      <c r="L13" s="172"/>
-      <c r="M13" s="167"/>
-      <c r="N13" s="174"/>
+      <c r="J13" s="162"/>
+      <c r="K13" s="171"/>
+      <c r="L13" s="168"/>
+      <c r="M13" s="158"/>
+      <c r="N13" s="176"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="94">
@@ -5192,15 +5204,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="167"/>
+      <c r="H14" s="158"/>
       <c r="I14" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="J14" s="168"/>
-      <c r="K14" s="170"/>
-      <c r="L14" s="172"/>
-      <c r="M14" s="167"/>
-      <c r="N14" s="174"/>
+      <c r="J14" s="162"/>
+      <c r="K14" s="171"/>
+      <c r="L14" s="168"/>
+      <c r="M14" s="158"/>
+      <c r="N14" s="176"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="95">
@@ -5226,15 +5238,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="166"/>
+      <c r="H15" s="159"/>
       <c r="I15" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="169"/>
-      <c r="K15" s="171"/>
-      <c r="L15" s="173"/>
-      <c r="M15" s="166"/>
-      <c r="N15" s="175"/>
+      <c r="J15" s="163"/>
+      <c r="K15" s="172"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="159"/>
+      <c r="N15" s="177"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="93">
@@ -5260,22 +5272,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="165" t="s">
+      <c r="H16" s="160" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="176" t="s">
+      <c r="J16" s="161" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="183" t="s">
+      <c r="K16" s="164" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="178" t="s">
+      <c r="L16" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="165" t="s">
+      <c r="M16" s="160" t="s">
         <v>119</v>
       </c>
       <c r="N16" s="48" t="s">
@@ -5306,14 +5318,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="167"/>
+      <c r="H17" s="158"/>
       <c r="I17" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="168"/>
-      <c r="K17" s="184"/>
-      <c r="L17" s="172"/>
-      <c r="M17" s="167"/>
+      <c r="J17" s="162"/>
+      <c r="K17" s="165"/>
+      <c r="L17" s="168"/>
+      <c r="M17" s="158"/>
       <c r="N17" s="52" t="s">
         <v>107</v>
       </c>
@@ -5342,14 +5354,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="167"/>
+      <c r="H18" s="158"/>
       <c r="I18" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="168"/>
-      <c r="K18" s="184"/>
-      <c r="L18" s="172"/>
-      <c r="M18" s="167"/>
+      <c r="J18" s="162"/>
+      <c r="K18" s="165"/>
+      <c r="L18" s="168"/>
+      <c r="M18" s="158"/>
       <c r="N18" s="52" t="s">
         <v>109</v>
       </c>
@@ -5378,14 +5390,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="166"/>
+      <c r="H19" s="159"/>
       <c r="I19" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="169"/>
-      <c r="K19" s="185"/>
-      <c r="L19" s="173"/>
-      <c r="M19" s="166"/>
+      <c r="J19" s="163"/>
+      <c r="K19" s="166"/>
+      <c r="L19" s="169"/>
+      <c r="M19" s="159"/>
       <c r="N19" s="55" t="s">
         <v>110</v>
       </c>
@@ -5414,22 +5426,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="165" t="s">
+      <c r="H20" s="160" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="176" t="s">
+      <c r="J20" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="177" t="s">
+      <c r="K20" s="170" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="178" t="s">
+      <c r="L20" s="167" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="180" t="s">
+      <c r="M20" s="173" t="s">
         <v>118</v>
       </c>
       <c r="N20" s="52" t="s">
@@ -5460,14 +5472,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="167"/>
+      <c r="H21" s="158"/>
       <c r="I21" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="168"/>
-      <c r="K21" s="170"/>
-      <c r="L21" s="172"/>
-      <c r="M21" s="181"/>
+      <c r="J21" s="162"/>
+      <c r="K21" s="171"/>
+      <c r="L21" s="168"/>
+      <c r="M21" s="174"/>
       <c r="N21" s="86" t="s">
         <v>101</v>
       </c>
@@ -5496,14 +5508,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="167"/>
+      <c r="H22" s="158"/>
       <c r="I22" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="168"/>
-      <c r="K22" s="170"/>
-      <c r="L22" s="172"/>
-      <c r="M22" s="181"/>
+      <c r="J22" s="162"/>
+      <c r="K22" s="171"/>
+      <c r="L22" s="168"/>
+      <c r="M22" s="174"/>
       <c r="N22" s="86" t="s">
         <v>102</v>
       </c>
@@ -5532,14 +5544,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="166"/>
+      <c r="H23" s="159"/>
       <c r="I23" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="169"/>
-      <c r="K23" s="171"/>
-      <c r="L23" s="173"/>
-      <c r="M23" s="182"/>
+      <c r="J23" s="163"/>
+      <c r="K23" s="172"/>
+      <c r="L23" s="169"/>
+      <c r="M23" s="175"/>
       <c r="N23" s="52" t="s">
         <v>103</v>
       </c>
@@ -5568,7 +5580,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="165" t="s">
+      <c r="H24" s="160" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="76" t="s">
@@ -5614,7 +5626,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="166"/>
+      <c r="H25" s="159"/>
       <c r="I25" s="49" t="s">
         <v>46</v>
       </c>
@@ -5658,7 +5670,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="165" t="s">
+      <c r="H26" s="160" t="s">
         <v>59</v>
       </c>
       <c r="I26" s="76" t="s">
@@ -5705,7 +5717,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="166"/>
+      <c r="H27" s="159"/>
       <c r="I27" s="53" t="s">
         <v>24</v>
       </c>
@@ -5749,7 +5761,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="165" t="s">
+      <c r="H28" s="160" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="46" t="s">
@@ -5795,7 +5807,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="167"/>
+      <c r="H29" s="158"/>
       <c r="I29" s="82" t="s">
         <v>52</v>
       </c>
@@ -5839,7 +5851,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30" s="166"/>
+      <c r="H30" s="159"/>
       <c r="I30" s="53" t="s">
         <v>53</v>
       </c>
@@ -6038,6 +6050,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="M16:M19"/>
     <mergeCell ref="M20:M23"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="H24:H25"/>
@@ -6050,26 +6082,6 @@
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="H16:H19"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="H20:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add baud rate docs
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F82BDC-E079-4297-A546-B9A36032A5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A587625A-3939-4290-8478-BFA201804500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -1615,6 +1615,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1654,94 +1690,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1750,17 +1732,35 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2117,7 +2117,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2750,73 +2750,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="161" t="s">
+      <c r="C3" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="163"/>
-      <c r="H3" s="158" t="s">
+      <c r="D3" s="149"/>
+      <c r="E3" s="149"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="145" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="159"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="158" t="s">
+      <c r="I3" s="146"/>
+      <c r="J3" s="147"/>
+      <c r="K3" s="145" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="159"/>
-      <c r="M3" s="159"/>
-      <c r="N3" s="145" t="s">
+      <c r="L3" s="146"/>
+      <c r="M3" s="146"/>
+      <c r="N3" s="157" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="146"/>
-      <c r="P3" s="147"/>
+      <c r="O3" s="158"/>
+      <c r="P3" s="159"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="139" t="s">
+      <c r="S3" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="140"/>
-      <c r="U3" s="140"/>
-      <c r="V3" s="140"/>
-      <c r="W3" s="140"/>
-      <c r="X3" s="140"/>
-      <c r="Y3" s="140"/>
-      <c r="Z3" s="141"/>
-      <c r="AA3" s="142" t="s">
+      <c r="T3" s="152"/>
+      <c r="U3" s="152"/>
+      <c r="V3" s="152"/>
+      <c r="W3" s="152"/>
+      <c r="X3" s="152"/>
+      <c r="Y3" s="152"/>
+      <c r="Z3" s="153"/>
+      <c r="AA3" s="154" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="143"/>
-      <c r="AC3" s="143"/>
-      <c r="AD3" s="143"/>
-      <c r="AE3" s="143"/>
-      <c r="AF3" s="143"/>
-      <c r="AG3" s="143"/>
-      <c r="AH3" s="144"/>
+      <c r="AB3" s="155"/>
+      <c r="AC3" s="155"/>
+      <c r="AD3" s="155"/>
+      <c r="AE3" s="155"/>
+      <c r="AF3" s="155"/>
+      <c r="AG3" s="155"/>
+      <c r="AH3" s="156"/>
     </row>
     <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="162" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="148"/>
-      <c r="E5" s="148"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
-      <c r="I5" s="148"/>
-      <c r="J5" s="149"/>
+      <c r="D5" s="160"/>
+      <c r="E5" s="160"/>
+      <c r="F5" s="160"/>
+      <c r="G5" s="160"/>
+      <c r="H5" s="160"/>
+      <c r="I5" s="160"/>
+      <c r="J5" s="161"/>
     </row>
     <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="151"/>
+      <c r="B6" s="163"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -2846,16 +2846,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="139" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="153"/>
-      <c r="E7" s="153"/>
-      <c r="F7" s="153"/>
-      <c r="G7" s="153"/>
-      <c r="H7" s="153"/>
-      <c r="I7" s="153"/>
-      <c r="J7" s="154"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="141"/>
     </row>
     <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
@@ -2865,12 +2865,12 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="155" t="s">
+      <c r="G8" s="142" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="156"/>
-      <c r="I8" s="156"/>
-      <c r="J8" s="157"/>
+      <c r="H8" s="143"/>
+      <c r="I8" s="143"/>
+      <c r="J8" s="144"/>
     </row>
     <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="G10">
@@ -2882,16 +2882,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="S3:Z3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2919,25 +2919,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="187"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="166"/>
       <c r="H2" s="137" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="185" t="s">
+      <c r="J2" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="186"/>
-      <c r="L2" s="186"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
       <c r="M2" s="137" t="s">
         <v>116</v>
       </c>
@@ -3002,7 +3002,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="166" t="s">
+      <c r="H4" s="167" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="78" t="s">
@@ -3048,7 +3048,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="165"/>
+      <c r="H5" s="168"/>
       <c r="I5" s="52" t="s">
         <v>3</v>
       </c>
@@ -3092,25 +3092,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="169" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="170" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="177" t="s">
+      <c r="K6" s="172" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="174" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="179" t="s">
+      <c r="M6" s="182" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="182" t="s">
+      <c r="N6" s="176" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3138,15 +3138,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="164"/>
+      <c r="H7" s="169"/>
       <c r="I7" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="168"/>
-      <c r="K7" s="177"/>
+      <c r="J7" s="170"/>
+      <c r="K7" s="172"/>
       <c r="L7" s="174"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="182"/>
+      <c r="M7" s="183"/>
+      <c r="N7" s="176"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="93">
@@ -3172,15 +3172,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="164"/>
+      <c r="H8" s="169"/>
       <c r="I8" s="103" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="168"/>
-      <c r="K8" s="177"/>
+      <c r="J8" s="170"/>
+      <c r="K8" s="172"/>
       <c r="L8" s="174"/>
-      <c r="M8" s="180"/>
-      <c r="N8" s="182"/>
+      <c r="M8" s="183"/>
+      <c r="N8" s="176"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="93">
@@ -3206,15 +3206,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="164"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="103" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="168"/>
-      <c r="K9" s="177"/>
+      <c r="J9" s="170"/>
+      <c r="K9" s="172"/>
       <c r="L9" s="174"/>
-      <c r="M9" s="180"/>
-      <c r="N9" s="182"/>
+      <c r="M9" s="183"/>
+      <c r="N9" s="176"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="93">
@@ -3240,15 +3240,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="164"/>
+      <c r="H10" s="169"/>
       <c r="I10" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="168"/>
-      <c r="K10" s="177"/>
+      <c r="J10" s="170"/>
+      <c r="K10" s="172"/>
       <c r="L10" s="174"/>
-      <c r="M10" s="180"/>
-      <c r="N10" s="182"/>
+      <c r="M10" s="183"/>
+      <c r="N10" s="176"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="94">
@@ -3274,15 +3274,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="165"/>
+      <c r="H11" s="168"/>
       <c r="I11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="169"/>
-      <c r="K11" s="178"/>
+      <c r="J11" s="171"/>
+      <c r="K11" s="173"/>
       <c r="L11" s="175"/>
-      <c r="M11" s="181"/>
-      <c r="N11" s="183"/>
+      <c r="M11" s="184"/>
+      <c r="N11" s="177"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="92">
@@ -3308,25 +3308,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="166" t="s">
+      <c r="H12" s="167" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="167" t="s">
+      <c r="J12" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="176" t="s">
+      <c r="K12" s="179" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="173" t="s">
+      <c r="L12" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="166" t="s">
+      <c r="M12" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="N12" s="184" t="s">
+      <c r="N12" s="181" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3354,15 +3354,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="164"/>
+      <c r="H13" s="169"/>
       <c r="I13" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="168"/>
-      <c r="K13" s="177"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="172"/>
       <c r="L13" s="174"/>
-      <c r="M13" s="164"/>
-      <c r="N13" s="182"/>
+      <c r="M13" s="169"/>
+      <c r="N13" s="176"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="93">
@@ -3388,15 +3388,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="164"/>
+      <c r="H14" s="169"/>
       <c r="I14" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="168"/>
-      <c r="K14" s="177"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="172"/>
       <c r="L14" s="174"/>
-      <c r="M14" s="164"/>
-      <c r="N14" s="182"/>
+      <c r="M14" s="169"/>
+      <c r="N14" s="176"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="94">
@@ -3422,15 +3422,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="165"/>
+      <c r="H15" s="168"/>
       <c r="I15" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="169"/>
-      <c r="K15" s="178"/>
+      <c r="J15" s="171"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="175"/>
-      <c r="M15" s="165"/>
-      <c r="N15" s="183"/>
+      <c r="M15" s="168"/>
+      <c r="N15" s="177"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="92">
@@ -3456,22 +3456,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="166" t="s">
+      <c r="H16" s="167" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="167" t="s">
+      <c r="J16" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="170" t="s">
+      <c r="K16" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="173" t="s">
+      <c r="L16" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="166" t="s">
+      <c r="M16" s="167" t="s">
         <v>118</v>
       </c>
       <c r="N16" s="86" t="s">
@@ -3502,14 +3502,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="164"/>
+      <c r="H17" s="169"/>
       <c r="I17" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="168"/>
-      <c r="K17" s="171"/>
+      <c r="J17" s="170"/>
+      <c r="K17" s="186"/>
       <c r="L17" s="174"/>
-      <c r="M17" s="164"/>
+      <c r="M17" s="169"/>
       <c r="N17" s="85" t="s">
         <v>106</v>
       </c>
@@ -3538,14 +3538,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="164"/>
+      <c r="H18" s="169"/>
       <c r="I18" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="168"/>
-      <c r="K18" s="171"/>
+      <c r="J18" s="170"/>
+      <c r="K18" s="186"/>
       <c r="L18" s="174"/>
-      <c r="M18" s="164"/>
+      <c r="M18" s="169"/>
       <c r="N18" s="85" t="s">
         <v>108</v>
       </c>
@@ -3574,14 +3574,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="165"/>
+      <c r="H19" s="168"/>
       <c r="I19" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="169"/>
-      <c r="K19" s="172"/>
+      <c r="J19" s="171"/>
+      <c r="K19" s="187"/>
       <c r="L19" s="175"/>
-      <c r="M19" s="165"/>
+      <c r="M19" s="168"/>
       <c r="N19" s="54" t="s">
         <v>109</v>
       </c>
@@ -3611,22 +3611,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="166" t="s">
+      <c r="H20" s="167" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="167" t="s">
+      <c r="J20" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="176" t="s">
+      <c r="K20" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="173" t="s">
+      <c r="L20" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="179" t="s">
+      <c r="M20" s="182" t="s">
         <v>117</v>
       </c>
       <c r="N20" s="51" t="s">
@@ -3657,14 +3657,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="164"/>
+      <c r="H21" s="169"/>
       <c r="I21" s="81" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="168"/>
-      <c r="K21" s="177"/>
+      <c r="J21" s="170"/>
+      <c r="K21" s="172"/>
       <c r="L21" s="174"/>
-      <c r="M21" s="180"/>
+      <c r="M21" s="183"/>
       <c r="N21" s="85" t="s">
         <v>100</v>
       </c>
@@ -3693,14 +3693,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="164"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="168"/>
-      <c r="K22" s="177"/>
+      <c r="J22" s="170"/>
+      <c r="K22" s="172"/>
       <c r="L22" s="174"/>
-      <c r="M22" s="180"/>
+      <c r="M22" s="183"/>
       <c r="N22" s="85" t="s">
         <v>101</v>
       </c>
@@ -3729,14 +3729,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="165"/>
+      <c r="H23" s="168"/>
       <c r="I23" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="169"/>
-      <c r="K23" s="178"/>
+      <c r="J23" s="171"/>
+      <c r="K23" s="173"/>
       <c r="L23" s="175"/>
-      <c r="M23" s="181"/>
+      <c r="M23" s="184"/>
       <c r="N23" s="51" t="s">
         <v>102</v>
       </c>
@@ -3765,7 +3765,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="166" t="s">
+      <c r="H24" s="167" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="75" t="s">
@@ -3811,7 +3811,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="164"/>
+      <c r="H25" s="169"/>
       <c r="I25" s="81" t="s">
         <v>46</v>
       </c>
@@ -3855,7 +3855,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="164"/>
+      <c r="H26" s="169"/>
       <c r="I26" s="122" t="s">
         <v>122</v>
       </c>
@@ -3889,7 +3889,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="165"/>
+      <c r="H27" s="168"/>
       <c r="I27" s="52" t="s">
         <v>123</v>
       </c>
@@ -3923,7 +3923,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="166" t="s">
+      <c r="H28" s="167" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="45" t="s">
@@ -3969,7 +3969,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="164"/>
+      <c r="H29" s="169"/>
       <c r="I29" s="81" t="s">
         <v>52</v>
       </c>
@@ -4013,7 +4013,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="164"/>
+      <c r="H30" s="169"/>
       <c r="I30" s="81" t="s">
         <v>53</v>
       </c>
@@ -4057,7 +4057,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="165"/>
+      <c r="H31" s="168"/>
       <c r="I31" s="105" t="s">
         <v>124</v>
       </c>
@@ -4091,7 +4091,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="164" t="s">
+      <c r="H32" s="169" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="75" t="s">
@@ -4138,7 +4138,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="164"/>
+      <c r="H33" s="169"/>
       <c r="I33" s="81" t="s">
         <v>24</v>
       </c>
@@ -4183,7 +4183,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="165"/>
+      <c r="H34" s="168"/>
       <c r="I34" s="113" t="s">
         <v>125</v>
       </c>
@@ -4242,17 +4242,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="M20:M23"/>
     <mergeCell ref="N6:N11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
@@ -4261,19 +4263,17 @@
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
     <mergeCell ref="M6:M11"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4295,12 +4295,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="164" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="187"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="166"/>
       <c r="F2" s="137" t="s">
         <v>32</v>
       </c>
@@ -4494,7 +4494,7 @@
   <dimension ref="B1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4746,25 +4746,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="186"/>
-      <c r="E2" s="186"/>
-      <c r="F2" s="186"/>
-      <c r="G2" s="187"/>
+      <c r="C2" s="165"/>
+      <c r="D2" s="165"/>
+      <c r="E2" s="165"/>
+      <c r="F2" s="165"/>
+      <c r="G2" s="166"/>
       <c r="H2" s="137" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="185" t="s">
+      <c r="J2" s="164" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="186"/>
-      <c r="L2" s="186"/>
+      <c r="K2" s="165"/>
+      <c r="L2" s="165"/>
       <c r="M2" s="137" t="s">
         <v>116</v>
       </c>
@@ -4829,7 +4829,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="166" t="s">
+      <c r="H4" s="167" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="78" t="s">
@@ -4875,7 +4875,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="165"/>
+      <c r="H5" s="168"/>
       <c r="I5" s="52" t="s">
         <v>3</v>
       </c>
@@ -4919,25 +4919,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="169" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="168" t="s">
+      <c r="J6" s="170" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="177" t="s">
+      <c r="K6" s="172" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="174" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="179" t="s">
+      <c r="M6" s="182" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="182" t="s">
+      <c r="N6" s="176" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4965,15 +4965,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="164"/>
+      <c r="H7" s="169"/>
       <c r="I7" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="168"/>
-      <c r="K7" s="177"/>
+      <c r="J7" s="170"/>
+      <c r="K7" s="172"/>
       <c r="L7" s="174"/>
-      <c r="M7" s="180"/>
-      <c r="N7" s="182"/>
+      <c r="M7" s="183"/>
+      <c r="N7" s="176"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="93">
@@ -4999,15 +4999,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="164"/>
+      <c r="H8" s="169"/>
       <c r="I8" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="168"/>
-      <c r="K8" s="177"/>
+      <c r="J8" s="170"/>
+      <c r="K8" s="172"/>
       <c r="L8" s="174"/>
-      <c r="M8" s="180"/>
-      <c r="N8" s="182"/>
+      <c r="M8" s="183"/>
+      <c r="N8" s="176"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="93">
@@ -5033,15 +5033,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="164"/>
+      <c r="H9" s="169"/>
       <c r="I9" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="168"/>
-      <c r="K9" s="177"/>
+      <c r="J9" s="170"/>
+      <c r="K9" s="172"/>
       <c r="L9" s="174"/>
-      <c r="M9" s="180"/>
-      <c r="N9" s="182"/>
+      <c r="M9" s="183"/>
+      <c r="N9" s="176"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="93">
@@ -5067,15 +5067,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="164"/>
+      <c r="H10" s="169"/>
       <c r="I10" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="168"/>
-      <c r="K10" s="177"/>
+      <c r="J10" s="170"/>
+      <c r="K10" s="172"/>
       <c r="L10" s="174"/>
-      <c r="M10" s="180"/>
-      <c r="N10" s="182"/>
+      <c r="M10" s="183"/>
+      <c r="N10" s="176"/>
     </row>
     <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="94">
@@ -5101,15 +5101,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="165"/>
+      <c r="H11" s="168"/>
       <c r="I11" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="169"/>
-      <c r="K11" s="178"/>
+      <c r="J11" s="171"/>
+      <c r="K11" s="173"/>
       <c r="L11" s="175"/>
-      <c r="M11" s="181"/>
-      <c r="N11" s="183"/>
+      <c r="M11" s="184"/>
+      <c r="N11" s="177"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="92">
@@ -5135,25 +5135,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="166" t="s">
+      <c r="H12" s="167" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="167" t="s">
+      <c r="J12" s="178" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="176" t="s">
+      <c r="K12" s="179" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="173" t="s">
+      <c r="L12" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="166" t="s">
+      <c r="M12" s="167" t="s">
         <v>118</v>
       </c>
-      <c r="N12" s="184" t="s">
+      <c r="N12" s="181" t="s">
         <v>105</v>
       </c>
     </row>
@@ -5181,15 +5181,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="164"/>
+      <c r="H13" s="169"/>
       <c r="I13" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="168"/>
-      <c r="K13" s="177"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="172"/>
       <c r="L13" s="174"/>
-      <c r="M13" s="164"/>
-      <c r="N13" s="182"/>
+      <c r="M13" s="169"/>
+      <c r="N13" s="176"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="93">
@@ -5215,15 +5215,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="164"/>
+      <c r="H14" s="169"/>
       <c r="I14" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="168"/>
-      <c r="K14" s="177"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="172"/>
       <c r="L14" s="174"/>
-      <c r="M14" s="164"/>
-      <c r="N14" s="182"/>
+      <c r="M14" s="169"/>
+      <c r="N14" s="176"/>
     </row>
     <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="94">
@@ -5249,15 +5249,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="165"/>
+      <c r="H15" s="168"/>
       <c r="I15" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="169"/>
-      <c r="K15" s="178"/>
+      <c r="J15" s="171"/>
+      <c r="K15" s="173"/>
       <c r="L15" s="175"/>
-      <c r="M15" s="165"/>
-      <c r="N15" s="183"/>
+      <c r="M15" s="168"/>
+      <c r="N15" s="177"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="92">
@@ -5283,22 +5283,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="166" t="s">
+      <c r="H16" s="167" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="167" t="s">
+      <c r="J16" s="178" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="170" t="s">
+      <c r="K16" s="185" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="173" t="s">
+      <c r="L16" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="166" t="s">
+      <c r="M16" s="167" t="s">
         <v>118</v>
       </c>
       <c r="N16" s="47" t="s">
@@ -5329,14 +5329,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="164"/>
+      <c r="H17" s="169"/>
       <c r="I17" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="168"/>
-      <c r="K17" s="171"/>
+      <c r="J17" s="170"/>
+      <c r="K17" s="186"/>
       <c r="L17" s="174"/>
-      <c r="M17" s="164"/>
+      <c r="M17" s="169"/>
       <c r="N17" s="51" t="s">
         <v>106</v>
       </c>
@@ -5365,14 +5365,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="164"/>
+      <c r="H18" s="169"/>
       <c r="I18" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="168"/>
-      <c r="K18" s="171"/>
+      <c r="J18" s="170"/>
+      <c r="K18" s="186"/>
       <c r="L18" s="174"/>
-      <c r="M18" s="164"/>
+      <c r="M18" s="169"/>
       <c r="N18" s="51" t="s">
         <v>108</v>
       </c>
@@ -5401,14 +5401,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="165"/>
+      <c r="H19" s="168"/>
       <c r="I19" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="169"/>
-      <c r="K19" s="172"/>
+      <c r="J19" s="171"/>
+      <c r="K19" s="187"/>
       <c r="L19" s="175"/>
-      <c r="M19" s="165"/>
+      <c r="M19" s="168"/>
       <c r="N19" s="54" t="s">
         <v>109</v>
       </c>
@@ -5437,22 +5437,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="166" t="s">
+      <c r="H20" s="167" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="167" t="s">
+      <c r="J20" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="176" t="s">
+      <c r="K20" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="173" t="s">
+      <c r="L20" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="179" t="s">
+      <c r="M20" s="182" t="s">
         <v>117</v>
       </c>
       <c r="N20" s="51" t="s">
@@ -5483,14 +5483,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="164"/>
+      <c r="H21" s="169"/>
       <c r="I21" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="168"/>
-      <c r="K21" s="177"/>
+      <c r="J21" s="170"/>
+      <c r="K21" s="172"/>
       <c r="L21" s="174"/>
-      <c r="M21" s="180"/>
+      <c r="M21" s="183"/>
       <c r="N21" s="85" t="s">
         <v>100</v>
       </c>
@@ -5519,14 +5519,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="164"/>
+      <c r="H22" s="169"/>
       <c r="I22" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="168"/>
-      <c r="K22" s="177"/>
+      <c r="J22" s="170"/>
+      <c r="K22" s="172"/>
       <c r="L22" s="174"/>
-      <c r="M22" s="180"/>
+      <c r="M22" s="183"/>
       <c r="N22" s="85" t="s">
         <v>101</v>
       </c>
@@ -5555,14 +5555,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="165"/>
+      <c r="H23" s="168"/>
       <c r="I23" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="169"/>
-      <c r="K23" s="178"/>
+      <c r="J23" s="171"/>
+      <c r="K23" s="173"/>
       <c r="L23" s="175"/>
-      <c r="M23" s="181"/>
+      <c r="M23" s="184"/>
       <c r="N23" s="51" t="s">
         <v>102</v>
       </c>
@@ -5591,7 +5591,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="166" t="s">
+      <c r="H24" s="167" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="75" t="s">
@@ -5637,7 +5637,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="165"/>
+      <c r="H25" s="168"/>
       <c r="I25" s="48" t="s">
         <v>46</v>
       </c>
@@ -5681,7 +5681,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="166" t="s">
+      <c r="H26" s="167" t="s">
         <v>59</v>
       </c>
       <c r="I26" s="75" t="s">
@@ -5728,7 +5728,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="165"/>
+      <c r="H27" s="168"/>
       <c r="I27" s="52" t="s">
         <v>24</v>
       </c>
@@ -5772,7 +5772,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="166" t="s">
+      <c r="H28" s="167" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="45" t="s">
@@ -5818,7 +5818,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="164"/>
+      <c r="H29" s="169"/>
       <c r="I29" s="81" t="s">
         <v>52</v>
       </c>
@@ -5862,7 +5862,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30" s="165"/>
+      <c r="H30" s="168"/>
       <c r="I30" s="52" t="s">
         <v>53</v>
       </c>
@@ -6061,14 +6061,18 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="M20:M23"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="H16:H19"/>
     <mergeCell ref="N6:N11"/>
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="J16:J19"/>
@@ -6081,18 +6085,14 @@
     <mergeCell ref="M6:M11"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="M16:M19"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H20:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added unit interface documentation
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B96D482-F831-4AED-AF36-0057DEA1151B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DA28AA-FE99-4CB6-9E92-74DBF9832079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="2" r:id="rId1"/>
@@ -1728,6 +1728,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1764,44 +1803,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1812,69 +1875,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1895,7 +1895,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1916,7 +1916,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2238,15 +2238,15 @@
       <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="6" width="4.7109375" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" customWidth="1"/>
+    <col min="3" max="6" width="4.73046875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1328125" customWidth="1"/>
+    <col min="10" max="10" width="34.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="156" t="s">
         <v>15</v>
       </c>
@@ -2263,7 +2263,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="64" t="s">
         <v>16</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="J3" s="160"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="126">
         <v>0</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="13">
         <v>8</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="13">
         <v>9</v>
       </c>
@@ -2616,7 +2616,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="19">
         <v>10</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="22">
         <v>11</v>
       </c>
@@ -2672,7 +2672,7 @@
       <c r="I15" s="133"/>
       <c r="J15" s="34"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="13">
         <v>12</v>
       </c>
@@ -2697,7 +2697,7 @@
       <c r="I16" s="134"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="13">
         <v>13</v>
       </c>
@@ -2722,7 +2722,7 @@
       <c r="I17" s="134"/>
       <c r="J17" s="32"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="19">
         <v>14</v>
       </c>
@@ -2747,7 +2747,7 @@
       <c r="I18" s="135"/>
       <c r="J18" s="33"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="16">
         <v>15</v>
       </c>
@@ -2791,13 +2791,13 @@
       <selection activeCell="AA5" sqref="AA5:AD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="34" width="7.7109375" customWidth="1"/>
+    <col min="3" max="34" width="7.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="2">
         <v>31</v>
       </c>
@@ -2895,74 +2895,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="173" t="s">
+    <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="174"/>
-      <c r="E3" s="174"/>
-      <c r="F3" s="174"/>
-      <c r="G3" s="175"/>
-      <c r="H3" s="170" t="s">
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="183" t="s">
         <v>98</v>
       </c>
-      <c r="I3" s="171"/>
-      <c r="J3" s="172"/>
-      <c r="K3" s="170" t="s">
+      <c r="I3" s="184"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="183" t="s">
         <v>97</v>
       </c>
-      <c r="L3" s="171"/>
-      <c r="M3" s="171"/>
-      <c r="N3" s="182" t="s">
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="170" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="183"/>
-      <c r="P3" s="184"/>
+      <c r="O3" s="171"/>
+      <c r="P3" s="172"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="176" t="s">
+      <c r="S3" s="164" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="177"/>
-      <c r="U3" s="177"/>
-      <c r="V3" s="177"/>
-      <c r="W3" s="177"/>
-      <c r="X3" s="177"/>
-      <c r="Y3" s="177"/>
-      <c r="Z3" s="178"/>
-      <c r="AA3" s="179" t="s">
+      <c r="T3" s="165"/>
+      <c r="U3" s="165"/>
+      <c r="V3" s="165"/>
+      <c r="W3" s="165"/>
+      <c r="X3" s="165"/>
+      <c r="Y3" s="165"/>
+      <c r="Z3" s="166"/>
+      <c r="AA3" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="180"/>
-      <c r="AC3" s="180"/>
-      <c r="AD3" s="180"/>
-      <c r="AE3" s="180"/>
-      <c r="AF3" s="180"/>
-      <c r="AG3" s="180"/>
-      <c r="AH3" s="181"/>
-    </row>
-    <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="187" t="s">
+      <c r="AB3" s="168"/>
+      <c r="AC3" s="168"/>
+      <c r="AD3" s="168"/>
+      <c r="AE3" s="168"/>
+      <c r="AF3" s="168"/>
+      <c r="AG3" s="168"/>
+      <c r="AH3" s="169"/>
+    </row>
+    <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.45">
+      <c r="B5" s="175" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="185" t="s">
+      <c r="C5" s="173" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="185"/>
-      <c r="G5" s="185"/>
-      <c r="H5" s="185"/>
-      <c r="I5" s="185"/>
-      <c r="J5" s="186"/>
-    </row>
-    <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="188"/>
+      <c r="D5" s="173"/>
+      <c r="E5" s="173"/>
+      <c r="F5" s="173"/>
+      <c r="G5" s="173"/>
+      <c r="H5" s="173"/>
+      <c r="I5" s="173"/>
+      <c r="J5" s="174"/>
+    </row>
+    <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="176"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -2988,22 +2988,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.45">
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="164" t="s">
+      <c r="C7" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="165"/>
-      <c r="E7" s="165"/>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
-      <c r="I7" s="165"/>
-      <c r="J7" s="166"/>
-    </row>
-    <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="178"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="178"/>
+      <c r="J7" s="179"/>
+    </row>
+    <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -3011,14 +3011,14 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="167" t="s">
+      <c r="G8" s="180" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="168"/>
-      <c r="I8" s="168"/>
-      <c r="J8" s="169"/>
-    </row>
-    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="182"/>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.45">
       <c r="G10">
         <v>1</v>
       </c>
@@ -3028,16 +3028,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3052,38 +3052,38 @@
       <selection activeCell="L20" sqref="L20:L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="7" width="4.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="12" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="7" width="4.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20.73046875" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="90.28515625" customWidth="1"/>
+    <col min="14" max="14" width="90.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="189" t="s">
+    <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="191"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="212"/>
       <c r="H2" s="159" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="189" t="s">
+      <c r="J2" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="190"/>
-      <c r="L2" s="190"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
       <c r="M2" s="159" t="s">
         <v>116</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="93" t="s">
         <v>16</v>
       </c>
@@ -3124,7 +3124,7 @@
       <c r="M3" s="160"/>
       <c r="N3" s="160"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="89">
         <v>0</v>
       </c>
@@ -3148,7 +3148,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="192" t="s">
+      <c r="H4" s="191" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="75" t="s">
@@ -3170,7 +3170,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="91">
         <v>1</v>
       </c>
@@ -3194,7 +3194,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="193"/>
+      <c r="H5" s="190"/>
       <c r="I5" s="49" t="s">
         <v>3</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B6" s="90">
         <v>2</v>
       </c>
@@ -3238,29 +3238,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="194" t="s">
+      <c r="H6" s="189" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="195" t="s">
+      <c r="J6" s="193" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="197" t="s">
+      <c r="K6" s="202" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="207" t="s">
+      <c r="M6" s="204" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="201" t="s">
+      <c r="N6" s="207" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7" s="90">
         <v>3</v>
       </c>
@@ -3284,17 +3284,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="194"/>
+      <c r="H7" s="189"/>
       <c r="I7" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="195"/>
-      <c r="K7" s="197"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="202"/>
       <c r="L7" s="199"/>
-      <c r="M7" s="208"/>
-      <c r="N7" s="201"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="205"/>
+      <c r="N7" s="207"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="90">
         <v>4</v>
       </c>
@@ -3318,17 +3318,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="194"/>
+      <c r="H8" s="189"/>
       <c r="I8" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="195"/>
-      <c r="K8" s="197"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="202"/>
       <c r="L8" s="199"/>
-      <c r="M8" s="208"/>
-      <c r="N8" s="201"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="205"/>
+      <c r="N8" s="207"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="90">
         <v>5</v>
       </c>
@@ -3352,17 +3352,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="194"/>
+      <c r="H9" s="189"/>
       <c r="I9" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="195"/>
-      <c r="K9" s="197"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="202"/>
       <c r="L9" s="199"/>
-      <c r="M9" s="208"/>
-      <c r="N9" s="201"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="205"/>
+      <c r="N9" s="207"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="90">
         <v>6</v>
       </c>
@@ -3386,17 +3386,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="194"/>
+      <c r="H10" s="189"/>
       <c r="I10" s="100" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="195"/>
-      <c r="K10" s="197"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="202"/>
       <c r="L10" s="199"/>
-      <c r="M10" s="208"/>
-      <c r="N10" s="201"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="205"/>
+      <c r="N10" s="207"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="91">
         <v>7</v>
       </c>
@@ -3420,17 +3420,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="193"/>
+      <c r="H11" s="190"/>
       <c r="I11" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="196"/>
-      <c r="K11" s="198"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="203"/>
       <c r="L11" s="200"/>
-      <c r="M11" s="209"/>
-      <c r="N11" s="202"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="206"/>
+      <c r="N11" s="208"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="89">
         <v>8</v>
       </c>
@@ -3454,29 +3454,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="192" t="s">
+      <c r="H12" s="191" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="72" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="203" t="s">
+      <c r="J12" s="192" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="204" t="s">
+      <c r="K12" s="201" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="205" t="s">
+      <c r="L12" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="192" t="s">
+      <c r="M12" s="191" t="s">
         <v>118</v>
       </c>
-      <c r="N12" s="206" t="s">
+      <c r="N12" s="209" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="90">
         <v>9</v>
       </c>
@@ -3500,17 +3500,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="194"/>
+      <c r="H13" s="189"/>
       <c r="I13" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="195"/>
-      <c r="K13" s="197"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="202"/>
       <c r="L13" s="199"/>
-      <c r="M13" s="194"/>
-      <c r="N13" s="201"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="189"/>
+      <c r="N13" s="207"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="90">
         <v>10</v>
       </c>
@@ -3534,17 +3534,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="194"/>
+      <c r="H14" s="189"/>
       <c r="I14" s="100" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="195"/>
-      <c r="K14" s="197"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="202"/>
       <c r="L14" s="199"/>
-      <c r="M14" s="194"/>
-      <c r="N14" s="201"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="189"/>
+      <c r="N14" s="207"/>
+    </row>
+    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="91">
         <v>11</v>
       </c>
@@ -3568,17 +3568,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="193"/>
+      <c r="H15" s="190"/>
       <c r="I15" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="196"/>
-      <c r="K15" s="198"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="203"/>
       <c r="L15" s="200"/>
-      <c r="M15" s="193"/>
-      <c r="N15" s="202"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="190"/>
+      <c r="N15" s="208"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="89">
         <v>12</v>
       </c>
@@ -3602,29 +3602,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="192" t="s">
+      <c r="H16" s="191" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="203" t="s">
+      <c r="J16" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="210" t="s">
+      <c r="K16" s="195" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="205" t="s">
+      <c r="L16" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="192" t="s">
+      <c r="M16" s="191" t="s">
         <v>118</v>
       </c>
       <c r="N16" s="83" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="90">
         <v>13</v>
       </c>
@@ -3648,19 +3648,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="194"/>
+      <c r="H17" s="189"/>
       <c r="I17" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="195"/>
-      <c r="K17" s="211"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="196"/>
       <c r="L17" s="199"/>
-      <c r="M17" s="194"/>
+      <c r="M17" s="189"/>
       <c r="N17" s="82" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="90">
         <v>14</v>
       </c>
@@ -3684,19 +3684,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="194"/>
+      <c r="H18" s="189"/>
       <c r="I18" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="195"/>
-      <c r="K18" s="211"/>
+      <c r="J18" s="193"/>
+      <c r="K18" s="196"/>
       <c r="L18" s="199"/>
-      <c r="M18" s="194"/>
+      <c r="M18" s="189"/>
       <c r="N18" s="82" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="91">
         <v>15</v>
       </c>
@@ -3720,20 +3720,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="193"/>
+      <c r="H19" s="190"/>
       <c r="I19" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="196"/>
-      <c r="K19" s="212"/>
+      <c r="J19" s="194"/>
+      <c r="K19" s="197"/>
       <c r="L19" s="200"/>
-      <c r="M19" s="193"/>
+      <c r="M19" s="190"/>
       <c r="N19" s="51" t="s">
         <v>109</v>
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="89">
         <v>16</v>
       </c>
@@ -3757,29 +3757,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="192" t="s">
+      <c r="H20" s="191" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="203" t="s">
+      <c r="J20" s="192" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="204" t="s">
+      <c r="K20" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="205" t="s">
+      <c r="L20" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="207" t="s">
+      <c r="M20" s="204" t="s">
         <v>117</v>
       </c>
       <c r="N20" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="90">
         <v>17</v>
       </c>
@@ -3803,19 +3803,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="194"/>
+      <c r="H21" s="189"/>
       <c r="I21" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="195"/>
-      <c r="K21" s="197"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="202"/>
       <c r="L21" s="199"/>
-      <c r="M21" s="208"/>
+      <c r="M21" s="205"/>
       <c r="N21" s="82" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="90">
         <v>18</v>
       </c>
@@ -3839,19 +3839,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="194"/>
+      <c r="H22" s="189"/>
       <c r="I22" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="195"/>
-      <c r="K22" s="197"/>
+      <c r="J22" s="193"/>
+      <c r="K22" s="202"/>
       <c r="L22" s="199"/>
-      <c r="M22" s="208"/>
+      <c r="M22" s="205"/>
       <c r="N22" s="82" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="90">
         <v>19</v>
       </c>
@@ -3875,19 +3875,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="193"/>
+      <c r="H23" s="190"/>
       <c r="I23" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="196"/>
-      <c r="K23" s="198"/>
+      <c r="J23" s="194"/>
+      <c r="K23" s="203"/>
       <c r="L23" s="200"/>
-      <c r="M23" s="209"/>
+      <c r="M23" s="206"/>
       <c r="N23" s="48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="89">
         <v>20</v>
       </c>
@@ -3911,7 +3911,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="192" t="s">
+      <c r="H24" s="191" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="72" t="s">
@@ -3933,7 +3933,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25" s="90">
         <v>21</v>
       </c>
@@ -3957,7 +3957,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="194"/>
+      <c r="H25" s="189"/>
       <c r="I25" s="78" t="s">
         <v>46</v>
       </c>
@@ -3977,7 +3977,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="90">
         <v>22</v>
       </c>
@@ -4001,7 +4001,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="194"/>
+      <c r="H26" s="189"/>
       <c r="I26" s="119" t="s">
         <v>122</v>
       </c>
@@ -4011,7 +4011,7 @@
       <c r="M26" s="123"/>
       <c r="N26" s="123"/>
     </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="91">
         <v>23</v>
       </c>
@@ -4035,7 +4035,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="190"/>
       <c r="I27" s="49" t="s">
         <v>123</v>
       </c>
@@ -4045,7 +4045,7 @@
       <c r="M27" s="51"/>
       <c r="N27" s="51"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="89">
         <v>24</v>
       </c>
@@ -4069,7 +4069,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="192" t="s">
+      <c r="H28" s="191" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="42" t="s">
@@ -4091,7 +4091,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29" s="90">
         <v>25</v>
       </c>
@@ -4115,7 +4115,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="194"/>
+      <c r="H29" s="189"/>
       <c r="I29" s="78" t="s">
         <v>52</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30" s="90">
         <v>26</v>
       </c>
@@ -4159,7 +4159,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="194"/>
+      <c r="H30" s="189"/>
       <c r="I30" s="78" t="s">
         <v>53</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="91">
         <v>27</v>
       </c>
@@ -4203,7 +4203,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="193"/>
+      <c r="H31" s="190"/>
       <c r="I31" s="102" t="s">
         <v>124</v>
       </c>
@@ -4213,7 +4213,7 @@
       <c r="M31" s="109"/>
       <c r="N31" s="106"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32" s="90">
         <v>28</v>
       </c>
@@ -4237,7 +4237,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="194" t="s">
+      <c r="H32" s="189" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="72" t="s">
@@ -4260,7 +4260,7 @@
       </c>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33" s="90">
         <v>29</v>
       </c>
@@ -4284,7 +4284,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="194"/>
+      <c r="H33" s="189"/>
       <c r="I33" s="78" t="s">
         <v>24</v>
       </c>
@@ -4305,7 +4305,7 @@
       </c>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="90">
         <v>30</v>
       </c>
@@ -4329,7 +4329,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="193"/>
+      <c r="H34" s="190"/>
       <c r="I34" s="110" t="s">
         <v>125</v>
       </c>
@@ -4340,7 +4340,7 @@
       <c r="N34" s="106"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="92">
         <v>31</v>
       </c>
@@ -4388,11 +4388,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4401,25 +4415,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4434,24 +4434,24 @@
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="5" width="4.7109375" customWidth="1"/>
+    <col min="3" max="5" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="189" t="s">
+    <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="210" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="191"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="212"/>
       <c r="F2" s="159" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
       <c r="F3" s="160"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
         <v>0</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -4606,7 +4606,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -4643,13 +4643,13 @@
       <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B2" s="159" t="s">
         <v>81</v>
       </c>
@@ -4664,7 +4664,7 @@
       <c r="I2" s="215"/>
       <c r="J2" s="216"/>
     </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="160"/>
       <c r="C3" s="94">
         <v>7</v>
@@ -4691,7 +4691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="96" t="s">
         <v>82</v>
       </c>
@@ -4712,7 +4712,7 @@
       <c r="I4" s="217"/>
       <c r="J4" s="218"/>
     </row>
-    <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="98" t="s">
         <v>3</v>
       </c>
@@ -4727,7 +4727,7 @@
       <c r="I5" s="213"/>
       <c r="J5" s="214"/>
     </row>
-    <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="98" t="s">
         <v>2</v>
       </c>
@@ -4742,7 +4742,7 @@
       <c r="I6" s="213"/>
       <c r="J6" s="214"/>
     </row>
-    <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="98" t="s">
         <v>83</v>
       </c>
@@ -4757,7 +4757,7 @@
       <c r="I7" s="213"/>
       <c r="J7" s="214"/>
     </row>
-    <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="98" t="s">
         <v>84</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="99" t="s">
         <v>90</v>
       </c>
@@ -4816,12 +4816,12 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>126</v>
       </c>
@@ -4829,7 +4829,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>127</v>
       </c>
@@ -4837,12 +4837,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>128</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>129</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>46</v>
       </c>
@@ -4879,38 +4879,38 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="7" width="4.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="12" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="7" width="4.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20.73046875" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="90.28515625" customWidth="1"/>
+    <col min="14" max="14" width="90.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="189" t="s">
+    <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="210" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="190"/>
-      <c r="F2" s="190"/>
-      <c r="G2" s="191"/>
+      <c r="C2" s="211"/>
+      <c r="D2" s="211"/>
+      <c r="E2" s="211"/>
+      <c r="F2" s="211"/>
+      <c r="G2" s="212"/>
       <c r="H2" s="159" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="159" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="189" t="s">
+      <c r="J2" s="210" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="190"/>
-      <c r="L2" s="190"/>
+      <c r="K2" s="211"/>
+      <c r="L2" s="211"/>
       <c r="M2" s="159" t="s">
         <v>116</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="93" t="s">
         <v>16</v>
       </c>
@@ -4951,7 +4951,7 @@
       <c r="M3" s="160"/>
       <c r="N3" s="160"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="89">
         <v>0</v>
       </c>
@@ -4975,7 +4975,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="192" t="s">
+      <c r="H4" s="191" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="75" t="s">
@@ -4997,7 +4997,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="91">
         <v>1</v>
       </c>
@@ -5021,7 +5021,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="193"/>
+      <c r="H5" s="190"/>
       <c r="I5" s="49" t="s">
         <v>3</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B6" s="90">
         <v>2</v>
       </c>
@@ -5065,29 +5065,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="194" t="s">
+      <c r="H6" s="189" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="195" t="s">
+      <c r="J6" s="193" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="197" t="s">
+      <c r="K6" s="202" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="199" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="207" t="s">
+      <c r="M6" s="204" t="s">
         <v>117</v>
       </c>
-      <c r="N6" s="201" t="s">
+      <c r="N6" s="207" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7" s="90">
         <v>3</v>
       </c>
@@ -5111,17 +5111,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="194"/>
+      <c r="H7" s="189"/>
       <c r="I7" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="195"/>
-      <c r="K7" s="197"/>
+      <c r="J7" s="193"/>
+      <c r="K7" s="202"/>
       <c r="L7" s="199"/>
-      <c r="M7" s="208"/>
-      <c r="N7" s="201"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="205"/>
+      <c r="N7" s="207"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="90">
         <v>4</v>
       </c>
@@ -5145,17 +5145,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="194"/>
+      <c r="H8" s="189"/>
       <c r="I8" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="195"/>
-      <c r="K8" s="197"/>
+      <c r="J8" s="193"/>
+      <c r="K8" s="202"/>
       <c r="L8" s="199"/>
-      <c r="M8" s="208"/>
-      <c r="N8" s="201"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="205"/>
+      <c r="N8" s="207"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="90">
         <v>5</v>
       </c>
@@ -5179,17 +5179,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="194"/>
+      <c r="H9" s="189"/>
       <c r="I9" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="195"/>
-      <c r="K9" s="197"/>
+      <c r="J9" s="193"/>
+      <c r="K9" s="202"/>
       <c r="L9" s="199"/>
-      <c r="M9" s="208"/>
-      <c r="N9" s="201"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="205"/>
+      <c r="N9" s="207"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="90">
         <v>6</v>
       </c>
@@ -5213,17 +5213,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="194"/>
+      <c r="H10" s="189"/>
       <c r="I10" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="195"/>
-      <c r="K10" s="197"/>
+      <c r="J10" s="193"/>
+      <c r="K10" s="202"/>
       <c r="L10" s="199"/>
-      <c r="M10" s="208"/>
-      <c r="N10" s="201"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="205"/>
+      <c r="N10" s="207"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="91">
         <v>7</v>
       </c>
@@ -5247,17 +5247,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="193"/>
+      <c r="H11" s="190"/>
       <c r="I11" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="196"/>
-      <c r="K11" s="198"/>
+      <c r="J11" s="194"/>
+      <c r="K11" s="203"/>
       <c r="L11" s="200"/>
-      <c r="M11" s="209"/>
-      <c r="N11" s="202"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="206"/>
+      <c r="N11" s="208"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="89">
         <v>8</v>
       </c>
@@ -5281,29 +5281,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="192" t="s">
+      <c r="H12" s="191" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="203" t="s">
+      <c r="J12" s="192" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="204" t="s">
+      <c r="K12" s="201" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="205" t="s">
+      <c r="L12" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="192" t="s">
+      <c r="M12" s="191" t="s">
         <v>118</v>
       </c>
-      <c r="N12" s="206" t="s">
+      <c r="N12" s="209" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="90">
         <v>9</v>
       </c>
@@ -5327,17 +5327,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="194"/>
+      <c r="H13" s="189"/>
       <c r="I13" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="195"/>
-      <c r="K13" s="197"/>
+      <c r="J13" s="193"/>
+      <c r="K13" s="202"/>
       <c r="L13" s="199"/>
-      <c r="M13" s="194"/>
-      <c r="N13" s="201"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="189"/>
+      <c r="N13" s="207"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="90">
         <v>10</v>
       </c>
@@ -5361,17 +5361,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="194"/>
+      <c r="H14" s="189"/>
       <c r="I14" s="46" t="s">
         <v>103</v>
       </c>
-      <c r="J14" s="195"/>
-      <c r="K14" s="197"/>
+      <c r="J14" s="193"/>
+      <c r="K14" s="202"/>
       <c r="L14" s="199"/>
-      <c r="M14" s="194"/>
-      <c r="N14" s="201"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="189"/>
+      <c r="N14" s="207"/>
+    </row>
+    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="91">
         <v>11</v>
       </c>
@@ -5395,17 +5395,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="193"/>
+      <c r="H15" s="190"/>
       <c r="I15" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="J15" s="196"/>
-      <c r="K15" s="198"/>
+      <c r="J15" s="194"/>
+      <c r="K15" s="203"/>
       <c r="L15" s="200"/>
-      <c r="M15" s="193"/>
-      <c r="N15" s="202"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="190"/>
+      <c r="N15" s="208"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="89">
         <v>12</v>
       </c>
@@ -5429,29 +5429,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="192" t="s">
+      <c r="H16" s="191" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="203" t="s">
+      <c r="J16" s="192" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="210" t="s">
+      <c r="K16" s="195" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="205" t="s">
+      <c r="L16" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="192" t="s">
+      <c r="M16" s="191" t="s">
         <v>118</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="90">
         <v>13</v>
       </c>
@@ -5475,19 +5475,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="194"/>
+      <c r="H17" s="189"/>
       <c r="I17" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="195"/>
-      <c r="K17" s="211"/>
+      <c r="J17" s="193"/>
+      <c r="K17" s="196"/>
       <c r="L17" s="199"/>
-      <c r="M17" s="194"/>
+      <c r="M17" s="189"/>
       <c r="N17" s="48" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="90">
         <v>14</v>
       </c>
@@ -5511,19 +5511,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="194"/>
+      <c r="H18" s="189"/>
       <c r="I18" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="195"/>
-      <c r="K18" s="211"/>
+      <c r="J18" s="193"/>
+      <c r="K18" s="196"/>
       <c r="L18" s="199"/>
-      <c r="M18" s="194"/>
+      <c r="M18" s="189"/>
       <c r="N18" s="48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="91">
         <v>15</v>
       </c>
@@ -5547,19 +5547,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="193"/>
+      <c r="H19" s="190"/>
       <c r="I19" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="196"/>
-      <c r="K19" s="212"/>
+      <c r="J19" s="194"/>
+      <c r="K19" s="197"/>
       <c r="L19" s="200"/>
-      <c r="M19" s="193"/>
+      <c r="M19" s="190"/>
       <c r="N19" s="51" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="89">
         <v>16</v>
       </c>
@@ -5583,29 +5583,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="192" t="s">
+      <c r="H20" s="191" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="203" t="s">
+      <c r="J20" s="192" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="204" t="s">
+      <c r="K20" s="201" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="205" t="s">
+      <c r="L20" s="198" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="207" t="s">
+      <c r="M20" s="204" t="s">
         <v>117</v>
       </c>
       <c r="N20" s="48" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="90">
         <v>17</v>
       </c>
@@ -5629,19 +5629,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="194"/>
+      <c r="H21" s="189"/>
       <c r="I21" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="195"/>
-      <c r="K21" s="197"/>
+      <c r="J21" s="193"/>
+      <c r="K21" s="202"/>
       <c r="L21" s="199"/>
-      <c r="M21" s="208"/>
+      <c r="M21" s="205"/>
       <c r="N21" s="82" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="90">
         <v>18</v>
       </c>
@@ -5665,19 +5665,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="194"/>
+      <c r="H22" s="189"/>
       <c r="I22" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="195"/>
-      <c r="K22" s="197"/>
+      <c r="J22" s="193"/>
+      <c r="K22" s="202"/>
       <c r="L22" s="199"/>
-      <c r="M22" s="208"/>
+      <c r="M22" s="205"/>
       <c r="N22" s="82" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="90">
         <v>19</v>
       </c>
@@ -5701,19 +5701,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="193"/>
+      <c r="H23" s="190"/>
       <c r="I23" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="196"/>
-      <c r="K23" s="198"/>
+      <c r="J23" s="194"/>
+      <c r="K23" s="203"/>
       <c r="L23" s="200"/>
-      <c r="M23" s="209"/>
+      <c r="M23" s="206"/>
       <c r="N23" s="48" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="89">
         <v>20</v>
       </c>
@@ -5737,7 +5737,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="192" t="s">
+      <c r="H24" s="191" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="72" t="s">
@@ -5759,7 +5759,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B25" s="90">
         <v>21</v>
       </c>
@@ -5783,7 +5783,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="193"/>
+      <c r="H25" s="190"/>
       <c r="I25" s="45" t="s">
         <v>46</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="89">
         <v>22</v>
       </c>
@@ -5827,7 +5827,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="192" t="s">
+      <c r="H26" s="191" t="s">
         <v>59</v>
       </c>
       <c r="I26" s="72" t="s">
@@ -5850,7 +5850,7 @@
       </c>
       <c r="P26" s="1"/>
     </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="91">
         <v>23</v>
       </c>
@@ -5874,7 +5874,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="193"/>
+      <c r="H27" s="190"/>
       <c r="I27" s="49" t="s">
         <v>24</v>
       </c>
@@ -5894,7 +5894,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="89">
         <v>24</v>
       </c>
@@ -5918,7 +5918,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H28" s="192" t="s">
+      <c r="H28" s="191" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="42" t="s">
@@ -5940,7 +5940,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29" s="90">
         <v>25</v>
       </c>
@@ -5964,7 +5964,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H29" s="194"/>
+      <c r="H29" s="189"/>
       <c r="I29" s="78" t="s">
         <v>52</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B30" s="91">
         <v>26</v>
       </c>
@@ -6008,7 +6008,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H30" s="193"/>
+      <c r="H30" s="190"/>
       <c r="I30" s="49" t="s">
         <v>53</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B31" s="113">
         <v>27</v>
       </c>
@@ -6060,7 +6060,7 @@
       <c r="M31" s="109"/>
       <c r="N31" s="106"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32" s="113">
         <v>28</v>
       </c>
@@ -6093,7 +6093,7 @@
       <c r="N32" s="106"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33" s="113">
         <v>29</v>
       </c>
@@ -6126,7 +6126,7 @@
       <c r="N33" s="106"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="113">
         <v>30</v>
       </c>
@@ -6159,7 +6159,7 @@
       <c r="N34" s="106"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="92">
         <v>31</v>
       </c>
@@ -6207,6 +6207,26 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="M16:M19"/>
     <mergeCell ref="M20:M23"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="H24:H25"/>
@@ -6219,26 +6239,6 @@
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="H16:H19"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="H20:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed RGSET faulty schematic connection
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6976C181-05DE-4A71-AE15-947CC39B5192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5535E9-88E0-46DA-B174-3BADAB2D3DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
   <si>
     <t>MODE B</t>
   </si>
@@ -520,6 +520,30 @@
   </si>
   <si>
     <t>Write output to selected register if condition is met</t>
+  </si>
+  <si>
+    <t>FREEZE WORD</t>
+  </si>
+  <si>
+    <t>Freeze A Immediate value / A address, B immediate value / B address, OUT address, condition result</t>
+  </si>
+  <si>
+    <t>FREEZE OP</t>
+  </si>
+  <si>
+    <t>Freezes OPCODE, will be set to 0 if condition is false</t>
+  </si>
+  <si>
+    <t>HOLD OUTPUT</t>
+  </si>
+  <si>
+    <t>Freezes register side output bus</t>
+  </si>
+  <si>
+    <t>Stores output to register</t>
+  </si>
+  <si>
+    <t>Increments PC</t>
   </si>
 </sst>
 </file>
@@ -1871,6 +1895,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1910,94 +1970,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2006,17 +2012,44 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2027,12 +2060,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2049,9 +2076,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2080,7 +2104,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2101,7 +2125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2423,15 +2447,15 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="6" width="4.7109375" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" customWidth="1"/>
+    <col min="3" max="6" width="4.73046875" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.1328125" customWidth="1"/>
+    <col min="10" max="10" width="34.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B2" s="166" t="s">
         <v>15</v>
       </c>
@@ -2448,7 +2472,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="57" t="s">
         <v>16</v>
       </c>
@@ -2475,7 +2499,7 @@
       </c>
       <c r="J3" s="170"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
         <v>0</v>
       </c>
@@ -2508,7 +2532,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -2541,7 +2565,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -2574,7 +2598,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -2607,7 +2631,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -2640,7 +2664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -2673,7 +2697,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -2706,7 +2730,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -2739,7 +2763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B12" s="13">
         <v>8</v>
       </c>
@@ -2770,7 +2794,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B13" s="13">
         <v>9</v>
       </c>
@@ -2799,7 +2823,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B14" s="19">
         <v>10</v>
       </c>
@@ -2824,7 +2848,7 @@
       <c r="I14" s="116"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B15" s="22">
         <v>11</v>
       </c>
@@ -2855,7 +2879,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B16" s="13">
         <v>12</v>
       </c>
@@ -2880,7 +2904,7 @@
       <c r="I16" s="115"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B17" s="13">
         <v>13</v>
       </c>
@@ -2905,7 +2929,7 @@
       <c r="I17" s="115"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B18" s="19">
         <v>14</v>
       </c>
@@ -2930,7 +2954,7 @@
       <c r="I18" s="116"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="16">
         <v>15</v>
       </c>
@@ -2974,13 +2998,13 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="34" width="7.7109375" customWidth="1"/>
+    <col min="3" max="34" width="7.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C2" s="2">
         <v>31</v>
       </c>
@@ -3078,74 +3102,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="196" t="s">
+    <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="C3" s="183" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="197"/>
-      <c r="E3" s="197"/>
-      <c r="F3" s="197"/>
-      <c r="G3" s="198"/>
-      <c r="H3" s="193" t="s">
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="185"/>
+      <c r="H3" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="194"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="193" t="s">
+      <c r="I3" s="181"/>
+      <c r="J3" s="182"/>
+      <c r="K3" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="194"/>
-      <c r="M3" s="194"/>
-      <c r="N3" s="180" t="s">
+      <c r="L3" s="181"/>
+      <c r="M3" s="181"/>
+      <c r="N3" s="192" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="181"/>
-      <c r="P3" s="182"/>
+      <c r="O3" s="193"/>
+      <c r="P3" s="194"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="174" t="s">
+      <c r="S3" s="186" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="175"/>
-      <c r="U3" s="175"/>
-      <c r="V3" s="175"/>
-      <c r="W3" s="175"/>
-      <c r="X3" s="175"/>
-      <c r="Y3" s="175"/>
-      <c r="Z3" s="176"/>
-      <c r="AA3" s="177" t="s">
+      <c r="T3" s="187"/>
+      <c r="U3" s="187"/>
+      <c r="V3" s="187"/>
+      <c r="W3" s="187"/>
+      <c r="X3" s="187"/>
+      <c r="Y3" s="187"/>
+      <c r="Z3" s="188"/>
+      <c r="AA3" s="189" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="178"/>
-      <c r="AC3" s="178"/>
-      <c r="AD3" s="178"/>
-      <c r="AE3" s="178"/>
-      <c r="AF3" s="178"/>
-      <c r="AG3" s="178"/>
-      <c r="AH3" s="179"/>
-    </row>
-    <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="185" t="s">
+      <c r="AB3" s="190"/>
+      <c r="AC3" s="190"/>
+      <c r="AD3" s="190"/>
+      <c r="AE3" s="190"/>
+      <c r="AF3" s="190"/>
+      <c r="AG3" s="190"/>
+      <c r="AH3" s="191"/>
+    </row>
+    <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.45">
+      <c r="B5" s="197" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="183" t="s">
+      <c r="C5" s="195" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="183"/>
-      <c r="E5" s="183"/>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183"/>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="184"/>
-    </row>
-    <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="186"/>
+      <c r="D5" s="195"/>
+      <c r="E5" s="195"/>
+      <c r="F5" s="195"/>
+      <c r="G5" s="195"/>
+      <c r="H5" s="195"/>
+      <c r="I5" s="195"/>
+      <c r="J5" s="196"/>
+    </row>
+    <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="198"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3171,22 +3195,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.45">
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="187" t="s">
+      <c r="C7" s="174" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="188"/>
-      <c r="E7" s="188"/>
-      <c r="F7" s="188"/>
-      <c r="G7" s="188"/>
-      <c r="H7" s="188"/>
-      <c r="I7" s="188"/>
-      <c r="J7" s="189"/>
-    </row>
-    <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="175"/>
+      <c r="E7" s="175"/>
+      <c r="F7" s="175"/>
+      <c r="G7" s="175"/>
+      <c r="H7" s="175"/>
+      <c r="I7" s="175"/>
+      <c r="J7" s="176"/>
+    </row>
+    <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -3194,25 +3218,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="190" t="s">
+      <c r="G8" s="177" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="191"/>
-      <c r="I8" s="191"/>
-      <c r="J8" s="192"/>
+      <c r="H8" s="178"/>
+      <c r="I8" s="178"/>
+      <c r="J8" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="S3:Z3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3227,38 +3251,38 @@
       <selection activeCell="J16" sqref="J16:J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="7" width="4.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
-    <col min="10" max="12" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1"/>
+    <col min="3" max="7" width="4.73046875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.73046875" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20.73046875" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="90.28515625" customWidth="1"/>
+    <col min="14" max="14" width="90.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="220" t="s">
+    <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B2" s="199" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="222"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="200"/>
+      <c r="F2" s="200"/>
+      <c r="G2" s="201"/>
       <c r="H2" s="169" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="220" t="s">
+      <c r="J2" s="199" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
+      <c r="K2" s="200"/>
+      <c r="L2" s="200"/>
       <c r="M2" s="169" t="s">
         <v>115</v>
       </c>
@@ -3266,7 +3290,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="85" t="s">
         <v>16</v>
       </c>
@@ -3299,7 +3323,7 @@
       <c r="M3" s="170"/>
       <c r="N3" s="170"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
         <v>0</v>
       </c>
@@ -3323,7 +3347,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="201" t="s">
+      <c r="H4" s="202" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3345,7 +3369,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="83">
         <v>1</v>
       </c>
@@ -3369,7 +3393,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="200"/>
+      <c r="H5" s="203"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3389,7 +3413,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B6" s="82">
         <v>2</v>
       </c>
@@ -3413,29 +3437,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="199" t="s">
+      <c r="H6" s="204" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="203" t="s">
+      <c r="J6" s="205" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="212" t="s">
+      <c r="K6" s="207" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="214" t="s">
+      <c r="M6" s="217" t="s">
         <v>116</v>
       </c>
-      <c r="N6" s="217" t="s">
+      <c r="N6" s="211" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7" s="82">
         <v>3</v>
       </c>
@@ -3459,17 +3483,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="199"/>
+      <c r="H7" s="204"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="203"/>
-      <c r="K7" s="212"/>
+      <c r="J7" s="205"/>
+      <c r="K7" s="207"/>
       <c r="L7" s="209"/>
-      <c r="M7" s="215"/>
-      <c r="N7" s="217"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M7" s="218"/>
+      <c r="N7" s="211"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
         <v>4</v>
       </c>
@@ -3493,17 +3517,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="199"/>
+      <c r="H8" s="204"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="203"/>
-      <c r="K8" s="212"/>
+      <c r="J8" s="205"/>
+      <c r="K8" s="207"/>
       <c r="L8" s="209"/>
-      <c r="M8" s="215"/>
-      <c r="N8" s="217"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M8" s="218"/>
+      <c r="N8" s="211"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
         <v>5</v>
       </c>
@@ -3527,17 +3551,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="199"/>
+      <c r="H9" s="204"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="203"/>
-      <c r="K9" s="212"/>
+      <c r="J9" s="205"/>
+      <c r="K9" s="207"/>
       <c r="L9" s="209"/>
-      <c r="M9" s="215"/>
-      <c r="N9" s="217"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="218"/>
+      <c r="N9" s="211"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
         <v>6</v>
       </c>
@@ -3561,17 +3585,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="199"/>
+      <c r="H10" s="204"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="203"/>
-      <c r="K10" s="212"/>
+      <c r="J10" s="205"/>
+      <c r="K10" s="207"/>
       <c r="L10" s="209"/>
-      <c r="M10" s="215"/>
-      <c r="N10" s="217"/>
-    </row>
-    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="218"/>
+      <c r="N10" s="211"/>
+    </row>
+    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
         <v>7</v>
       </c>
@@ -3595,17 +3619,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="200"/>
+      <c r="H11" s="203"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="204"/>
-      <c r="K11" s="213"/>
+      <c r="J11" s="206"/>
+      <c r="K11" s="208"/>
       <c r="L11" s="210"/>
-      <c r="M11" s="216"/>
-      <c r="N11" s="218"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="219"/>
+      <c r="N11" s="212"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
         <v>8</v>
       </c>
@@ -3629,29 +3653,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="201" t="s">
+      <c r="H12" s="202" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="202" t="s">
+      <c r="J12" s="213" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="211" t="s">
+      <c r="K12" s="214" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="208" t="s">
+      <c r="L12" s="215" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="201" t="s">
+      <c r="M12" s="202" t="s">
         <v>117</v>
       </c>
-      <c r="N12" s="219" t="s">
+      <c r="N12" s="216" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="82">
         <v>9</v>
       </c>
@@ -3675,17 +3699,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="199"/>
+      <c r="H13" s="204"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="203"/>
-      <c r="K13" s="212"/>
+      <c r="J13" s="205"/>
+      <c r="K13" s="207"/>
       <c r="L13" s="209"/>
-      <c r="M13" s="199"/>
-      <c r="N13" s="217"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="204"/>
+      <c r="N13" s="211"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
         <v>10</v>
       </c>
@@ -3709,17 +3733,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="199"/>
+      <c r="H14" s="204"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="203"/>
-      <c r="K14" s="212"/>
+      <c r="J14" s="205"/>
+      <c r="K14" s="207"/>
       <c r="L14" s="209"/>
-      <c r="M14" s="199"/>
-      <c r="N14" s="217"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="204"/>
+      <c r="N14" s="211"/>
+    </row>
+    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
         <v>11</v>
       </c>
@@ -3743,17 +3767,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="200"/>
+      <c r="H15" s="203"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="204"/>
-      <c r="K15" s="213"/>
+      <c r="J15" s="206"/>
+      <c r="K15" s="208"/>
       <c r="L15" s="210"/>
-      <c r="M15" s="200"/>
-      <c r="N15" s="218"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M15" s="203"/>
+      <c r="N15" s="212"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
         <v>12</v>
       </c>
@@ -3777,29 +3801,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="201" t="s">
+      <c r="H16" s="202" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="202" t="s">
+      <c r="J16" s="213" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="205" t="s">
+      <c r="K16" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="208" t="s">
+      <c r="L16" s="215" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="201" t="s">
+      <c r="M16" s="202" t="s">
         <v>117</v>
       </c>
       <c r="N16" s="76" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B17" s="82">
         <v>13</v>
       </c>
@@ -3823,19 +3847,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="199"/>
+      <c r="H17" s="204"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="203"/>
-      <c r="K17" s="206"/>
+      <c r="J17" s="205"/>
+      <c r="K17" s="221"/>
       <c r="L17" s="209"/>
-      <c r="M17" s="199"/>
+      <c r="M17" s="204"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B18" s="82">
         <v>14</v>
       </c>
@@ -3859,19 +3883,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="199"/>
+      <c r="H18" s="204"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="203"/>
-      <c r="K18" s="206"/>
+      <c r="J18" s="205"/>
+      <c r="K18" s="221"/>
       <c r="L18" s="209"/>
-      <c r="M18" s="199"/>
+      <c r="M18" s="204"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
         <v>15</v>
       </c>
@@ -3895,20 +3919,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="200"/>
+      <c r="H19" s="203"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="204"/>
-      <c r="K19" s="207"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="222"/>
       <c r="L19" s="210"/>
-      <c r="M19" s="200"/>
+      <c r="M19" s="203"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B20" s="81">
         <v>16</v>
       </c>
@@ -3932,29 +3956,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="201" t="s">
+      <c r="H20" s="202" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="202" t="s">
+      <c r="J20" s="213" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="211" t="s">
+      <c r="K20" s="214" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="208" t="s">
+      <c r="L20" s="215" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="214" t="s">
+      <c r="M20" s="217" t="s">
         <v>116</v>
       </c>
       <c r="N20" s="42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B21" s="82">
         <v>17</v>
       </c>
@@ -3978,19 +4002,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="199"/>
+      <c r="H21" s="204"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="203"/>
-      <c r="K21" s="212"/>
+      <c r="J21" s="205"/>
+      <c r="K21" s="207"/>
       <c r="L21" s="209"/>
-      <c r="M21" s="215"/>
+      <c r="M21" s="218"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
         <v>18</v>
       </c>
@@ -4014,19 +4038,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="199"/>
+      <c r="H22" s="204"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="203"/>
-      <c r="K22" s="212"/>
+      <c r="J22" s="205"/>
+      <c r="K22" s="207"/>
       <c r="L22" s="209"/>
-      <c r="M22" s="215"/>
+      <c r="M22" s="218"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
         <v>19</v>
       </c>
@@ -4050,19 +4074,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="200"/>
+      <c r="H23" s="203"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="204"/>
-      <c r="K23" s="213"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="208"/>
       <c r="L23" s="210"/>
-      <c r="M23" s="216"/>
+      <c r="M23" s="219"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
         <v>20</v>
       </c>
@@ -4086,7 +4110,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="201" t="s">
+      <c r="H24" s="202" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4108,7 +4132,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B25" s="82">
         <v>21</v>
       </c>
@@ -4132,7 +4156,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="199"/>
+      <c r="H25" s="204"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4152,7 +4176,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B26" s="82">
         <v>22</v>
       </c>
@@ -4176,7 +4200,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="199"/>
+      <c r="H26" s="204"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4184,7 +4208,7 @@
       <c r="M26" s="106"/>
       <c r="N26" s="106"/>
     </row>
-    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
         <v>23</v>
       </c>
@@ -4208,7 +4232,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="200"/>
+      <c r="H27" s="203"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4216,7 +4240,7 @@
       <c r="M27" s="135"/>
       <c r="N27" s="135"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
         <v>24</v>
       </c>
@@ -4240,7 +4264,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="201" t="s">
+      <c r="H28" s="202" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4262,7 +4286,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B29" s="82">
         <v>25</v>
       </c>
@@ -4286,7 +4310,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="199"/>
+      <c r="H29" s="204"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4306,7 +4330,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B30" s="82">
         <v>26</v>
       </c>
@@ -4330,7 +4354,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="199"/>
+      <c r="H30" s="204"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4350,7 +4374,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="83">
         <v>27</v>
       </c>
@@ -4374,7 +4398,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="200"/>
+      <c r="H31" s="203"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4382,7 +4406,7 @@
       <c r="M31" s="97"/>
       <c r="N31" s="94"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B32" s="82">
         <v>28</v>
       </c>
@@ -4406,7 +4430,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="199" t="s">
+      <c r="H32" s="204" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4429,7 +4453,7 @@
       </c>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B33" s="82">
         <v>29</v>
       </c>
@@ -4453,7 +4477,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="199"/>
+      <c r="H33" s="204"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4474,7 +4498,7 @@
       </c>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="82">
         <v>30</v>
       </c>
@@ -4498,7 +4522,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="200"/>
+      <c r="H34" s="203"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4507,7 +4531,7 @@
       <c r="N34" s="94"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="84">
         <v>31</v>
       </c>
@@ -4555,17 +4579,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="M20:M23"/>
     <mergeCell ref="N6:N11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
@@ -4574,19 +4600,17 @@
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
     <mergeCell ref="M6:M11"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4601,24 +4625,24 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="5" width="4.7109375" customWidth="1"/>
+    <col min="3" max="5" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="220" t="s">
+    <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="199" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="222"/>
+      <c r="C2" s="200"/>
+      <c r="D2" s="200"/>
+      <c r="E2" s="201"/>
       <c r="F2" s="169" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
@@ -4633,7 +4657,7 @@
       </c>
       <c r="F3" s="170"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
         <v>0</v>
       </c>
@@ -4653,7 +4677,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -4673,7 +4697,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -4693,7 +4717,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -4713,7 +4737,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -4733,7 +4757,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -4753,7 +4777,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -4773,7 +4797,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -4806,40 +4830,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{197DCCAF-E75B-41F9-A939-BF94359E828F}">
   <dimension ref="B1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.45">
       <c r="B2" s="169" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="231" t="s">
+      <c r="C2" s="232" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="232"/>
-      <c r="E2" s="232"/>
-      <c r="F2" s="232"/>
-      <c r="G2" s="232"/>
-      <c r="H2" s="232"/>
-      <c r="I2" s="232"/>
-      <c r="J2" s="232"/>
-      <c r="K2" s="232"/>
-      <c r="L2" s="232"/>
-      <c r="M2" s="232"/>
-      <c r="N2" s="232"/>
-      <c r="O2" s="232"/>
-      <c r="P2" s="232"/>
-      <c r="Q2" s="232"/>
-      <c r="R2" s="233"/>
-    </row>
-    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="233"/>
+      <c r="E2" s="233"/>
+      <c r="F2" s="233"/>
+      <c r="G2" s="233"/>
+      <c r="H2" s="233"/>
+      <c r="I2" s="233"/>
+      <c r="J2" s="233"/>
+      <c r="K2" s="233"/>
+      <c r="L2" s="233"/>
+      <c r="M2" s="233"/>
+      <c r="N2" s="233"/>
+      <c r="O2" s="233"/>
+      <c r="P2" s="233"/>
+      <c r="Q2" s="233"/>
+      <c r="R2" s="234"/>
+    </row>
+    <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="170"/>
       <c r="C3" s="118">
         <v>15</v>
@@ -4890,7 +4914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="88" t="s">
         <v>82</v>
       </c>
@@ -4911,15 +4935,15 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="223" t="s">
+      <c r="N4" s="226" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="223"/>
-      <c r="P4" s="223"/>
-      <c r="Q4" s="223"/>
-      <c r="R4" s="224"/>
-    </row>
-    <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4" s="226"/>
+      <c r="P4" s="226"/>
+      <c r="Q4" s="226"/>
+      <c r="R4" s="227"/>
+    </row>
+    <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
         <v>3</v>
       </c>
@@ -4931,18 +4955,18 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="225" t="s">
+      <c r="K5" s="228" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="226"/>
-      <c r="M5" s="226"/>
-      <c r="N5" s="226"/>
-      <c r="O5" s="226"/>
-      <c r="P5" s="226"/>
-      <c r="Q5" s="226"/>
-      <c r="R5" s="227"/>
-    </row>
-    <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="224"/>
+      <c r="M5" s="224"/>
+      <c r="N5" s="224"/>
+      <c r="O5" s="224"/>
+      <c r="P5" s="224"/>
+      <c r="Q5" s="224"/>
+      <c r="R5" s="225"/>
+    </row>
+    <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
         <v>2</v>
       </c>
@@ -4954,18 +4978,18 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="225" t="s">
+      <c r="K6" s="228" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="226"/>
-      <c r="M6" s="226"/>
-      <c r="N6" s="226"/>
-      <c r="O6" s="226"/>
-      <c r="P6" s="226"/>
-      <c r="Q6" s="226"/>
-      <c r="R6" s="227"/>
-    </row>
-    <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="224"/>
+      <c r="M6" s="224"/>
+      <c r="N6" s="224"/>
+      <c r="O6" s="224"/>
+      <c r="P6" s="224"/>
+      <c r="Q6" s="224"/>
+      <c r="R6" s="225"/>
+    </row>
+    <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
         <v>83</v>
       </c>
@@ -4977,41 +5001,41 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="228" t="s">
+      <c r="K7" s="229" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="229"/>
-      <c r="M7" s="229"/>
-      <c r="N7" s="229"/>
-      <c r="O7" s="229"/>
-      <c r="P7" s="229"/>
-      <c r="Q7" s="229"/>
-      <c r="R7" s="230"/>
-    </row>
-    <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="230"/>
+      <c r="M7" s="230"/>
+      <c r="N7" s="230"/>
+      <c r="O7" s="230"/>
+      <c r="P7" s="230"/>
+      <c r="Q7" s="230"/>
+      <c r="R7" s="231"/>
+    </row>
+    <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="234" t="s">
+      <c r="C8" s="223" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="226"/>
-      <c r="E8" s="226"/>
-      <c r="F8" s="226"/>
-      <c r="G8" s="226"/>
-      <c r="H8" s="226"/>
-      <c r="I8" s="226"/>
-      <c r="J8" s="226"/>
-      <c r="K8" s="226"/>
-      <c r="L8" s="226"/>
-      <c r="M8" s="226"/>
-      <c r="N8" s="226"/>
-      <c r="O8" s="226"/>
-      <c r="P8" s="226"/>
-      <c r="Q8" s="226"/>
-      <c r="R8" s="227"/>
-    </row>
-    <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="224"/>
+      <c r="E8" s="224"/>
+      <c r="F8" s="224"/>
+      <c r="G8" s="224"/>
+      <c r="H8" s="224"/>
+      <c r="I8" s="224"/>
+      <c r="J8" s="224"/>
+      <c r="K8" s="224"/>
+      <c r="L8" s="224"/>
+      <c r="M8" s="224"/>
+      <c r="N8" s="224"/>
+      <c r="O8" s="224"/>
+      <c r="P8" s="224"/>
+      <c r="Q8" s="224"/>
+      <c r="R8" s="225"/>
+    </row>
+    <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
         <v>90</v>
       </c>
@@ -5055,20 +5079,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
-  <dimension ref="B1:C8"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="85.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.1328125" customWidth="1"/>
+    <col min="3" max="3" width="85.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="160" t="s">
         <v>155</v>
       </c>
@@ -5076,7 +5098,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" s="161" t="s">
         <v>121</v>
       </c>
@@ -5084,7 +5106,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" s="163" t="s">
         <v>122</v>
       </c>
@@ -5092,7 +5114,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" s="161" t="s">
         <v>128</v>
       </c>
@@ -5100,7 +5122,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" s="163" t="s">
         <v>123</v>
       </c>
@@ -5108,7 +5130,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B7" s="161" t="s">
         <v>124</v>
       </c>
@@ -5116,12 +5138,61 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="164" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="165" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="160" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="162" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B12" s="163" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B13" s="161" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" s="42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="163" t="s">
+        <v>163</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B15" s="161" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="164" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" s="165" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -5137,20 +5208,20 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="7.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B2" s="235" t="s">
         <v>144</v>
       </c>
       <c r="C2" s="236"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="143" t="s">
         <v>142</v>
       </c>
@@ -5159,7 +5230,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B4" s="93"/>
       <c r="C4" s="133" t="s">
         <v>146</v>
@@ -5168,21 +5239,21 @@
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="95"/>
       <c r="C5" s="134" t="s">
         <v>145</v>
       </c>
       <c r="D5" s="238"/>
     </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>147</v>
       </c>
       <c r="D6" s="239"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>146</v>
       </c>
@@ -5191,21 +5262,21 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" s="41" t="s">
         <v>145</v>
       </c>
       <c r="C8" s="146"/>
       <c r="D8" s="241"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>147</v>
       </c>
       <c r="C9" s="146"/>
       <c r="D9" s="241"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
         <v>148</v>
       </c>
@@ -5214,7 +5285,7 @@
       </c>
       <c r="D10" s="241"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
         <v>145</v>
       </c>
@@ -5224,7 +5295,7 @@
       <c r="D11" s="241"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B12" s="149" t="s">
         <v>149</v>
       </c>

</xml_diff>

<commit_message>
corrected hardware clock cycle documentation
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5535E9-88E0-46DA-B174-3BADAB2D3DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB679B66-88B8-4BE1-B035-1E387F9E80BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="169">
   <si>
     <t>MODE B</t>
   </si>
@@ -544,6 +544,12 @@
   </si>
   <si>
     <t>Increments PC</t>
+  </si>
+  <si>
+    <t>Switch output address to PC</t>
+  </si>
+  <si>
+    <t>PRE INCREMENT</t>
   </si>
 </sst>
 </file>
@@ -1895,6 +1901,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1931,61 +1976,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1994,16 +1994,40 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2012,35 +2036,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3103,73 +3109,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="183" t="s">
+      <c r="C3" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="180" t="s">
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="193" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="181"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="180" t="s">
+      <c r="I3" s="194"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="193" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="181"/>
-      <c r="M3" s="181"/>
-      <c r="N3" s="192" t="s">
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="193"/>
-      <c r="P3" s="194"/>
+      <c r="O3" s="181"/>
+      <c r="P3" s="182"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="186" t="s">
+      <c r="S3" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="187"/>
-      <c r="U3" s="187"/>
-      <c r="V3" s="187"/>
-      <c r="W3" s="187"/>
-      <c r="X3" s="187"/>
-      <c r="Y3" s="187"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="189" t="s">
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="177" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="190"/>
-      <c r="AC3" s="190"/>
-      <c r="AD3" s="190"/>
-      <c r="AE3" s="190"/>
-      <c r="AF3" s="190"/>
-      <c r="AG3" s="190"/>
-      <c r="AH3" s="191"/>
+      <c r="AB3" s="178"/>
+      <c r="AC3" s="178"/>
+      <c r="AD3" s="178"/>
+      <c r="AE3" s="178"/>
+      <c r="AF3" s="178"/>
+      <c r="AG3" s="178"/>
+      <c r="AH3" s="179"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="185" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="195" t="s">
+      <c r="C5" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="195"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="195"/>
-      <c r="J5" s="196"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="184"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="198"/>
+      <c r="B6" s="186"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3199,16 +3205,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="174" t="s">
+      <c r="C7" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="176"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="188"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="189"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3218,25 +3224,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="177" t="s">
+      <c r="G8" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="H8" s="191"/>
+      <c r="I8" s="191"/>
+      <c r="J8" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3264,25 +3270,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="220" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="222"/>
       <c r="H2" s="169" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="199" t="s">
+      <c r="J2" s="220" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
       <c r="M2" s="169" t="s">
         <v>115</v>
       </c>
@@ -3347,7 +3353,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="201" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3393,7 +3399,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="200"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3437,25 +3443,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="199" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="205" t="s">
+      <c r="J6" s="203" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="212" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="217" t="s">
+      <c r="M6" s="214" t="s">
         <v>116</v>
       </c>
-      <c r="N6" s="211" t="s">
+      <c r="N6" s="217" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3483,15 +3489,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
+      <c r="H7" s="199"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="205"/>
-      <c r="K7" s="207"/>
+      <c r="J7" s="203"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="209"/>
-      <c r="M7" s="218"/>
-      <c r="N7" s="211"/>
+      <c r="M7" s="215"/>
+      <c r="N7" s="217"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3517,15 +3523,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
+      <c r="H8" s="199"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="205"/>
-      <c r="K8" s="207"/>
+      <c r="J8" s="203"/>
+      <c r="K8" s="212"/>
       <c r="L8" s="209"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="211"/>
+      <c r="M8" s="215"/>
+      <c r="N8" s="217"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3551,15 +3557,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
+      <c r="H9" s="199"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="205"/>
-      <c r="K9" s="207"/>
+      <c r="J9" s="203"/>
+      <c r="K9" s="212"/>
       <c r="L9" s="209"/>
-      <c r="M9" s="218"/>
-      <c r="N9" s="211"/>
+      <c r="M9" s="215"/>
+      <c r="N9" s="217"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3585,15 +3591,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="199"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="205"/>
-      <c r="K10" s="207"/>
+      <c r="J10" s="203"/>
+      <c r="K10" s="212"/>
       <c r="L10" s="209"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="211"/>
+      <c r="M10" s="215"/>
+      <c r="N10" s="217"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3619,15 +3625,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="203"/>
+      <c r="H11" s="200"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="206"/>
-      <c r="K11" s="208"/>
+      <c r="J11" s="204"/>
+      <c r="K11" s="213"/>
       <c r="L11" s="210"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="212"/>
+      <c r="M11" s="216"/>
+      <c r="N11" s="218"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3653,25 +3659,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="201" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="213" t="s">
+      <c r="J12" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="214" t="s">
+      <c r="K12" s="211" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="215" t="s">
+      <c r="L12" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="202" t="s">
+      <c r="M12" s="201" t="s">
         <v>117</v>
       </c>
-      <c r="N12" s="216" t="s">
+      <c r="N12" s="219" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3699,15 +3705,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="199"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="205"/>
-      <c r="K13" s="207"/>
+      <c r="J13" s="203"/>
+      <c r="K13" s="212"/>
       <c r="L13" s="209"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="211"/>
+      <c r="M13" s="199"/>
+      <c r="N13" s="217"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3733,15 +3739,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="199"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="205"/>
-      <c r="K14" s="207"/>
+      <c r="J14" s="203"/>
+      <c r="K14" s="212"/>
       <c r="L14" s="209"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="211"/>
+      <c r="M14" s="199"/>
+      <c r="N14" s="217"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3767,15 +3773,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="203"/>
+      <c r="H15" s="200"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="206"/>
-      <c r="K15" s="208"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="213"/>
       <c r="L15" s="210"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="212"/>
+      <c r="M15" s="200"/>
+      <c r="N15" s="218"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3801,22 +3807,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="202" t="s">
+      <c r="H16" s="201" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="213" t="s">
+      <c r="J16" s="202" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="220" t="s">
+      <c r="K16" s="205" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="215" t="s">
+      <c r="L16" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="202" t="s">
+      <c r="M16" s="201" t="s">
         <v>117</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -3847,14 +3853,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="199"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="205"/>
-      <c r="K17" s="221"/>
+      <c r="J17" s="203"/>
+      <c r="K17" s="206"/>
       <c r="L17" s="209"/>
-      <c r="M17" s="204"/>
+      <c r="M17" s="199"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -3883,14 +3889,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
+      <c r="H18" s="199"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="205"/>
-      <c r="K18" s="221"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="206"/>
       <c r="L18" s="209"/>
-      <c r="M18" s="204"/>
+      <c r="M18" s="199"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -3919,14 +3925,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="203"/>
+      <c r="H19" s="200"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="206"/>
-      <c r="K19" s="222"/>
+      <c r="J19" s="204"/>
+      <c r="K19" s="207"/>
       <c r="L19" s="210"/>
-      <c r="M19" s="203"/>
+      <c r="M19" s="200"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -3956,22 +3962,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="202" t="s">
+      <c r="H20" s="201" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="213" t="s">
+      <c r="J20" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="214" t="s">
+      <c r="K20" s="211" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="215" t="s">
+      <c r="L20" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="217" t="s">
+      <c r="M20" s="214" t="s">
         <v>116</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4002,14 +4008,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="204"/>
+      <c r="H21" s="199"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="205"/>
-      <c r="K21" s="207"/>
+      <c r="J21" s="203"/>
+      <c r="K21" s="212"/>
       <c r="L21" s="209"/>
-      <c r="M21" s="218"/>
+      <c r="M21" s="215"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4038,14 +4044,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="204"/>
+      <c r="H22" s="199"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="205"/>
-      <c r="K22" s="207"/>
+      <c r="J22" s="203"/>
+      <c r="K22" s="212"/>
       <c r="L22" s="209"/>
-      <c r="M22" s="218"/>
+      <c r="M22" s="215"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4074,14 +4080,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="203"/>
+      <c r="H23" s="200"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="206"/>
-      <c r="K23" s="208"/>
+      <c r="J23" s="204"/>
+      <c r="K23" s="213"/>
       <c r="L23" s="210"/>
-      <c r="M23" s="219"/>
+      <c r="M23" s="216"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4110,7 +4116,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="202" t="s">
+      <c r="H24" s="201" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4156,7 +4162,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="199"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4200,7 +4206,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
+      <c r="H26" s="199"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4232,7 +4238,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="203"/>
+      <c r="H27" s="200"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4264,7 +4270,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="202" t="s">
+      <c r="H28" s="201" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4310,7 +4316,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="199"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4354,7 +4360,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="199"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4398,7 +4404,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="203"/>
+      <c r="H31" s="200"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4430,7 +4436,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="199" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4477,7 +4483,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="199"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4522,7 +4528,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="203"/>
+      <c r="H34" s="200"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4579,11 +4585,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4592,25 +4612,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4632,12 +4638,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="220" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="222"/>
       <c r="F2" s="169" t="s">
         <v>32</v>
       </c>
@@ -5079,9 +5085,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5180,18 +5188,26 @@
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B15" s="161" t="s">
+      <c r="B15" s="163" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="42" t="s">
+      <c r="C15" s="75" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="164" t="s">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="161" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="164" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="165" t="s">
+      <c r="C17" s="165" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use UART for IO module
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\computer\ax08-pc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32296325-F7CF-4F66-AB10-50DC0BB2CB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C416CC6A-8BF0-4A69-B70E-4E00D10B3725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="2" r:id="rId1"/>
@@ -378,15 +378,6 @@
     <t>Pops a value from the stack and writes it to the PC</t>
   </si>
   <si>
-    <t>Returns 1 if a new value is available from rs232 unit, otherwise returns 0.</t>
-  </si>
-  <si>
-    <t>Copies the value from the rs232 unit and returns it.</t>
-  </si>
-  <si>
-    <t>Writes the value to the rs232 unit.</t>
-  </si>
-  <si>
     <t>Causes the computer to enter a breakpoint.</t>
   </si>
   <si>
@@ -550,6 +541,15 @@
   </si>
   <si>
     <t>PRE INCREMENT</t>
+  </si>
+  <si>
+    <t>Returns 1 if a new value is available from UART unit, otherwise returns 0.</t>
+  </si>
+  <si>
+    <t>Copies the value from the UART unit and returns it.</t>
+  </si>
+  <si>
+    <t>Writes the value to the UART unit.</t>
   </si>
 </sst>
 </file>
@@ -1901,6 +1901,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1937,61 +1976,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2000,16 +1994,40 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2018,35 +2036,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2110,7 +2110,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2131,7 +2131,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2453,15 +2453,15 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="6" width="4.73046875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.1328125" customWidth="1"/>
-    <col min="10" max="10" width="34.265625" customWidth="1"/>
+    <col min="3" max="6" width="4.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="166" t="s">
         <v>15</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="57" t="s">
         <v>16</v>
       </c>
@@ -2501,11 +2501,11 @@
         <v>53</v>
       </c>
       <c r="I3" s="51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="J3" s="170"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="107">
         <v>0</v>
       </c>
@@ -2526,19 +2526,19 @@
         <v>0</v>
       </c>
       <c r="G4" s="119" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H4" s="126" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="I4" s="110" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J4" s="108" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -2559,19 +2559,19 @@
         <v>1</v>
       </c>
       <c r="G5" s="120" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H5" s="127" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I5" s="111" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J5" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -2592,19 +2592,19 @@
         <v>0</v>
       </c>
       <c r="G6" s="121" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H6" s="128" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I6" s="112" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J6" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -2625,19 +2625,19 @@
         <v>1</v>
       </c>
       <c r="G7" s="122" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H7" s="129" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="I7" s="113" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J7" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -2658,19 +2658,19 @@
         <v>0</v>
       </c>
       <c r="G8" s="120" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H8" s="127" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="I8" s="111" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J8" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -2691,19 +2691,19 @@
         <v>1</v>
       </c>
       <c r="G9" s="120" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="H9" s="127" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I9" s="111" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J9" s="26" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -2724,19 +2724,19 @@
         <v>0</v>
       </c>
       <c r="G10" s="121" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H10" s="128" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I10" s="112" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J10" s="28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -2757,19 +2757,19 @@
         <v>1</v>
       </c>
       <c r="G11" s="122" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H11" s="129" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="I11" s="113" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J11" s="30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="13">
         <v>8</v>
       </c>
@@ -2790,17 +2790,17 @@
         <v>0</v>
       </c>
       <c r="G12" s="121" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H12" s="151" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="I12" s="116"/>
       <c r="J12" s="28" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="13">
         <v>9</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="120" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H13" s="152"/>
       <c r="I13" s="115"/>
@@ -2829,7 +2829,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="19">
         <v>10</v>
       </c>
@@ -2854,7 +2854,7 @@
       <c r="I14" s="116"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="22">
         <v>11</v>
       </c>
@@ -2875,17 +2875,17 @@
         <v>1</v>
       </c>
       <c r="G15" s="122" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H15" s="142" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I15" s="114"/>
       <c r="J15" s="30" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="13">
         <v>12</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="I16" s="115"/>
       <c r="J16" s="31"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="13">
         <v>13</v>
       </c>
@@ -2935,7 +2935,7 @@
       <c r="I17" s="115"/>
       <c r="J17" s="31"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="19">
         <v>14</v>
       </c>
@@ -2960,7 +2960,7 @@
       <c r="I18" s="116"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="16">
         <v>15</v>
       </c>
@@ -3001,16 +3001,16 @@
   <dimension ref="B1:AH8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="H3" sqref="H3:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="34" width="7.73046875" customWidth="1"/>
+    <col min="3" max="34" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2">
         <v>31</v>
       </c>
@@ -3108,74 +3108,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="183" t="s">
+    <row r="3" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="180" t="s">
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="193" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="181"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="180" t="s">
+      <c r="I3" s="194"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="193" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="181"/>
-      <c r="M3" s="181"/>
-      <c r="N3" s="192" t="s">
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="193"/>
-      <c r="P3" s="194"/>
+      <c r="O3" s="181"/>
+      <c r="P3" s="182"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="186" t="s">
+      <c r="S3" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="187"/>
-      <c r="U3" s="187"/>
-      <c r="V3" s="187"/>
-      <c r="W3" s="187"/>
-      <c r="X3" s="187"/>
-      <c r="Y3" s="187"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="189" t="s">
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="177" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="190"/>
-      <c r="AC3" s="190"/>
-      <c r="AD3" s="190"/>
-      <c r="AE3" s="190"/>
-      <c r="AF3" s="190"/>
-      <c r="AG3" s="190"/>
-      <c r="AH3" s="191"/>
-    </row>
-    <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="197" t="s">
+      <c r="AB3" s="178"/>
+      <c r="AC3" s="178"/>
+      <c r="AD3" s="178"/>
+      <c r="AE3" s="178"/>
+      <c r="AF3" s="178"/>
+      <c r="AG3" s="178"/>
+      <c r="AH3" s="179"/>
+    </row>
+    <row r="4" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B5" s="185" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="195" t="s">
+      <c r="C5" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="195"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="195"/>
-      <c r="J5" s="196"/>
-    </row>
-    <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="198"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="184"/>
+    </row>
+    <row r="6" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="186"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3201,22 +3201,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="174" t="s">
+      <c r="C7" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="176"/>
-    </row>
-    <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="188"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="189"/>
+    </row>
+    <row r="8" spans="2:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -3224,25 +3224,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="177" t="s">
+      <c r="G8" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="H8" s="191"/>
+      <c r="I8" s="191"/>
+      <c r="J8" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3253,50 +3253,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B20B11-9266-4E5E-A2B3-3496A1A10C3B}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.1328125" style="1"/>
-    <col min="3" max="7" width="4.73046875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="16.73046875" style="1" customWidth="1"/>
-    <col min="10" max="12" width="20.73046875" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="7" width="4.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" style="1" customWidth="1"/>
+    <col min="10" max="12" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="90.265625" customWidth="1"/>
+    <col min="14" max="14" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+    <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="220" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="222"/>
       <c r="H2" s="169" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="199" t="s">
+      <c r="J2" s="220" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
       <c r="M2" s="169" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="N2" s="169" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="85" t="s">
         <v>16</v>
       </c>
@@ -3329,7 +3329,7 @@
       <c r="M3" s="170"/>
       <c r="N3" s="170"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="81">
         <v>0</v>
       </c>
@@ -3353,7 +3353,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="201" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3363,19 +3363,19 @@
         <v>85</v>
       </c>
       <c r="K4" s="67" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L4" s="70" t="s">
         <v>44</v>
       </c>
       <c r="M4" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="N4" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="N4" s="76" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="5" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="83">
         <v>1</v>
       </c>
@@ -3399,7 +3399,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="200"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3413,13 +3413,13 @@
         <v>66</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N5" s="45" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="82">
         <v>2</v>
       </c>
@@ -3443,29 +3443,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="199" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="205" t="s">
+      <c r="J6" s="203" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="212" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="217" t="s">
-        <v>116</v>
-      </c>
-      <c r="N6" s="211" t="s">
+      <c r="M6" s="214" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" s="217" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="82">
         <v>3</v>
       </c>
@@ -3489,17 +3489,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
+      <c r="H7" s="199"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="205"/>
-      <c r="K7" s="207"/>
+      <c r="J7" s="203"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="209"/>
-      <c r="M7" s="218"/>
-      <c r="N7" s="211"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M7" s="215"/>
+      <c r="N7" s="217"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="82">
         <v>4</v>
       </c>
@@ -3523,17 +3523,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
+      <c r="H8" s="199"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="205"/>
-      <c r="K8" s="207"/>
+      <c r="J8" s="203"/>
+      <c r="K8" s="212"/>
       <c r="L8" s="209"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="211"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M8" s="215"/>
+      <c r="N8" s="217"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="82">
         <v>5</v>
       </c>
@@ -3557,17 +3557,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
+      <c r="H9" s="199"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="205"/>
-      <c r="K9" s="207"/>
+      <c r="J9" s="203"/>
+      <c r="K9" s="212"/>
       <c r="L9" s="209"/>
-      <c r="M9" s="218"/>
-      <c r="N9" s="211"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M9" s="215"/>
+      <c r="N9" s="217"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="82">
         <v>6</v>
       </c>
@@ -3591,17 +3591,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="199"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="205"/>
-      <c r="K10" s="207"/>
+      <c r="J10" s="203"/>
+      <c r="K10" s="212"/>
       <c r="L10" s="209"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="211"/>
-    </row>
-    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M10" s="215"/>
+      <c r="N10" s="217"/>
+    </row>
+    <row r="11" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="83">
         <v>7</v>
       </c>
@@ -3625,17 +3625,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="203"/>
+      <c r="H11" s="200"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="206"/>
-      <c r="K11" s="208"/>
+      <c r="J11" s="204"/>
+      <c r="K11" s="213"/>
       <c r="L11" s="210"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="212"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M11" s="216"/>
+      <c r="N11" s="218"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="81">
         <v>8</v>
       </c>
@@ -3659,29 +3659,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="201" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="213" t="s">
+      <c r="J12" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="214" t="s">
+      <c r="K12" s="211" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="215" t="s">
+      <c r="L12" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="202" t="s">
-        <v>117</v>
-      </c>
-      <c r="N12" s="216" t="s">
+      <c r="M12" s="201" t="s">
+        <v>114</v>
+      </c>
+      <c r="N12" s="219" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="82">
         <v>9</v>
       </c>
@@ -3705,17 +3705,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="199"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="205"/>
-      <c r="K13" s="207"/>
+      <c r="J13" s="203"/>
+      <c r="K13" s="212"/>
       <c r="L13" s="209"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="211"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M13" s="199"/>
+      <c r="N13" s="217"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="82">
         <v>10</v>
       </c>
@@ -3739,17 +3739,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="199"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="205"/>
-      <c r="K14" s="207"/>
+      <c r="J14" s="203"/>
+      <c r="K14" s="212"/>
       <c r="L14" s="209"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="211"/>
-    </row>
-    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M14" s="199"/>
+      <c r="N14" s="217"/>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="83">
         <v>11</v>
       </c>
@@ -3773,17 +3773,17 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="203"/>
+      <c r="H15" s="200"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="206"/>
-      <c r="K15" s="208"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="213"/>
       <c r="L15" s="210"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="212"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M15" s="200"/>
+      <c r="N15" s="218"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="81">
         <v>12</v>
       </c>
@@ -3807,29 +3807,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="202" t="s">
+      <c r="H16" s="201" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="213" t="s">
+      <c r="J16" s="202" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="220" t="s">
+      <c r="K16" s="205" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="215" t="s">
+      <c r="L16" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="202" t="s">
-        <v>117</v>
+      <c r="M16" s="201" t="s">
+        <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="82">
         <v>13</v>
       </c>
@@ -3853,19 +3853,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="199"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="205"/>
-      <c r="K17" s="221"/>
+      <c r="J17" s="203"/>
+      <c r="K17" s="206"/>
       <c r="L17" s="209"/>
-      <c r="M17" s="204"/>
+      <c r="M17" s="199"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="82">
         <v>14</v>
       </c>
@@ -3889,19 +3889,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
+      <c r="H18" s="199"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="205"/>
-      <c r="K18" s="221"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="206"/>
       <c r="L18" s="209"/>
-      <c r="M18" s="204"/>
+      <c r="M18" s="199"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="83">
         <v>15</v>
       </c>
@@ -3925,20 +3925,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="203"/>
+      <c r="H19" s="200"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="206"/>
-      <c r="K19" s="222"/>
+      <c r="J19" s="204"/>
+      <c r="K19" s="207"/>
       <c r="L19" s="210"/>
-      <c r="M19" s="203"/>
+      <c r="M19" s="200"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="81">
         <v>16</v>
       </c>
@@ -3962,29 +3962,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="202" t="s">
+      <c r="H20" s="201" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="213" t="s">
+      <c r="J20" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="214" t="s">
+      <c r="K20" s="211" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="215" t="s">
+      <c r="L20" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="217" t="s">
-        <v>116</v>
+      <c r="M20" s="214" t="s">
+        <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="82">
         <v>17</v>
       </c>
@@ -4008,19 +4008,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="204"/>
+      <c r="H21" s="199"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="205"/>
-      <c r="K21" s="207"/>
+      <c r="J21" s="203"/>
+      <c r="K21" s="212"/>
       <c r="L21" s="209"/>
-      <c r="M21" s="218"/>
+      <c r="M21" s="215"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="82">
         <v>18</v>
       </c>
@@ -4044,19 +4044,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="204"/>
+      <c r="H22" s="199"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="205"/>
-      <c r="K22" s="207"/>
+      <c r="J22" s="203"/>
+      <c r="K22" s="212"/>
       <c r="L22" s="209"/>
-      <c r="M22" s="218"/>
+      <c r="M22" s="215"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="82">
         <v>19</v>
       </c>
@@ -4080,19 +4080,19 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="203"/>
+      <c r="H23" s="200"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="206"/>
-      <c r="K23" s="208"/>
+      <c r="J23" s="204"/>
+      <c r="K23" s="213"/>
       <c r="L23" s="210"/>
-      <c r="M23" s="219"/>
+      <c r="M23" s="216"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="81">
         <v>20</v>
       </c>
@@ -4116,7 +4116,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="202" t="s">
+      <c r="H24" s="201" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4132,13 +4132,13 @@
         <v>16</v>
       </c>
       <c r="M24" s="103" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N24" s="76" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="82">
         <v>21</v>
       </c>
@@ -4162,7 +4162,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="199"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4176,13 +4176,13 @@
         <v>44</v>
       </c>
       <c r="M25" s="100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N25" s="75" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="82">
         <v>22</v>
       </c>
@@ -4206,7 +4206,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
+      <c r="H26" s="199"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4214,7 +4214,7 @@
       <c r="M26" s="106"/>
       <c r="N26" s="106"/>
     </row>
-    <row r="27" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="83">
         <v>23</v>
       </c>
@@ -4238,7 +4238,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="203"/>
+      <c r="H27" s="200"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4246,7 +4246,7 @@
       <c r="M27" s="135"/>
       <c r="N27" s="135"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="81">
         <v>24</v>
       </c>
@@ -4270,7 +4270,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="202" t="s">
+      <c r="H28" s="201" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4286,13 +4286,13 @@
         <v>62</v>
       </c>
       <c r="M28" s="99" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="82">
         <v>25</v>
       </c>
@@ -4316,7 +4316,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="199"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4330,13 +4330,13 @@
         <v>63</v>
       </c>
       <c r="M29" s="100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N29" s="75" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="82">
         <v>26</v>
       </c>
@@ -4360,7 +4360,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="199"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4374,13 +4374,13 @@
         <v>44</v>
       </c>
       <c r="M30" s="100" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N30" s="75" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="83">
         <v>27</v>
       </c>
@@ -4404,7 +4404,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="203"/>
+      <c r="H31" s="200"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4412,7 +4412,7 @@
       <c r="M31" s="97"/>
       <c r="N31" s="94"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="82">
         <v>28</v>
       </c>
@@ -4436,7 +4436,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="199" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4452,14 +4452,14 @@
         <v>44</v>
       </c>
       <c r="M32" s="70" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N32" s="76" t="s">
         <v>109</v>
       </c>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="82">
         <v>29</v>
       </c>
@@ -4483,7 +4483,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="199"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4497,14 +4497,14 @@
         <v>44</v>
       </c>
       <c r="M33" s="102" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N33" s="75" t="s">
         <v>110</v>
       </c>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="82">
         <v>30</v>
       </c>
@@ -4528,7 +4528,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="203"/>
+      <c r="H34" s="200"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4537,7 +4537,7 @@
       <c r="N34" s="94"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="84">
         <v>31</v>
       </c>
@@ -4577,19 +4577,33 @@
         <v>44</v>
       </c>
       <c r="M35" s="33" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="N35" s="47" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4598,25 +4612,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4631,24 +4631,24 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="5" width="4.73046875" customWidth="1"/>
+    <col min="3" max="5" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="220" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="222"/>
       <c r="F2" s="169" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
         <v>16</v>
       </c>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="F3" s="170"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="13">
         <v>0</v>
       </c>
@@ -4683,7 +4683,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>1</v>
       </c>
@@ -4703,7 +4703,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -4723,7 +4723,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="22">
         <v>3</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="13">
         <v>4</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>5</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="19">
         <v>6</v>
       </c>
@@ -4803,7 +4803,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="22">
         <v>7</v>
       </c>
@@ -4840,13 +4840,13 @@
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.265625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="169" t="s">
         <v>81</v>
       </c>
@@ -4869,7 +4869,7 @@
       <c r="Q2" s="233"/>
       <c r="R2" s="234"/>
     </row>
-    <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="170"/>
       <c r="C3" s="118">
         <v>15</v>
@@ -4920,7 +4920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="88" t="s">
         <v>82</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="Q4" s="226"/>
       <c r="R4" s="227"/>
     </row>
-    <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="89" t="s">
         <v>3</v>
       </c>
@@ -4972,7 +4972,7 @@
       <c r="Q5" s="224"/>
       <c r="R5" s="225"/>
     </row>
-    <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="89" t="s">
         <v>2</v>
       </c>
@@ -4995,7 +4995,7 @@
       <c r="Q6" s="224"/>
       <c r="R6" s="225"/>
     </row>
-    <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="89" t="s">
         <v>83</v>
       </c>
@@ -5018,12 +5018,12 @@
       <c r="Q7" s="230"/>
       <c r="R7" s="231"/>
     </row>
-    <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
       <c r="C8" s="223" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D8" s="224"/>
       <c r="E8" s="224"/>
@@ -5041,7 +5041,7 @@
       <c r="Q8" s="224"/>
       <c r="R8" s="225"/>
     </row>
-    <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="90" t="s">
         <v>90</v>
       </c>
@@ -5087,126 +5087,128 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
   <dimension ref="B1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="85.73046875" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="85.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="160" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2" s="162" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="161" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="163" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="161" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="163" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="161" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B4" s="163" t="s">
-        <v>122</v>
-      </c>
-      <c r="C4" s="75" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B5" s="161" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B6" s="163" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B7" s="161" t="s">
+      <c r="C7" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="164" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="165" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="160" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="162" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="163" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="161" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="160" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="162" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B12" s="163" t="s">
+      <c r="C13" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="75" t="s">
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="163" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B13" s="161" t="s">
+      <c r="C14" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="42" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B14" s="163" t="s">
-        <v>163</v>
-      </c>
-      <c r="C14" s="75" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="163" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="75" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="161" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="161" t="s">
-        <v>168</v>
-      </c>
       <c r="C16" s="42" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="164" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C17" s="165" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5222,99 +5224,99 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="7.265625" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="235" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C2" s="236"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="143" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C3" s="150" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="93"/>
       <c r="C4" s="133" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D4" s="237" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="95"/>
       <c r="C5" s="134" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D5" s="238"/>
     </row>
-    <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D6" s="239"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="144" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C7" s="145"/>
       <c r="D7" s="240" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C8" s="146"/>
       <c r="D8" s="241"/>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C9" s="146"/>
       <c r="D9" s="241"/>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="147" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C10" s="148" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D10" s="241"/>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C11" s="134" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D11" s="241"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="149" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D12" s="242"/>
     </row>

</xml_diff>

<commit_message>
added general architecture master documentation (final)
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2F4F2A-BFF4-4491-AC98-97662F9B16F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11366203-CD24-4D1F-BEB1-508778DEDBCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
   <sheets>
     <sheet name="registers" sheetId="2" r:id="rId1"/>
@@ -534,9 +534,6 @@
     <t>Stores output to register</t>
   </si>
   <si>
-    <t>Increments PC</t>
-  </si>
-  <si>
     <t>Switch output address to PC</t>
   </si>
   <si>
@@ -550,6 +547,9 @@
   </si>
   <si>
     <t>Writes the value to the UART unit.</t>
+  </si>
+  <si>
+    <t>Updates PC</t>
   </si>
 </sst>
 </file>
@@ -1901,6 +1901,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1937,61 +1976,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2000,16 +1994,40 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2018,35 +2036,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F30110-9AA6-4607-84AE-181659F51D05}">
   <dimension ref="B1:J19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3000,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE0A35C-77D4-4A92-BE06-765002DB2402}">
   <dimension ref="B1:AH8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:J3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3109,73 +3109,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="183" t="s">
+      <c r="C3" s="196" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="180" t="s">
+      <c r="D3" s="197"/>
+      <c r="E3" s="197"/>
+      <c r="F3" s="197"/>
+      <c r="G3" s="198"/>
+      <c r="H3" s="193" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="181"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="180" t="s">
+      <c r="I3" s="194"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="193" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="181"/>
-      <c r="M3" s="181"/>
-      <c r="N3" s="192" t="s">
+      <c r="L3" s="194"/>
+      <c r="M3" s="194"/>
+      <c r="N3" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="193"/>
-      <c r="P3" s="194"/>
+      <c r="O3" s="181"/>
+      <c r="P3" s="182"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="186" t="s">
+      <c r="S3" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="187"/>
-      <c r="U3" s="187"/>
-      <c r="V3" s="187"/>
-      <c r="W3" s="187"/>
-      <c r="X3" s="187"/>
-      <c r="Y3" s="187"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="189" t="s">
+      <c r="T3" s="175"/>
+      <c r="U3" s="175"/>
+      <c r="V3" s="175"/>
+      <c r="W3" s="175"/>
+      <c r="X3" s="175"/>
+      <c r="Y3" s="175"/>
+      <c r="Z3" s="176"/>
+      <c r="AA3" s="177" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="190"/>
-      <c r="AC3" s="190"/>
-      <c r="AD3" s="190"/>
-      <c r="AE3" s="190"/>
-      <c r="AF3" s="190"/>
-      <c r="AG3" s="190"/>
-      <c r="AH3" s="191"/>
+      <c r="AB3" s="178"/>
+      <c r="AC3" s="178"/>
+      <c r="AD3" s="178"/>
+      <c r="AE3" s="178"/>
+      <c r="AF3" s="178"/>
+      <c r="AG3" s="178"/>
+      <c r="AH3" s="179"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="185" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="195" t="s">
+      <c r="C5" s="183" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="195"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="195"/>
-      <c r="J5" s="196"/>
+      <c r="D5" s="183"/>
+      <c r="E5" s="183"/>
+      <c r="F5" s="183"/>
+      <c r="G5" s="183"/>
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="184"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="198"/>
+      <c r="B6" s="186"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3205,16 +3205,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="174" t="s">
+      <c r="C7" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="176"/>
+      <c r="D7" s="188"/>
+      <c r="E7" s="188"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="188"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
+      <c r="J7" s="189"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3224,25 +3224,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="177" t="s">
+      <c r="G8" s="190" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="H8" s="191"/>
+      <c r="I8" s="191"/>
+      <c r="J8" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3254,7 +3254,7 @@
   <dimension ref="B1:Q35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3270,25 +3270,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="220" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="221"/>
+      <c r="F2" s="221"/>
+      <c r="G2" s="222"/>
       <c r="H2" s="169" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="169" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="199" t="s">
+      <c r="J2" s="220" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
+      <c r="K2" s="221"/>
+      <c r="L2" s="221"/>
       <c r="M2" s="169" t="s">
         <v>112</v>
       </c>
@@ -3353,7 +3353,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="201" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3399,7 +3399,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="200"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3443,25 +3443,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="199" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="205" t="s">
+      <c r="J6" s="203" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="212" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="209" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="217" t="s">
+      <c r="M6" s="214" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="211" t="s">
+      <c r="N6" s="217" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3489,15 +3489,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
+      <c r="H7" s="199"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="205"/>
-      <c r="K7" s="207"/>
+      <c r="J7" s="203"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="209"/>
-      <c r="M7" s="218"/>
-      <c r="N7" s="211"/>
+      <c r="M7" s="215"/>
+      <c r="N7" s="217"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3523,15 +3523,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
+      <c r="H8" s="199"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="205"/>
-      <c r="K8" s="207"/>
+      <c r="J8" s="203"/>
+      <c r="K8" s="212"/>
       <c r="L8" s="209"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="211"/>
+      <c r="M8" s="215"/>
+      <c r="N8" s="217"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3557,15 +3557,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
+      <c r="H9" s="199"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="205"/>
-      <c r="K9" s="207"/>
+      <c r="J9" s="203"/>
+      <c r="K9" s="212"/>
       <c r="L9" s="209"/>
-      <c r="M9" s="218"/>
-      <c r="N9" s="211"/>
+      <c r="M9" s="215"/>
+      <c r="N9" s="217"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3591,15 +3591,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="199"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="205"/>
-      <c r="K10" s="207"/>
+      <c r="J10" s="203"/>
+      <c r="K10" s="212"/>
       <c r="L10" s="209"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="211"/>
+      <c r="M10" s="215"/>
+      <c r="N10" s="217"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3625,15 +3625,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="203"/>
+      <c r="H11" s="200"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="206"/>
-      <c r="K11" s="208"/>
+      <c r="J11" s="204"/>
+      <c r="K11" s="213"/>
       <c r="L11" s="210"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="212"/>
+      <c r="M11" s="216"/>
+      <c r="N11" s="218"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3659,25 +3659,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="201" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="213" t="s">
+      <c r="J12" s="202" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="214" t="s">
+      <c r="K12" s="211" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="215" t="s">
+      <c r="L12" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="202" t="s">
+      <c r="M12" s="201" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="216" t="s">
+      <c r="N12" s="219" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3705,15 +3705,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="199"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="205"/>
-      <c r="K13" s="207"/>
+      <c r="J13" s="203"/>
+      <c r="K13" s="212"/>
       <c r="L13" s="209"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="211"/>
+      <c r="M13" s="199"/>
+      <c r="N13" s="217"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3739,15 +3739,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="199"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="205"/>
-      <c r="K14" s="207"/>
+      <c r="J14" s="203"/>
+      <c r="K14" s="212"/>
       <c r="L14" s="209"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="211"/>
+      <c r="M14" s="199"/>
+      <c r="N14" s="217"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3773,15 +3773,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="203"/>
+      <c r="H15" s="200"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="206"/>
-      <c r="K15" s="208"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="213"/>
       <c r="L15" s="210"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="212"/>
+      <c r="M15" s="200"/>
+      <c r="N15" s="218"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3807,22 +3807,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="202" t="s">
+      <c r="H16" s="201" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="213" t="s">
+      <c r="J16" s="202" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="220" t="s">
+      <c r="K16" s="205" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="215" t="s">
+      <c r="L16" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="202" t="s">
+      <c r="M16" s="201" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -3853,14 +3853,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="199"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="205"/>
-      <c r="K17" s="221"/>
+      <c r="J17" s="203"/>
+      <c r="K17" s="206"/>
       <c r="L17" s="209"/>
-      <c r="M17" s="204"/>
+      <c r="M17" s="199"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -3889,14 +3889,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
+      <c r="H18" s="199"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="205"/>
-      <c r="K18" s="221"/>
+      <c r="J18" s="203"/>
+      <c r="K18" s="206"/>
       <c r="L18" s="209"/>
-      <c r="M18" s="204"/>
+      <c r="M18" s="199"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -3925,14 +3925,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="203"/>
+      <c r="H19" s="200"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="206"/>
-      <c r="K19" s="222"/>
+      <c r="J19" s="204"/>
+      <c r="K19" s="207"/>
       <c r="L19" s="210"/>
-      <c r="M19" s="203"/>
+      <c r="M19" s="200"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -3962,22 +3962,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="202" t="s">
+      <c r="H20" s="201" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="213" t="s">
+      <c r="J20" s="202" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="214" t="s">
+      <c r="K20" s="211" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="215" t="s">
+      <c r="L20" s="208" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="217" t="s">
+      <c r="M20" s="214" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4008,14 +4008,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="204"/>
+      <c r="H21" s="199"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="205"/>
-      <c r="K21" s="207"/>
+      <c r="J21" s="203"/>
+      <c r="K21" s="212"/>
       <c r="L21" s="209"/>
-      <c r="M21" s="218"/>
+      <c r="M21" s="215"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4044,14 +4044,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="204"/>
+      <c r="H22" s="199"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="205"/>
-      <c r="K22" s="207"/>
+      <c r="J22" s="203"/>
+      <c r="K22" s="212"/>
       <c r="L22" s="209"/>
-      <c r="M22" s="218"/>
+      <c r="M22" s="215"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4080,14 +4080,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="203"/>
+      <c r="H23" s="200"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="206"/>
-      <c r="K23" s="208"/>
+      <c r="J23" s="204"/>
+      <c r="K23" s="213"/>
       <c r="L23" s="210"/>
-      <c r="M23" s="219"/>
+      <c r="M23" s="216"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4116,7 +4116,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="202" t="s">
+      <c r="H24" s="201" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4162,7 +4162,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="199"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4206,7 +4206,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
+      <c r="H26" s="199"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4238,7 +4238,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="203"/>
+      <c r="H27" s="200"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4270,7 +4270,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="202" t="s">
+      <c r="H28" s="201" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4289,7 +4289,7 @@
         <v>113</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.45">
@@ -4316,7 +4316,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="199"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>113</v>
       </c>
       <c r="N29" s="75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.45">
@@ -4360,7 +4360,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="199"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>113</v>
       </c>
       <c r="N30" s="75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -4404,7 +4404,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="203"/>
+      <c r="H31" s="200"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4436,7 +4436,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="199" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4483,7 +4483,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="199"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4528,7 +4528,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="203"/>
+      <c r="H34" s="200"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4585,11 +4585,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4598,25 +4612,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4628,7 +4628,7 @@
   <dimension ref="B1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4638,12 +4638,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="220" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="201"/>
+      <c r="C2" s="221"/>
+      <c r="D2" s="221"/>
+      <c r="E2" s="222"/>
       <c r="F2" s="169" t="s">
         <v>32</v>
       </c>
@@ -5087,7 +5087,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
   <dimension ref="B1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -5195,10 +5197,10 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B16" s="161" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5206,7 +5208,7 @@
         <v>121</v>
       </c>
       <c r="C17" s="165" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -5219,7 +5221,7 @@
   <dimension ref="B1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
updated pc address logic and decode unit wiring
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597569DE-90D2-47A3-BC8D-2AD328132BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E89B3E-EB16-4E20-8392-582F9E1C6952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="179">
   <si>
     <t>MODE B</t>
   </si>
@@ -535,12 +535,6 @@
     <t>Stores output to register</t>
   </si>
   <si>
-    <t>Switch output address to PC</t>
-  </si>
-  <si>
-    <t>PRE INCREMENT</t>
-  </si>
-  <si>
     <t>Returns 1 if a new value is available from UART unit, otherwise returns 0.</t>
   </si>
   <si>
@@ -557,6 +551,36 @@
   </si>
   <si>
     <t>IO_1</t>
+  </si>
+  <si>
+    <t>PRE STORE</t>
+  </si>
+  <si>
+    <t>Switch output address to OUT address</t>
+  </si>
+  <si>
+    <t>Net action</t>
+  </si>
+  <si>
+    <t>FREEZE_OP ↑, (FREEZE_WRD ↓)</t>
+  </si>
+  <si>
+    <t>HOLD ↑, PC_SOURCE_INC ↑, (FREEZE_OP ↓)</t>
+  </si>
+  <si>
+    <t>STORE ↑</t>
+  </si>
+  <si>
+    <t>FREEZE_WRD ↑, (STORE ↓)</t>
+  </si>
+  <si>
+    <t>AD_RGSET_OVERRIDE ↑, (HOLD ↓)</t>
+  </si>
+  <si>
+    <t>PC_SOURCE_INC ↓, AD_RGSET_OVERRIDE ↓</t>
+  </si>
+  <si>
+    <t>OVERRIDDEN</t>
   </si>
 </sst>
 </file>
@@ -578,7 +602,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +669,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="65">
     <border>
@@ -1446,7 +1476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="268">
+  <cellXfs count="269">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1897,6 +1927,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="63" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2068,6 +2107,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2128,79 +2230,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2557,19 +2590,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="169" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="171" t="s">
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="174" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="172"/>
-      <c r="I2" s="173"/>
-      <c r="J2" s="169" t="s">
+      <c r="H2" s="175"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="172" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2598,7 +2631,7 @@
       <c r="I3" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="170"/>
+      <c r="J3" s="173"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
@@ -3096,7 +3129,7 @@
   <dimension ref="B1:AH8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:AH3"/>
+      <selection activeCell="H3" sqref="C3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3204,73 +3237,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="183" t="s">
+      <c r="C3" s="186" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="185"/>
-      <c r="H3" s="180" t="s">
+      <c r="D3" s="187"/>
+      <c r="E3" s="187"/>
+      <c r="F3" s="187"/>
+      <c r="G3" s="188"/>
+      <c r="H3" s="183" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="181"/>
-      <c r="J3" s="182"/>
-      <c r="K3" s="180" t="s">
+      <c r="I3" s="184"/>
+      <c r="J3" s="185"/>
+      <c r="K3" s="183" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="181"/>
-      <c r="M3" s="181"/>
-      <c r="N3" s="192" t="s">
+      <c r="L3" s="184"/>
+      <c r="M3" s="184"/>
+      <c r="N3" s="195" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="193"/>
-      <c r="P3" s="194"/>
+      <c r="O3" s="196"/>
+      <c r="P3" s="197"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="186" t="s">
+      <c r="S3" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="187"/>
-      <c r="U3" s="187"/>
-      <c r="V3" s="187"/>
-      <c r="W3" s="187"/>
-      <c r="X3" s="187"/>
-      <c r="Y3" s="187"/>
-      <c r="Z3" s="188"/>
-      <c r="AA3" s="189" t="s">
+      <c r="T3" s="190"/>
+      <c r="U3" s="190"/>
+      <c r="V3" s="190"/>
+      <c r="W3" s="190"/>
+      <c r="X3" s="190"/>
+      <c r="Y3" s="190"/>
+      <c r="Z3" s="191"/>
+      <c r="AA3" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="190"/>
-      <c r="AC3" s="190"/>
-      <c r="AD3" s="190"/>
-      <c r="AE3" s="190"/>
-      <c r="AF3" s="190"/>
-      <c r="AG3" s="190"/>
-      <c r="AH3" s="191"/>
+      <c r="AB3" s="193"/>
+      <c r="AC3" s="193"/>
+      <c r="AD3" s="193"/>
+      <c r="AE3" s="193"/>
+      <c r="AF3" s="193"/>
+      <c r="AG3" s="193"/>
+      <c r="AH3" s="194"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="197" t="s">
+      <c r="B5" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="195" t="s">
+      <c r="C5" s="198" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="195"/>
-      <c r="E5" s="195"/>
-      <c r="F5" s="195"/>
-      <c r="G5" s="195"/>
-      <c r="H5" s="195"/>
-      <c r="I5" s="195"/>
-      <c r="J5" s="196"/>
+      <c r="D5" s="198"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="198"/>
+      <c r="G5" s="198"/>
+      <c r="H5" s="198"/>
+      <c r="I5" s="198"/>
+      <c r="J5" s="199"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="198"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3300,16 +3333,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="174" t="s">
+      <c r="C7" s="177" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="175"/>
-      <c r="E7" s="175"/>
-      <c r="F7" s="175"/>
-      <c r="G7" s="175"/>
-      <c r="H7" s="175"/>
-      <c r="I7" s="175"/>
-      <c r="J7" s="176"/>
+      <c r="D7" s="178"/>
+      <c r="E7" s="178"/>
+      <c r="F7" s="178"/>
+      <c r="G7" s="178"/>
+      <c r="H7" s="178"/>
+      <c r="I7" s="178"/>
+      <c r="J7" s="179"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3319,12 +3352,12 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="177" t="s">
+      <c r="G8" s="180" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="178"/>
-      <c r="I8" s="178"/>
-      <c r="J8" s="179"/>
+      <c r="H8" s="181"/>
+      <c r="I8" s="181"/>
+      <c r="J8" s="182"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3348,9 +3381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B20B11-9266-4E5E-A2B3-3496A1A10C3B}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3365,29 +3396,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="169" t="s">
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="199" t="s">
+      <c r="J2" s="202" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
-      <c r="M2" s="169" t="s">
+      <c r="K2" s="203"/>
+      <c r="L2" s="203"/>
+      <c r="M2" s="172" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="169" t="s">
+      <c r="N2" s="172" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3410,8 +3441,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
+      <c r="H3" s="173"/>
+      <c r="I3" s="173"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -3421,8 +3452,8 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="170"/>
-      <c r="N3" s="170"/>
+      <c r="M3" s="173"/>
+      <c r="N3" s="173"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -3448,7 +3479,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="205" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3494,7 +3525,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="206"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3538,25 +3569,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="207" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="205" t="s">
+      <c r="J6" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="210" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="209" t="s">
+      <c r="L6" s="212" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="217" t="s">
+      <c r="M6" s="220" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="211" t="s">
+      <c r="N6" s="214" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3584,15 +3615,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
+      <c r="H7" s="207"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="205"/>
-      <c r="K7" s="207"/>
-      <c r="L7" s="209"/>
-      <c r="M7" s="218"/>
-      <c r="N7" s="211"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="210"/>
+      <c r="L7" s="212"/>
+      <c r="M7" s="221"/>
+      <c r="N7" s="214"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3618,15 +3649,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
+      <c r="H8" s="207"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="205"/>
-      <c r="K8" s="207"/>
-      <c r="L8" s="209"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="211"/>
+      <c r="J8" s="208"/>
+      <c r="K8" s="210"/>
+      <c r="L8" s="212"/>
+      <c r="M8" s="221"/>
+      <c r="N8" s="214"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3652,15 +3683,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
+      <c r="H9" s="207"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="205"/>
-      <c r="K9" s="207"/>
-      <c r="L9" s="209"/>
-      <c r="M9" s="218"/>
-      <c r="N9" s="211"/>
+      <c r="J9" s="208"/>
+      <c r="K9" s="210"/>
+      <c r="L9" s="212"/>
+      <c r="M9" s="221"/>
+      <c r="N9" s="214"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3686,15 +3717,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="207"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="205"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="209"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="211"/>
+      <c r="J10" s="208"/>
+      <c r="K10" s="210"/>
+      <c r="L10" s="212"/>
+      <c r="M10" s="221"/>
+      <c r="N10" s="214"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3720,15 +3751,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="203"/>
+      <c r="H11" s="206"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="206"/>
-      <c r="K11" s="208"/>
-      <c r="L11" s="210"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="212"/>
+      <c r="J11" s="209"/>
+      <c r="K11" s="211"/>
+      <c r="L11" s="213"/>
+      <c r="M11" s="222"/>
+      <c r="N11" s="215"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3754,25 +3785,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="205" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="213" t="s">
+      <c r="J12" s="216" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="214" t="s">
+      <c r="K12" s="217" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="215" t="s">
+      <c r="L12" s="218" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="202" t="s">
+      <c r="M12" s="205" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="216" t="s">
+      <c r="N12" s="219" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3800,15 +3831,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="207"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="205"/>
-      <c r="K13" s="207"/>
-      <c r="L13" s="209"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="211"/>
+      <c r="J13" s="208"/>
+      <c r="K13" s="210"/>
+      <c r="L13" s="212"/>
+      <c r="M13" s="207"/>
+      <c r="N13" s="214"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3834,15 +3865,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="207"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="205"/>
-      <c r="K14" s="207"/>
-      <c r="L14" s="209"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="211"/>
+      <c r="J14" s="208"/>
+      <c r="K14" s="210"/>
+      <c r="L14" s="212"/>
+      <c r="M14" s="207"/>
+      <c r="N14" s="214"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3868,15 +3899,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="203"/>
+      <c r="H15" s="206"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="206"/>
-      <c r="K15" s="208"/>
-      <c r="L15" s="210"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="212"/>
+      <c r="J15" s="209"/>
+      <c r="K15" s="211"/>
+      <c r="L15" s="213"/>
+      <c r="M15" s="206"/>
+      <c r="N15" s="215"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3902,22 +3933,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="202" t="s">
+      <c r="H16" s="205" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="213" t="s">
+      <c r="J16" s="216" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="220" t="s">
+      <c r="K16" s="223" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="215" t="s">
+      <c r="L16" s="218" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="202" t="s">
+      <c r="M16" s="205" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -3948,14 +3979,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="207"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="205"/>
-      <c r="K17" s="221"/>
-      <c r="L17" s="209"/>
-      <c r="M17" s="204"/>
+      <c r="J17" s="208"/>
+      <c r="K17" s="224"/>
+      <c r="L17" s="212"/>
+      <c r="M17" s="207"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -3984,14 +4015,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
+      <c r="H18" s="207"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="205"/>
-      <c r="K18" s="221"/>
-      <c r="L18" s="209"/>
-      <c r="M18" s="204"/>
+      <c r="J18" s="208"/>
+      <c r="K18" s="224"/>
+      <c r="L18" s="212"/>
+      <c r="M18" s="207"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4020,14 +4051,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="203"/>
+      <c r="H19" s="206"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="206"/>
-      <c r="K19" s="222"/>
-      <c r="L19" s="210"/>
-      <c r="M19" s="203"/>
+      <c r="J19" s="209"/>
+      <c r="K19" s="225"/>
+      <c r="L19" s="213"/>
+      <c r="M19" s="206"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4057,22 +4088,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="202" t="s">
+      <c r="H20" s="205" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="213" t="s">
+      <c r="J20" s="216" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="214" t="s">
+      <c r="K20" s="217" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="215" t="s">
+      <c r="L20" s="218" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="217" t="s">
+      <c r="M20" s="220" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4103,14 +4134,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="204"/>
+      <c r="H21" s="207"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="205"/>
-      <c r="K21" s="207"/>
-      <c r="L21" s="209"/>
-      <c r="M21" s="218"/>
+      <c r="J21" s="208"/>
+      <c r="K21" s="210"/>
+      <c r="L21" s="212"/>
+      <c r="M21" s="221"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4139,14 +4170,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="204"/>
+      <c r="H22" s="207"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="205"/>
-      <c r="K22" s="207"/>
-      <c r="L22" s="209"/>
-      <c r="M22" s="218"/>
+      <c r="J22" s="208"/>
+      <c r="K22" s="210"/>
+      <c r="L22" s="212"/>
+      <c r="M22" s="221"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4175,14 +4206,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="203"/>
+      <c r="H23" s="206"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="206"/>
-      <c r="K23" s="208"/>
-      <c r="L23" s="210"/>
-      <c r="M23" s="219"/>
+      <c r="J23" s="209"/>
+      <c r="K23" s="211"/>
+      <c r="L23" s="213"/>
+      <c r="M23" s="222"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4211,7 +4242,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="202" t="s">
+      <c r="H24" s="205" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4257,7 +4288,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="207"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4301,7 +4332,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
+      <c r="H26" s="207"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4333,7 +4364,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="203"/>
+      <c r="H27" s="206"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4365,7 +4396,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="202" t="s">
+      <c r="H28" s="205" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4384,7 +4415,7 @@
         <v>113</v>
       </c>
       <c r="N28" s="39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.45">
@@ -4411,7 +4442,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="207"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4428,7 +4459,7 @@
         <v>113</v>
       </c>
       <c r="N29" s="75" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.45">
@@ -4455,7 +4486,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="207"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4472,7 +4503,7 @@
         <v>113</v>
       </c>
       <c r="N30" s="75" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -4499,7 +4530,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="203"/>
+      <c r="H31" s="206"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4531,7 +4562,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="207" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4578,7 +4609,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="207"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4623,7 +4654,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="203"/>
+      <c r="H34" s="206"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4720,7 +4751,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD788E61-AC5A-4E7F-9536-02553AF94143}">
-  <dimension ref="B1:Q35"/>
+  <dimension ref="B1:P35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4731,39 +4762,35 @@
     <col min="8" max="8" width="14.265625" style="1" customWidth="1"/>
     <col min="9" max="9" width="16.73046875" style="1" customWidth="1"/>
     <col min="10" max="12" width="20.73046875" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="90.265625" customWidth="1"/>
+    <col min="13" max="13" width="90.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+    <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B2" s="202" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="200"/>
-      <c r="F2" s="200"/>
-      <c r="G2" s="201"/>
-      <c r="H2" s="169" t="s">
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="203"/>
+      <c r="F2" s="203"/>
+      <c r="G2" s="204"/>
+      <c r="H2" s="172" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="199" t="s">
+      <c r="J2" s="202" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="200"/>
-      <c r="L2" s="200"/>
-      <c r="M2" s="169" t="s">
-        <v>112</v>
-      </c>
-      <c r="N2" s="169" t="s">
+      <c r="K2" s="203"/>
+      <c r="L2" s="203"/>
+      <c r="M2" s="172" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="85" t="s">
         <v>16</v>
       </c>
@@ -4782,8 +4809,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="170"/>
-      <c r="I3" s="170"/>
+      <c r="H3" s="173"/>
+      <c r="I3" s="173"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -4793,10 +4820,9 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="170"/>
-      <c r="N3" s="170"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="M3" s="173"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
         <v>0</v>
       </c>
@@ -4820,7 +4846,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="202" t="s">
+      <c r="H4" s="205" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4832,17 +4858,14 @@
       <c r="K4" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="267" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="70" t="s">
-        <v>113</v>
-      </c>
-      <c r="N4" s="76" t="s">
+      <c r="L4" s="268" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="76" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B5" s="83">
         <v>1</v>
       </c>
@@ -4866,7 +4889,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="203"/>
+      <c r="H5" s="206"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4879,14 +4902,11 @@
       <c r="L5" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="M5" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="N5" s="45" t="s">
+      <c r="M5" s="45" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B6" s="82">
         <v>2</v>
       </c>
@@ -4910,29 +4930,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="207" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="205" t="s">
+      <c r="J6" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="207" t="s">
+      <c r="K6" s="210" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="209" t="s">
+      <c r="L6" s="212" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="217" t="s">
-        <v>113</v>
-      </c>
-      <c r="N6" s="211" t="s">
+      <c r="M6" s="214" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B7" s="82">
         <v>3</v>
       </c>
@@ -4956,15 +4973,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="205"/>
-      <c r="K7" s="207"/>
-      <c r="L7" s="209"/>
-      <c r="M7" s="218"/>
-      <c r="N7" s="211"/>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H7" s="207"/>
+      <c r="I7" s="229"/>
+      <c r="J7" s="208"/>
+      <c r="K7" s="210"/>
+      <c r="L7" s="212"/>
+      <c r="M7" s="214"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
         <v>4</v>
       </c>
@@ -4988,15 +5004,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
-      <c r="I8" s="244"/>
-      <c r="J8" s="205"/>
-      <c r="K8" s="207"/>
-      <c r="L8" s="209"/>
-      <c r="M8" s="218"/>
-      <c r="N8" s="211"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H8" s="207"/>
+      <c r="I8" s="230"/>
+      <c r="J8" s="208"/>
+      <c r="K8" s="210"/>
+      <c r="L8" s="212"/>
+      <c r="M8" s="214"/>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
         <v>5</v>
       </c>
@@ -5020,15 +5035,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
-      <c r="I9" s="247"/>
-      <c r="J9" s="205"/>
-      <c r="K9" s="207"/>
-      <c r="L9" s="209"/>
-      <c r="M9" s="218"/>
-      <c r="N9" s="211"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H9" s="207"/>
+      <c r="I9" s="232"/>
+      <c r="J9" s="208"/>
+      <c r="K9" s="210"/>
+      <c r="L9" s="212"/>
+      <c r="M9" s="214"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
         <v>6</v>
       </c>
@@ -5052,17 +5066,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="207"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="205"/>
-      <c r="K10" s="207"/>
-      <c r="L10" s="209"/>
-      <c r="M10" s="218"/>
-      <c r="N10" s="211"/>
-    </row>
-    <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J10" s="208"/>
+      <c r="K10" s="210"/>
+      <c r="L10" s="212"/>
+      <c r="M10" s="214"/>
+    </row>
+    <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
         <v>7</v>
       </c>
@@ -5086,15 +5099,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="203"/>
+      <c r="H11" s="206"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="206"/>
-      <c r="K11" s="208"/>
-      <c r="L11" s="210"/>
-      <c r="M11" s="219"/>
-      <c r="N11" s="212"/>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J11" s="209"/>
+      <c r="K11" s="211"/>
+      <c r="L11" s="213"/>
+      <c r="M11" s="215"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
         <v>8</v>
       </c>
@@ -5118,29 +5130,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="202" t="s">
+      <c r="H12" s="205" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="213" t="s">
+      <c r="J12" s="216" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="214" t="s">
+      <c r="K12" s="217" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="215" t="s">
+      <c r="L12" s="218" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="202" t="s">
-        <v>114</v>
-      </c>
-      <c r="N12" s="216" t="s">
+      <c r="M12" s="219" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B13" s="82">
         <v>9</v>
       </c>
@@ -5164,15 +5173,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="207"/>
       <c r="I13" s="105"/>
-      <c r="J13" s="205"/>
-      <c r="K13" s="207"/>
-      <c r="L13" s="209"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="211"/>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J13" s="208"/>
+      <c r="K13" s="210"/>
+      <c r="L13" s="212"/>
+      <c r="M13" s="214"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
         <v>10</v>
       </c>
@@ -5196,15 +5204,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="207"/>
       <c r="I14" s="105"/>
-      <c r="J14" s="205"/>
-      <c r="K14" s="207"/>
-      <c r="L14" s="209"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="211"/>
-    </row>
-    <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="J14" s="208"/>
+      <c r="K14" s="210"/>
+      <c r="L14" s="212"/>
+      <c r="M14" s="214"/>
+    </row>
+    <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
         <v>11</v>
       </c>
@@ -5228,15 +5235,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="203"/>
+      <c r="H15" s="206"/>
       <c r="I15" s="105"/>
-      <c r="J15" s="206"/>
-      <c r="K15" s="208"/>
-      <c r="L15" s="210"/>
-      <c r="M15" s="203"/>
-      <c r="N15" s="212"/>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="J15" s="209"/>
+      <c r="K15" s="211"/>
+      <c r="L15" s="213"/>
+      <c r="M15" s="215"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
         <v>12</v>
       </c>
@@ -5260,29 +5266,26 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="202" t="s">
+      <c r="H16" s="205" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="213" t="s">
+      <c r="J16" s="216" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="220" t="s">
+      <c r="K16" s="223" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="215" t="s">
+      <c r="L16" s="218" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="202" t="s">
-        <v>114</v>
-      </c>
-      <c r="N16" s="76" t="s">
+      <c r="M16" s="76" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B17" s="82">
         <v>13</v>
       </c>
@@ -5306,19 +5309,18 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="207"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="205"/>
-      <c r="K17" s="221"/>
-      <c r="L17" s="209"/>
-      <c r="M17" s="204"/>
-      <c r="N17" s="75" t="s">
+      <c r="J17" s="208"/>
+      <c r="K17" s="224"/>
+      <c r="L17" s="212"/>
+      <c r="M17" s="75" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B18" s="82">
         <v>14</v>
       </c>
@@ -5342,15 +5344,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
-      <c r="I18" s="246"/>
-      <c r="J18" s="205"/>
-      <c r="K18" s="221"/>
-      <c r="L18" s="209"/>
-      <c r="M18" s="204"/>
-      <c r="N18" s="246"/>
-    </row>
-    <row r="19" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H18" s="207"/>
+      <c r="I18" s="229"/>
+      <c r="J18" s="208"/>
+      <c r="K18" s="224"/>
+      <c r="L18" s="212"/>
+      <c r="M18" s="229"/>
+    </row>
+    <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
         <v>15</v>
       </c>
@@ -5374,16 +5375,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="203"/>
-      <c r="I19" s="245"/>
-      <c r="J19" s="206"/>
-      <c r="K19" s="222"/>
-      <c r="L19" s="210"/>
-      <c r="M19" s="203"/>
-      <c r="N19" s="245"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H19" s="206"/>
+      <c r="I19" s="231"/>
+      <c r="J19" s="209"/>
+      <c r="K19" s="225"/>
+      <c r="L19" s="213"/>
+      <c r="M19" s="231"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B20" s="81">
         <v>16</v>
       </c>
@@ -5407,15 +5407,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="243"/>
-      <c r="I20" s="244"/>
-      <c r="J20" s="263"/>
-      <c r="K20" s="264"/>
-      <c r="L20" s="261"/>
-      <c r="M20" s="246"/>
-      <c r="N20" s="244"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H20" s="233"/>
+      <c r="I20" s="230"/>
+      <c r="J20" s="234"/>
+      <c r="K20" s="237"/>
+      <c r="L20" s="226"/>
+      <c r="M20" s="230"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B21" s="82">
         <v>17</v>
       </c>
@@ -5439,15 +5438,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="244"/>
-      <c r="I21" s="244"/>
-      <c r="J21" s="259"/>
-      <c r="K21" s="265"/>
-      <c r="L21" s="262"/>
-      <c r="M21" s="244"/>
-      <c r="N21" s="244"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H21" s="230"/>
+      <c r="I21" s="230"/>
+      <c r="J21" s="235"/>
+      <c r="K21" s="238"/>
+      <c r="L21" s="227"/>
+      <c r="M21" s="230"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
         <v>18</v>
       </c>
@@ -5471,15 +5469,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="244"/>
-      <c r="I22" s="244"/>
-      <c r="J22" s="259"/>
-      <c r="K22" s="265"/>
-      <c r="L22" s="262"/>
-      <c r="M22" s="244"/>
-      <c r="N22" s="244"/>
-    </row>
-    <row r="23" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H22" s="230"/>
+      <c r="I22" s="230"/>
+      <c r="J22" s="235"/>
+      <c r="K22" s="238"/>
+      <c r="L22" s="227"/>
+      <c r="M22" s="230"/>
+    </row>
+    <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
         <v>19</v>
       </c>
@@ -5503,15 +5500,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="245"/>
-      <c r="I23" s="245"/>
-      <c r="J23" s="260"/>
-      <c r="K23" s="266"/>
-      <c r="L23" s="253"/>
-      <c r="M23" s="245"/>
-      <c r="N23" s="245"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H23" s="231"/>
+      <c r="I23" s="231"/>
+      <c r="J23" s="236"/>
+      <c r="K23" s="239"/>
+      <c r="L23" s="228"/>
+      <c r="M23" s="231"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
         <v>20</v>
       </c>
@@ -5535,7 +5531,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="202" t="s">
+      <c r="H24" s="205" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5550,14 +5546,11 @@
       <c r="L24" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="M24" s="103" t="s">
-        <v>113</v>
-      </c>
-      <c r="N24" s="76" t="s">
+      <c r="M24" s="76" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B25" s="82">
         <v>21</v>
       </c>
@@ -5581,7 +5574,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="207"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5594,14 +5587,11 @@
       <c r="L25" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="M25" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="N25" s="75" t="s">
+      <c r="M25" s="75" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B26" s="82">
         <v>22</v>
       </c>
@@ -5625,15 +5615,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
-      <c r="I26" s="246"/>
-      <c r="J26" s="248"/>
-      <c r="K26" s="250"/>
-      <c r="L26" s="252"/>
-      <c r="M26" s="254"/>
-      <c r="N26" s="254"/>
-    </row>
-    <row r="27" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="H26" s="207"/>
+      <c r="I26" s="229"/>
+      <c r="J26" s="240"/>
+      <c r="K26" s="242"/>
+      <c r="L26" s="244"/>
+      <c r="M26" s="245"/>
+    </row>
+    <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
         <v>23</v>
       </c>
@@ -5657,15 +5646,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="203"/>
-      <c r="I27" s="245"/>
-      <c r="J27" s="249"/>
-      <c r="K27" s="251"/>
-      <c r="L27" s="253"/>
-      <c r="M27" s="255"/>
-      <c r="N27" s="255"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="H27" s="206"/>
+      <c r="I27" s="231"/>
+      <c r="J27" s="241"/>
+      <c r="K27" s="243"/>
+      <c r="L27" s="228"/>
+      <c r="M27" s="246"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
         <v>24</v>
       </c>
@@ -5689,8 +5677,8 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="202" t="s">
-        <v>169</v>
+      <c r="H28" s="205" t="s">
+        <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
         <v>51</v>
@@ -5704,14 +5692,11 @@
       <c r="L28" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="M28" s="99" t="s">
-        <v>113</v>
-      </c>
-      <c r="N28" s="39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="M28" s="39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B29" s="82">
         <v>25</v>
       </c>
@@ -5735,7 +5720,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="207"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5748,14 +5733,11 @@
       <c r="L29" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="M29" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="N29" s="75" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="M29" s="75" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B30" s="82">
         <v>26</v>
       </c>
@@ -5779,7 +5761,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="207"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5792,14 +5774,11 @@
       <c r="L30" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="M30" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="N30" s="75" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M30" s="75" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B31" s="83">
         <v>27</v>
       </c>
@@ -5823,15 +5802,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="203"/>
+      <c r="H31" s="206"/>
       <c r="I31" s="92"/>
-      <c r="J31" s="256"/>
-      <c r="K31" s="257"/>
-      <c r="L31" s="258"/>
-      <c r="M31" s="97"/>
-      <c r="N31" s="94"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="J31" s="166"/>
+      <c r="K31" s="167"/>
+      <c r="L31" s="168"/>
+      <c r="M31" s="94"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B32" s="82">
         <v>28</v>
       </c>
@@ -5855,8 +5833,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
-        <v>170</v>
+      <c r="H32" s="207" t="s">
+        <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
         <v>51</v>
@@ -5870,15 +5848,12 @@
       <c r="L32" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="M32" s="99" t="s">
-        <v>113</v>
-      </c>
-      <c r="N32" s="39" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.45">
+      <c r="M32" s="39" t="s">
+        <v>163</v>
+      </c>
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B33" s="82">
         <v>29</v>
       </c>
@@ -5902,7 +5877,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="207"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5915,15 +5890,12 @@
       <c r="L33" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="M33" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="N33" s="75" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M33" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B34" s="82">
         <v>30</v>
       </c>
@@ -5947,7 +5919,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="203"/>
+      <c r="H34" s="206"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -5960,15 +5932,12 @@
       <c r="L34" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="M34" s="100" t="s">
-        <v>113</v>
-      </c>
-      <c r="N34" s="75" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="2:17" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="M34" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B35" s="84">
         <v>31</v>
       </c>
@@ -6004,61 +5973,52 @@
       <c r="K35" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="M35" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="N35" s="47" t="s">
+      <c r="L35" s="267" t="s">
+        <v>178</v>
+      </c>
+      <c r="M35" s="47" t="s">
         <v>111</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="43">
+  <mergeCells count="37">
     <mergeCell ref="J26:J27"/>
     <mergeCell ref="K26:K27"/>
     <mergeCell ref="L26:L27"/>
     <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="H28:H31"/>
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
-    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="M18:M19"/>
     <mergeCell ref="I20:I23"/>
-    <mergeCell ref="N20:N23"/>
+    <mergeCell ref="M20:M23"/>
     <mergeCell ref="I26:I27"/>
     <mergeCell ref="H16:H19"/>
     <mergeCell ref="J16:J19"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="J20:J23"/>
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
     <mergeCell ref="K12:K15"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H11"/>
     <mergeCell ref="J6:J11"/>
     <mergeCell ref="K6:K11"/>
     <mergeCell ref="L6:L11"/>
-    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6069,9 +6029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4182B34D-1176-43D9-83DE-D8E7EA5C96ED}">
   <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6080,13 +6038,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="199" t="s">
+      <c r="B2" s="202" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="200"/>
-      <c r="D2" s="200"/>
-      <c r="E2" s="201"/>
-      <c r="F2" s="169" t="s">
+      <c r="C2" s="203"/>
+      <c r="D2" s="203"/>
+      <c r="E2" s="204"/>
+      <c r="F2" s="172" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6103,7 +6061,7 @@
       <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="170"/>
+      <c r="F3" s="173"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
@@ -6289,30 +6247,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="172" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="232" t="s">
+      <c r="C2" s="256" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="233"/>
-      <c r="E2" s="233"/>
-      <c r="F2" s="233"/>
-      <c r="G2" s="233"/>
-      <c r="H2" s="233"/>
-      <c r="I2" s="233"/>
-      <c r="J2" s="233"/>
-      <c r="K2" s="233"/>
-      <c r="L2" s="233"/>
-      <c r="M2" s="233"/>
-      <c r="N2" s="233"/>
-      <c r="O2" s="233"/>
-      <c r="P2" s="233"/>
-      <c r="Q2" s="233"/>
-      <c r="R2" s="234"/>
+      <c r="D2" s="257"/>
+      <c r="E2" s="257"/>
+      <c r="F2" s="257"/>
+      <c r="G2" s="257"/>
+      <c r="H2" s="257"/>
+      <c r="I2" s="257"/>
+      <c r="J2" s="257"/>
+      <c r="K2" s="257"/>
+      <c r="L2" s="257"/>
+      <c r="M2" s="257"/>
+      <c r="N2" s="257"/>
+      <c r="O2" s="257"/>
+      <c r="P2" s="257"/>
+      <c r="Q2" s="257"/>
+      <c r="R2" s="258"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="170"/>
+      <c r="B3" s="173"/>
       <c r="C3" s="118">
         <v>15</v>
       </c>
@@ -6383,13 +6341,13 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="226" t="s">
+      <c r="N4" s="250" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="226"/>
-      <c r="P4" s="226"/>
-      <c r="Q4" s="226"/>
-      <c r="R4" s="227"/>
+      <c r="O4" s="250"/>
+      <c r="P4" s="250"/>
+      <c r="Q4" s="250"/>
+      <c r="R4" s="251"/>
     </row>
     <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
@@ -6403,16 +6361,16 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="228" t="s">
+      <c r="K5" s="252" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="224"/>
-      <c r="M5" s="224"/>
-      <c r="N5" s="224"/>
-      <c r="O5" s="224"/>
-      <c r="P5" s="224"/>
-      <c r="Q5" s="224"/>
-      <c r="R5" s="225"/>
+      <c r="L5" s="248"/>
+      <c r="M5" s="248"/>
+      <c r="N5" s="248"/>
+      <c r="O5" s="248"/>
+      <c r="P5" s="248"/>
+      <c r="Q5" s="248"/>
+      <c r="R5" s="249"/>
     </row>
     <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
@@ -6426,16 +6384,16 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="228" t="s">
+      <c r="K6" s="252" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="224"/>
-      <c r="M6" s="224"/>
-      <c r="N6" s="224"/>
-      <c r="O6" s="224"/>
-      <c r="P6" s="224"/>
-      <c r="Q6" s="224"/>
-      <c r="R6" s="225"/>
+      <c r="L6" s="248"/>
+      <c r="M6" s="248"/>
+      <c r="N6" s="248"/>
+      <c r="O6" s="248"/>
+      <c r="P6" s="248"/>
+      <c r="Q6" s="248"/>
+      <c r="R6" s="249"/>
     </row>
     <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
@@ -6449,39 +6407,39 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="229" t="s">
+      <c r="K7" s="253" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="230"/>
-      <c r="M7" s="230"/>
-      <c r="N7" s="230"/>
-      <c r="O7" s="230"/>
-      <c r="P7" s="230"/>
-      <c r="Q7" s="230"/>
-      <c r="R7" s="231"/>
+      <c r="L7" s="254"/>
+      <c r="M7" s="254"/>
+      <c r="N7" s="254"/>
+      <c r="O7" s="254"/>
+      <c r="P7" s="254"/>
+      <c r="Q7" s="254"/>
+      <c r="R7" s="255"/>
     </row>
     <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="223" t="s">
+      <c r="C8" s="247" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="224"/>
-      <c r="E8" s="224"/>
-      <c r="F8" s="224"/>
-      <c r="G8" s="224"/>
-      <c r="H8" s="224"/>
-      <c r="I8" s="224"/>
-      <c r="J8" s="224"/>
-      <c r="K8" s="224"/>
-      <c r="L8" s="224"/>
-      <c r="M8" s="224"/>
-      <c r="N8" s="224"/>
-      <c r="O8" s="224"/>
-      <c r="P8" s="224"/>
-      <c r="Q8" s="224"/>
-      <c r="R8" s="225"/>
+      <c r="D8" s="248"/>
+      <c r="E8" s="248"/>
+      <c r="F8" s="248"/>
+      <c r="G8" s="248"/>
+      <c r="H8" s="248"/>
+      <c r="I8" s="248"/>
+      <c r="J8" s="248"/>
+      <c r="K8" s="248"/>
+      <c r="L8" s="248"/>
+      <c r="M8" s="248"/>
+      <c r="N8" s="248"/>
+      <c r="O8" s="248"/>
+      <c r="P8" s="248"/>
+      <c r="Q8" s="248"/>
+      <c r="R8" s="249"/>
     </row>
     <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
@@ -6527,20 +6485,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
-  <dimension ref="B1:C17"/>
+  <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="21.1328125" customWidth="1"/>
-    <col min="3" max="3" width="85.73046875" customWidth="1"/>
+    <col min="3" max="3" width="82.265625" customWidth="1"/>
+    <col min="4" max="4" width="43.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="2:3" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="2:4" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B2" s="160" t="s">
         <v>152</v>
       </c>
@@ -6548,7 +6505,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B3" s="161" t="s">
         <v>118</v>
       </c>
@@ -6556,7 +6513,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" s="163" t="s">
         <v>119</v>
       </c>
@@ -6564,7 +6521,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="161" t="s">
         <v>125</v>
       </c>
@@ -6572,7 +6529,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="163" t="s">
         <v>120</v>
       </c>
@@ -6580,7 +6537,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="161" t="s">
         <v>121</v>
       </c>
@@ -6588,7 +6545,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="164" t="s">
         <v>46</v>
       </c>
@@ -6596,61 +6553,82 @@
         <v>155</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="11" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="160" t="s">
         <v>152</v>
       </c>
       <c r="C11" s="162" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D11" s="162" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="163" t="s">
         <v>156</v>
       </c>
       <c r="C12" s="75" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D12" s="75" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="161" t="s">
         <v>158</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D13" s="42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="163" t="s">
         <v>160</v>
       </c>
       <c r="C14" s="75" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="D14" s="75" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" s="163" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="75" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B16" s="161" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="164" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C17" s="165" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B16" s="161" t="s">
-        <v>164</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C17" s="165" t="s">
-        <v>168</v>
+      <c r="D17" s="165" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -6673,10 +6651,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="235" t="s">
+      <c r="B2" s="259" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="236"/>
+      <c r="C2" s="260"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6693,7 +6671,7 @@
       <c r="C4" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="237" t="s">
+      <c r="D4" s="261" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6702,21 +6680,21 @@
       <c r="C5" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="238"/>
+      <c r="D5" s="262"/>
     </row>
     <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="239"/>
+      <c r="D6" s="263"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="145"/>
-      <c r="D7" s="240" t="s">
+      <c r="D7" s="264" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6725,14 +6703,14 @@
         <v>142</v>
       </c>
       <c r="C8" s="146"/>
-      <c r="D8" s="241"/>
+      <c r="D8" s="265"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
       <c r="C9" s="146"/>
-      <c r="D9" s="241"/>
+      <c r="D9" s="265"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
@@ -6741,7 +6719,7 @@
       <c r="C10" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="241"/>
+      <c r="D10" s="265"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
@@ -6750,7 +6728,7 @@
       <c r="C11" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="241"/>
+      <c r="D11" s="265"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6760,7 +6738,7 @@
       <c r="C12" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="242"/>
+      <c r="D12" s="266"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added hold unit, updated mem unit wiring
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E89B3E-EB16-4E20-8392-582F9E1C6952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF10C2F4-314D-429A-933A-D49AE7C6B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -1936,6 +1936,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1960,6 +1966,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1996,44 +2041,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2044,124 +2113,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2170,6 +2137,45 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2229,12 +2235,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2590,19 +2590,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="171"/>
-      <c r="G2" s="174" t="s">
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="172"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="176" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="175"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="172" t="s">
+      <c r="H2" s="177"/>
+      <c r="I2" s="178"/>
+      <c r="J2" s="174" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2631,7 +2631,7 @@
       <c r="I3" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="173"/>
+      <c r="J3" s="175"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
@@ -3237,73 +3237,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="186" t="s">
+      <c r="C3" s="201" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="187"/>
-      <c r="E3" s="187"/>
-      <c r="F3" s="187"/>
-      <c r="G3" s="188"/>
-      <c r="H3" s="183" t="s">
+      <c r="D3" s="202"/>
+      <c r="E3" s="202"/>
+      <c r="F3" s="202"/>
+      <c r="G3" s="203"/>
+      <c r="H3" s="198" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="184"/>
-      <c r="J3" s="185"/>
-      <c r="K3" s="183" t="s">
+      <c r="I3" s="199"/>
+      <c r="J3" s="200"/>
+      <c r="K3" s="198" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="184"/>
-      <c r="M3" s="184"/>
-      <c r="N3" s="195" t="s">
+      <c r="L3" s="199"/>
+      <c r="M3" s="199"/>
+      <c r="N3" s="185" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="196"/>
-      <c r="P3" s="197"/>
+      <c r="O3" s="186"/>
+      <c r="P3" s="187"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="189" t="s">
+      <c r="S3" s="179" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="190"/>
-      <c r="U3" s="190"/>
-      <c r="V3" s="190"/>
-      <c r="W3" s="190"/>
-      <c r="X3" s="190"/>
-      <c r="Y3" s="190"/>
-      <c r="Z3" s="191"/>
-      <c r="AA3" s="192" t="s">
+      <c r="T3" s="180"/>
+      <c r="U3" s="180"/>
+      <c r="V3" s="180"/>
+      <c r="W3" s="180"/>
+      <c r="X3" s="180"/>
+      <c r="Y3" s="180"/>
+      <c r="Z3" s="181"/>
+      <c r="AA3" s="182" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="193"/>
-      <c r="AC3" s="193"/>
-      <c r="AD3" s="193"/>
-      <c r="AE3" s="193"/>
-      <c r="AF3" s="193"/>
-      <c r="AG3" s="193"/>
-      <c r="AH3" s="194"/>
+      <c r="AB3" s="183"/>
+      <c r="AC3" s="183"/>
+      <c r="AD3" s="183"/>
+      <c r="AE3" s="183"/>
+      <c r="AF3" s="183"/>
+      <c r="AG3" s="183"/>
+      <c r="AH3" s="184"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="200" t="s">
+      <c r="B5" s="190" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="198" t="s">
+      <c r="C5" s="188" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="198"/>
-      <c r="E5" s="198"/>
-      <c r="F5" s="198"/>
-      <c r="G5" s="198"/>
-      <c r="H5" s="198"/>
-      <c r="I5" s="198"/>
-      <c r="J5" s="199"/>
+      <c r="D5" s="188"/>
+      <c r="E5" s="188"/>
+      <c r="F5" s="188"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="188"/>
+      <c r="I5" s="188"/>
+      <c r="J5" s="189"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="201"/>
+      <c r="B6" s="191"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3333,16 +3333,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="177" t="s">
+      <c r="C7" s="192" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="178"/>
-      <c r="E7" s="178"/>
-      <c r="F7" s="178"/>
-      <c r="G7" s="178"/>
-      <c r="H7" s="178"/>
-      <c r="I7" s="178"/>
-      <c r="J7" s="179"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="194"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3352,25 +3352,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="180" t="s">
+      <c r="G8" s="195" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="182"/>
+      <c r="H8" s="196"/>
+      <c r="I8" s="196"/>
+      <c r="J8" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3396,29 +3396,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="225" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="172" t="s">
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="174" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="172" t="s">
+      <c r="I2" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="202" t="s">
+      <c r="J2" s="225" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="203"/>
-      <c r="L2" s="203"/>
-      <c r="M2" s="172" t="s">
+      <c r="K2" s="226"/>
+      <c r="L2" s="226"/>
+      <c r="M2" s="174" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="172" t="s">
+      <c r="N2" s="174" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3441,8 +3441,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -3452,8 +3452,8 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="173"/>
-      <c r="N3" s="173"/>
+      <c r="M3" s="175"/>
+      <c r="N3" s="175"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -3479,7 +3479,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="205" t="s">
+      <c r="H4" s="206" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3525,7 +3525,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="206"/>
+      <c r="H5" s="205"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3569,7 +3569,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="207" t="s">
+      <c r="H6" s="204" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
@@ -3578,16 +3578,16 @@
       <c r="J6" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="210" t="s">
+      <c r="K6" s="217" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="212" t="s">
+      <c r="L6" s="214" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="220" t="s">
+      <c r="M6" s="219" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="214" t="s">
+      <c r="N6" s="222" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3615,15 +3615,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="207"/>
+      <c r="H7" s="204"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
       <c r="J7" s="208"/>
-      <c r="K7" s="210"/>
-      <c r="L7" s="212"/>
-      <c r="M7" s="221"/>
-      <c r="N7" s="214"/>
+      <c r="K7" s="217"/>
+      <c r="L7" s="214"/>
+      <c r="M7" s="220"/>
+      <c r="N7" s="222"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3649,15 +3649,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="207"/>
+      <c r="H8" s="204"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="208"/>
-      <c r="K8" s="210"/>
-      <c r="L8" s="212"/>
-      <c r="M8" s="221"/>
-      <c r="N8" s="214"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="214"/>
+      <c r="M8" s="220"/>
+      <c r="N8" s="222"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3683,15 +3683,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="207"/>
+      <c r="H9" s="204"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
       <c r="J9" s="208"/>
-      <c r="K9" s="210"/>
-      <c r="L9" s="212"/>
-      <c r="M9" s="221"/>
-      <c r="N9" s="214"/>
+      <c r="K9" s="217"/>
+      <c r="L9" s="214"/>
+      <c r="M9" s="220"/>
+      <c r="N9" s="222"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3717,15 +3717,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="207"/>
+      <c r="H10" s="204"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="208"/>
-      <c r="K10" s="210"/>
-      <c r="L10" s="212"/>
-      <c r="M10" s="221"/>
-      <c r="N10" s="214"/>
+      <c r="K10" s="217"/>
+      <c r="L10" s="214"/>
+      <c r="M10" s="220"/>
+      <c r="N10" s="222"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3751,15 +3751,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="206"/>
+      <c r="H11" s="205"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="209"/>
-      <c r="K11" s="211"/>
-      <c r="L11" s="213"/>
-      <c r="M11" s="222"/>
-      <c r="N11" s="215"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="215"/>
+      <c r="M11" s="221"/>
+      <c r="N11" s="223"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3785,25 +3785,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="205" t="s">
+      <c r="H12" s="206" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="216" t="s">
+      <c r="J12" s="207" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="217" t="s">
+      <c r="K12" s="216" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="218" t="s">
+      <c r="L12" s="213" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="205" t="s">
+      <c r="M12" s="206" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="219" t="s">
+      <c r="N12" s="224" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3831,15 +3831,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="207"/>
+      <c r="H13" s="204"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
       <c r="J13" s="208"/>
-      <c r="K13" s="210"/>
-      <c r="L13" s="212"/>
-      <c r="M13" s="207"/>
-      <c r="N13" s="214"/>
+      <c r="K13" s="217"/>
+      <c r="L13" s="214"/>
+      <c r="M13" s="204"/>
+      <c r="N13" s="222"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3865,15 +3865,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="207"/>
+      <c r="H14" s="204"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
       <c r="J14" s="208"/>
-      <c r="K14" s="210"/>
-      <c r="L14" s="212"/>
-      <c r="M14" s="207"/>
-      <c r="N14" s="214"/>
+      <c r="K14" s="217"/>
+      <c r="L14" s="214"/>
+      <c r="M14" s="204"/>
+      <c r="N14" s="222"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3899,15 +3899,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="206"/>
+      <c r="H15" s="205"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
       <c r="J15" s="209"/>
-      <c r="K15" s="211"/>
-      <c r="L15" s="213"/>
-      <c r="M15" s="206"/>
-      <c r="N15" s="215"/>
+      <c r="K15" s="218"/>
+      <c r="L15" s="215"/>
+      <c r="M15" s="205"/>
+      <c r="N15" s="223"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3933,22 +3933,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="205" t="s">
+      <c r="H16" s="206" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="216" t="s">
+      <c r="J16" s="207" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="223" t="s">
+      <c r="K16" s="210" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="218" t="s">
+      <c r="L16" s="213" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="205" t="s">
+      <c r="M16" s="206" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -3979,14 +3979,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="207"/>
+      <c r="H17" s="204"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
       <c r="J17" s="208"/>
-      <c r="K17" s="224"/>
-      <c r="L17" s="212"/>
-      <c r="M17" s="207"/>
+      <c r="K17" s="211"/>
+      <c r="L17" s="214"/>
+      <c r="M17" s="204"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4015,14 +4015,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="207"/>
+      <c r="H18" s="204"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
       <c r="J18" s="208"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="212"/>
-      <c r="M18" s="207"/>
+      <c r="K18" s="211"/>
+      <c r="L18" s="214"/>
+      <c r="M18" s="204"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4051,14 +4051,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="206"/>
+      <c r="H19" s="205"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
       <c r="J19" s="209"/>
-      <c r="K19" s="225"/>
-      <c r="L19" s="213"/>
-      <c r="M19" s="206"/>
+      <c r="K19" s="212"/>
+      <c r="L19" s="215"/>
+      <c r="M19" s="205"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4088,22 +4088,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="205" t="s">
+      <c r="H20" s="206" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="216" t="s">
+      <c r="J20" s="207" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="217" t="s">
+      <c r="K20" s="216" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="218" t="s">
+      <c r="L20" s="213" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="220" t="s">
+      <c r="M20" s="219" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4134,14 +4134,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="207"/>
+      <c r="H21" s="204"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
       <c r="J21" s="208"/>
-      <c r="K21" s="210"/>
-      <c r="L21" s="212"/>
-      <c r="M21" s="221"/>
+      <c r="K21" s="217"/>
+      <c r="L21" s="214"/>
+      <c r="M21" s="220"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4170,14 +4170,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="207"/>
+      <c r="H22" s="204"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
       <c r="J22" s="208"/>
-      <c r="K22" s="210"/>
-      <c r="L22" s="212"/>
-      <c r="M22" s="221"/>
+      <c r="K22" s="217"/>
+      <c r="L22" s="214"/>
+      <c r="M22" s="220"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4206,14 +4206,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="206"/>
+      <c r="H23" s="205"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
       <c r="J23" s="209"/>
-      <c r="K23" s="211"/>
-      <c r="L23" s="213"/>
-      <c r="M23" s="222"/>
+      <c r="K23" s="218"/>
+      <c r="L23" s="215"/>
+      <c r="M23" s="221"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4242,7 +4242,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="205" t="s">
+      <c r="H24" s="206" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4288,7 +4288,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="207"/>
+      <c r="H25" s="204"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4332,7 +4332,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="207"/>
+      <c r="H26" s="204"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4364,7 +4364,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="206"/>
+      <c r="H27" s="205"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4396,7 +4396,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="205" t="s">
+      <c r="H28" s="206" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4442,7 +4442,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="207"/>
+      <c r="H29" s="204"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4486,7 +4486,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="207"/>
+      <c r="H30" s="204"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4530,7 +4530,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="206"/>
+      <c r="H31" s="205"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4562,7 +4562,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="207" t="s">
+      <c r="H32" s="204" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4609,7 +4609,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="207"/>
+      <c r="H33" s="204"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4654,7 +4654,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="206"/>
+      <c r="H34" s="205"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4711,11 +4711,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4724,25 +4738,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4767,26 +4767,26 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="225" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="203"/>
-      <c r="F2" s="203"/>
-      <c r="G2" s="204"/>
-      <c r="H2" s="172" t="s">
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="226"/>
+      <c r="F2" s="226"/>
+      <c r="G2" s="227"/>
+      <c r="H2" s="174" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="172" t="s">
+      <c r="I2" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="202" t="s">
+      <c r="J2" s="225" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="203"/>
-      <c r="L2" s="203"/>
-      <c r="M2" s="172" t="s">
+      <c r="K2" s="226"/>
+      <c r="L2" s="226"/>
+      <c r="M2" s="174" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4809,8 +4809,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="173"/>
-      <c r="I3" s="173"/>
+      <c r="H3" s="175"/>
+      <c r="I3" s="175"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -4820,7 +4820,7 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="173"/>
+      <c r="M3" s="175"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -4846,7 +4846,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="205" t="s">
+      <c r="H4" s="206" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4858,7 +4858,7 @@
       <c r="K4" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="268" t="s">
+      <c r="L4" s="170" t="s">
         <v>3</v>
       </c>
       <c r="M4" s="76" t="s">
@@ -4889,7 +4889,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="206"/>
+      <c r="H5" s="205"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="M5" s="45" t="s">
         <v>117</v>
@@ -4930,7 +4930,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="207" t="s">
+      <c r="H6" s="204" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
@@ -4939,13 +4939,13 @@
       <c r="J6" s="208" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="210" t="s">
+      <c r="K6" s="217" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="212" t="s">
+      <c r="L6" s="214" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="214" t="s">
+      <c r="M6" s="222" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4973,12 +4973,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="207"/>
-      <c r="I7" s="229"/>
+      <c r="H7" s="204"/>
+      <c r="I7" s="236"/>
       <c r="J7" s="208"/>
-      <c r="K7" s="210"/>
-      <c r="L7" s="212"/>
-      <c r="M7" s="214"/>
+      <c r="K7" s="217"/>
+      <c r="L7" s="214"/>
+      <c r="M7" s="222"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5004,12 +5004,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="207"/>
-      <c r="I8" s="230"/>
+      <c r="H8" s="204"/>
+      <c r="I8" s="238"/>
       <c r="J8" s="208"/>
-      <c r="K8" s="210"/>
-      <c r="L8" s="212"/>
-      <c r="M8" s="214"/>
+      <c r="K8" s="217"/>
+      <c r="L8" s="214"/>
+      <c r="M8" s="222"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5035,12 +5035,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="207"/>
-      <c r="I9" s="232"/>
+      <c r="H9" s="204"/>
+      <c r="I9" s="248"/>
       <c r="J9" s="208"/>
-      <c r="K9" s="210"/>
-      <c r="L9" s="212"/>
-      <c r="M9" s="214"/>
+      <c r="K9" s="217"/>
+      <c r="L9" s="214"/>
+      <c r="M9" s="222"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5066,14 +5066,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="207"/>
+      <c r="H10" s="204"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="208"/>
-      <c r="K10" s="210"/>
-      <c r="L10" s="212"/>
-      <c r="M10" s="214"/>
+      <c r="K10" s="217"/>
+      <c r="L10" s="214"/>
+      <c r="M10" s="222"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5099,12 +5099,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="206"/>
+      <c r="H11" s="205"/>
       <c r="I11" s="105"/>
       <c r="J11" s="209"/>
-      <c r="K11" s="211"/>
-      <c r="L11" s="213"/>
-      <c r="M11" s="215"/>
+      <c r="K11" s="218"/>
+      <c r="L11" s="215"/>
+      <c r="M11" s="223"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5130,22 +5130,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="205" t="s">
+      <c r="H12" s="206" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="216" t="s">
+      <c r="J12" s="207" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="217" t="s">
+      <c r="K12" s="216" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="218" t="s">
+      <c r="L12" s="213" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="219" t="s">
+      <c r="M12" s="224" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5173,12 +5173,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="207"/>
+      <c r="H13" s="204"/>
       <c r="I13" s="105"/>
       <c r="J13" s="208"/>
-      <c r="K13" s="210"/>
-      <c r="L13" s="212"/>
-      <c r="M13" s="214"/>
+      <c r="K13" s="217"/>
+      <c r="L13" s="214"/>
+      <c r="M13" s="222"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5204,12 +5204,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="207"/>
+      <c r="H14" s="204"/>
       <c r="I14" s="105"/>
       <c r="J14" s="208"/>
-      <c r="K14" s="210"/>
-      <c r="L14" s="212"/>
-      <c r="M14" s="214"/>
+      <c r="K14" s="217"/>
+      <c r="L14" s="214"/>
+      <c r="M14" s="222"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5235,12 +5235,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="206"/>
+      <c r="H15" s="205"/>
       <c r="I15" s="105"/>
       <c r="J15" s="209"/>
-      <c r="K15" s="211"/>
-      <c r="L15" s="213"/>
-      <c r="M15" s="215"/>
+      <c r="K15" s="218"/>
+      <c r="L15" s="215"/>
+      <c r="M15" s="223"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5266,19 +5266,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="205" t="s">
+      <c r="H16" s="206" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="216" t="s">
+      <c r="J16" s="207" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="223" t="s">
+      <c r="K16" s="210" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="218" t="s">
+      <c r="L16" s="213" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5309,13 +5309,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="207"/>
+      <c r="H17" s="204"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
       <c r="J17" s="208"/>
-      <c r="K17" s="224"/>
-      <c r="L17" s="212"/>
+      <c r="K17" s="211"/>
+      <c r="L17" s="214"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
       </c>
@@ -5344,12 +5344,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="207"/>
-      <c r="I18" s="229"/>
+      <c r="H18" s="204"/>
+      <c r="I18" s="236"/>
       <c r="J18" s="208"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="212"/>
-      <c r="M18" s="229"/>
+      <c r="K18" s="211"/>
+      <c r="L18" s="214"/>
+      <c r="M18" s="236"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5375,12 +5375,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="206"/>
-      <c r="I19" s="231"/>
+      <c r="H19" s="205"/>
+      <c r="I19" s="237"/>
       <c r="J19" s="209"/>
-      <c r="K19" s="225"/>
-      <c r="L19" s="213"/>
-      <c r="M19" s="231"/>
+      <c r="K19" s="212"/>
+      <c r="L19" s="215"/>
+      <c r="M19" s="237"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5407,12 +5407,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="233"/>
-      <c r="I20" s="230"/>
-      <c r="J20" s="234"/>
-      <c r="K20" s="237"/>
-      <c r="L20" s="226"/>
-      <c r="M20" s="230"/>
+      <c r="H20" s="239"/>
+      <c r="I20" s="238"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="243"/>
+      <c r="L20" s="246"/>
+      <c r="M20" s="238"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B21" s="82">
@@ -5438,12 +5438,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="230"/>
-      <c r="I21" s="230"/>
-      <c r="J21" s="235"/>
-      <c r="K21" s="238"/>
-      <c r="L21" s="227"/>
-      <c r="M21" s="230"/>
+      <c r="H21" s="238"/>
+      <c r="I21" s="238"/>
+      <c r="J21" s="241"/>
+      <c r="K21" s="244"/>
+      <c r="L21" s="247"/>
+      <c r="M21" s="238"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
@@ -5469,12 +5469,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="230"/>
-      <c r="I22" s="230"/>
-      <c r="J22" s="235"/>
-      <c r="K22" s="238"/>
-      <c r="L22" s="227"/>
-      <c r="M22" s="230"/>
+      <c r="H22" s="238"/>
+      <c r="I22" s="238"/>
+      <c r="J22" s="241"/>
+      <c r="K22" s="244"/>
+      <c r="L22" s="247"/>
+      <c r="M22" s="238"/>
     </row>
     <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
@@ -5500,12 +5500,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="231"/>
-      <c r="I23" s="231"/>
-      <c r="J23" s="236"/>
-      <c r="K23" s="239"/>
-      <c r="L23" s="228"/>
-      <c r="M23" s="231"/>
+      <c r="H23" s="237"/>
+      <c r="I23" s="237"/>
+      <c r="J23" s="242"/>
+      <c r="K23" s="245"/>
+      <c r="L23" s="233"/>
+      <c r="M23" s="237"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
@@ -5531,7 +5531,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="205" t="s">
+      <c r="H24" s="206" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5574,7 +5574,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="207"/>
+      <c r="H25" s="204"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5615,12 +5615,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="207"/>
-      <c r="I26" s="229"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="242"/>
-      <c r="L26" s="244"/>
-      <c r="M26" s="245"/>
+      <c r="H26" s="204"/>
+      <c r="I26" s="236"/>
+      <c r="J26" s="228"/>
+      <c r="K26" s="230"/>
+      <c r="L26" s="232"/>
+      <c r="M26" s="234"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5646,12 +5646,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="206"/>
-      <c r="I27" s="231"/>
-      <c r="J27" s="241"/>
-      <c r="K27" s="243"/>
-      <c r="L27" s="228"/>
-      <c r="M27" s="246"/>
+      <c r="H27" s="205"/>
+      <c r="I27" s="237"/>
+      <c r="J27" s="229"/>
+      <c r="K27" s="231"/>
+      <c r="L27" s="233"/>
+      <c r="M27" s="235"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5677,7 +5677,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="205" t="s">
+      <c r="H28" s="206" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5720,7 +5720,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="207"/>
+      <c r="H29" s="204"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5761,7 +5761,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="207"/>
+      <c r="H30" s="204"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5802,7 +5802,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="206"/>
+      <c r="H31" s="205"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5833,7 +5833,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="207" t="s">
+      <c r="H32" s="204" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5877,7 +5877,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="207"/>
+      <c r="H33" s="204"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5919,7 +5919,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="206"/>
+      <c r="H34" s="205"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -5973,7 +5973,7 @@
       <c r="K35" s="56" t="s">
         <v>64</v>
       </c>
-      <c r="L35" s="267" t="s">
+      <c r="L35" s="169" t="s">
         <v>178</v>
       </c>
       <c r="M35" s="47" t="s">
@@ -5982,11 +5982,23 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="I7:I9"/>
     <mergeCell ref="H28:H31"/>
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
@@ -6002,23 +6014,11 @@
     <mergeCell ref="J20:J23"/>
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="H24:H27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6038,13 +6038,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="202" t="s">
+      <c r="B2" s="225" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="203"/>
-      <c r="D2" s="203"/>
-      <c r="E2" s="204"/>
-      <c r="F2" s="172" t="s">
+      <c r="C2" s="226"/>
+      <c r="D2" s="226"/>
+      <c r="E2" s="227"/>
+      <c r="F2" s="174" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6061,7 +6061,7 @@
       <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="173"/>
+      <c r="F3" s="175"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
@@ -6247,30 +6247,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="174" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="256" t="s">
+      <c r="C2" s="258" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="257"/>
-      <c r="E2" s="257"/>
-      <c r="F2" s="257"/>
-      <c r="G2" s="257"/>
-      <c r="H2" s="257"/>
-      <c r="I2" s="257"/>
-      <c r="J2" s="257"/>
-      <c r="K2" s="257"/>
-      <c r="L2" s="257"/>
-      <c r="M2" s="257"/>
-      <c r="N2" s="257"/>
-      <c r="O2" s="257"/>
-      <c r="P2" s="257"/>
-      <c r="Q2" s="257"/>
-      <c r="R2" s="258"/>
+      <c r="D2" s="259"/>
+      <c r="E2" s="259"/>
+      <c r="F2" s="259"/>
+      <c r="G2" s="259"/>
+      <c r="H2" s="259"/>
+      <c r="I2" s="259"/>
+      <c r="J2" s="259"/>
+      <c r="K2" s="259"/>
+      <c r="L2" s="259"/>
+      <c r="M2" s="259"/>
+      <c r="N2" s="259"/>
+      <c r="O2" s="259"/>
+      <c r="P2" s="259"/>
+      <c r="Q2" s="259"/>
+      <c r="R2" s="260"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="173"/>
+      <c r="B3" s="175"/>
       <c r="C3" s="118">
         <v>15</v>
       </c>
@@ -6341,13 +6341,13 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="250" t="s">
+      <c r="N4" s="252" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="250"/>
-      <c r="P4" s="250"/>
-      <c r="Q4" s="250"/>
-      <c r="R4" s="251"/>
+      <c r="O4" s="252"/>
+      <c r="P4" s="252"/>
+      <c r="Q4" s="252"/>
+      <c r="R4" s="253"/>
     </row>
     <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
@@ -6361,16 +6361,16 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="252" t="s">
+      <c r="K5" s="254" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="248"/>
-      <c r="M5" s="248"/>
-      <c r="N5" s="248"/>
-      <c r="O5" s="248"/>
-      <c r="P5" s="248"/>
-      <c r="Q5" s="248"/>
-      <c r="R5" s="249"/>
+      <c r="L5" s="250"/>
+      <c r="M5" s="250"/>
+      <c r="N5" s="250"/>
+      <c r="O5" s="250"/>
+      <c r="P5" s="250"/>
+      <c r="Q5" s="250"/>
+      <c r="R5" s="251"/>
     </row>
     <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
@@ -6384,16 +6384,16 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="252" t="s">
+      <c r="K6" s="254" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="248"/>
-      <c r="M6" s="248"/>
-      <c r="N6" s="248"/>
-      <c r="O6" s="248"/>
-      <c r="P6" s="248"/>
-      <c r="Q6" s="248"/>
-      <c r="R6" s="249"/>
+      <c r="L6" s="250"/>
+      <c r="M6" s="250"/>
+      <c r="N6" s="250"/>
+      <c r="O6" s="250"/>
+      <c r="P6" s="250"/>
+      <c r="Q6" s="250"/>
+      <c r="R6" s="251"/>
     </row>
     <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
@@ -6407,39 +6407,39 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="253" t="s">
+      <c r="K7" s="255" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="254"/>
-      <c r="M7" s="254"/>
-      <c r="N7" s="254"/>
-      <c r="O7" s="254"/>
-      <c r="P7" s="254"/>
-      <c r="Q7" s="254"/>
-      <c r="R7" s="255"/>
+      <c r="L7" s="256"/>
+      <c r="M7" s="256"/>
+      <c r="N7" s="256"/>
+      <c r="O7" s="256"/>
+      <c r="P7" s="256"/>
+      <c r="Q7" s="256"/>
+      <c r="R7" s="257"/>
     </row>
     <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="247" t="s">
+      <c r="C8" s="249" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="248"/>
-      <c r="E8" s="248"/>
-      <c r="F8" s="248"/>
-      <c r="G8" s="248"/>
-      <c r="H8" s="248"/>
-      <c r="I8" s="248"/>
-      <c r="J8" s="248"/>
-      <c r="K8" s="248"/>
-      <c r="L8" s="248"/>
-      <c r="M8" s="248"/>
-      <c r="N8" s="248"/>
-      <c r="O8" s="248"/>
-      <c r="P8" s="248"/>
-      <c r="Q8" s="248"/>
-      <c r="R8" s="249"/>
+      <c r="D8" s="250"/>
+      <c r="E8" s="250"/>
+      <c r="F8" s="250"/>
+      <c r="G8" s="250"/>
+      <c r="H8" s="250"/>
+      <c r="I8" s="250"/>
+      <c r="J8" s="250"/>
+      <c r="K8" s="250"/>
+      <c r="L8" s="250"/>
+      <c r="M8" s="250"/>
+      <c r="N8" s="250"/>
+      <c r="O8" s="250"/>
+      <c r="P8" s="250"/>
+      <c r="Q8" s="250"/>
+      <c r="R8" s="251"/>
     </row>
     <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
@@ -6651,10 +6651,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="259" t="s">
+      <c r="B2" s="261" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="260"/>
+      <c r="C2" s="262"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6671,7 +6671,7 @@
       <c r="C4" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="261" t="s">
+      <c r="D4" s="263" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6680,21 +6680,21 @@
       <c r="C5" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="262"/>
+      <c r="D5" s="264"/>
     </row>
     <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="263"/>
+      <c r="D6" s="265"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="145"/>
-      <c r="D7" s="264" t="s">
+      <c r="D7" s="266" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6703,14 +6703,14 @@
         <v>142</v>
       </c>
       <c r="C8" s="146"/>
-      <c r="D8" s="265"/>
+      <c r="D8" s="267"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
       <c r="C9" s="146"/>
-      <c r="D9" s="265"/>
+      <c r="D9" s="267"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
@@ -6719,7 +6719,7 @@
       <c r="C10" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="265"/>
+      <c r="D10" s="267"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
@@ -6728,7 +6728,7 @@
       <c r="C11" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="265"/>
+      <c r="D11" s="267"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6738,7 +6738,7 @@
       <c r="C12" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="266"/>
+      <c r="D12" s="268"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added frontpanel, sequencer, opcode decoder, updated lite opcodes
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF10C2F4-314D-429A-933A-D49AE7C6B758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF430FE-B514-48F9-B41E-98C7F88969A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="182">
   <si>
     <t>MODE B</t>
   </si>
@@ -581,6 +581,15 @@
   </si>
   <si>
     <t>OVERRIDDEN</t>
+  </si>
+  <si>
+    <t>"""BITWISE"""</t>
+  </si>
+  <si>
+    <t>Decodes Bit 0 - Bit 2 of input, upper bits unused.</t>
+  </si>
+  <si>
+    <t>value [0..2]</t>
   </si>
 </sst>
 </file>
@@ -1476,7 +1485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1966,6 +1975,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2005,94 +2050,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2101,17 +2092,44 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2126,9 +2144,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2137,45 +2152,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2235,6 +2211,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2578,7 +2599,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C12" sqref="C12:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2902,7 +2923,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="60">
-        <f t="shared" si="0"/>
+        <f>_xlfn.BITAND(_xlfn.BITRSHIFT($B12,3),1)</f>
         <v>1</v>
       </c>
       <c r="D12" s="14">
@@ -3237,73 +3258,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="201" t="s">
+      <c r="C3" s="188" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="202"/>
-      <c r="E3" s="202"/>
-      <c r="F3" s="202"/>
-      <c r="G3" s="203"/>
-      <c r="H3" s="198" t="s">
+      <c r="D3" s="189"/>
+      <c r="E3" s="189"/>
+      <c r="F3" s="189"/>
+      <c r="G3" s="190"/>
+      <c r="H3" s="185" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="199"/>
-      <c r="J3" s="200"/>
-      <c r="K3" s="198" t="s">
+      <c r="I3" s="186"/>
+      <c r="J3" s="187"/>
+      <c r="K3" s="185" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="199"/>
-      <c r="M3" s="199"/>
-      <c r="N3" s="185" t="s">
+      <c r="L3" s="186"/>
+      <c r="M3" s="186"/>
+      <c r="N3" s="197" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="186"/>
-      <c r="P3" s="187"/>
+      <c r="O3" s="198"/>
+      <c r="P3" s="199"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="179" t="s">
+      <c r="S3" s="191" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="180"/>
-      <c r="U3" s="180"/>
-      <c r="V3" s="180"/>
-      <c r="W3" s="180"/>
-      <c r="X3" s="180"/>
-      <c r="Y3" s="180"/>
-      <c r="Z3" s="181"/>
-      <c r="AA3" s="182" t="s">
+      <c r="T3" s="192"/>
+      <c r="U3" s="192"/>
+      <c r="V3" s="192"/>
+      <c r="W3" s="192"/>
+      <c r="X3" s="192"/>
+      <c r="Y3" s="192"/>
+      <c r="Z3" s="193"/>
+      <c r="AA3" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="183"/>
-      <c r="AC3" s="183"/>
-      <c r="AD3" s="183"/>
-      <c r="AE3" s="183"/>
-      <c r="AF3" s="183"/>
-      <c r="AG3" s="183"/>
-      <c r="AH3" s="184"/>
+      <c r="AB3" s="195"/>
+      <c r="AC3" s="195"/>
+      <c r="AD3" s="195"/>
+      <c r="AE3" s="195"/>
+      <c r="AF3" s="195"/>
+      <c r="AG3" s="195"/>
+      <c r="AH3" s="196"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="190" t="s">
+      <c r="B5" s="202" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="188" t="s">
+      <c r="C5" s="200" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="188"/>
-      <c r="E5" s="188"/>
-      <c r="F5" s="188"/>
-      <c r="G5" s="188"/>
-      <c r="H5" s="188"/>
-      <c r="I5" s="188"/>
-      <c r="J5" s="189"/>
+      <c r="D5" s="200"/>
+      <c r="E5" s="200"/>
+      <c r="F5" s="200"/>
+      <c r="G5" s="200"/>
+      <c r="H5" s="200"/>
+      <c r="I5" s="200"/>
+      <c r="J5" s="201"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="191"/>
+      <c r="B6" s="203"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3333,16 +3354,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="192" t="s">
+      <c r="C7" s="179" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="193"/>
-      <c r="E7" s="193"/>
-      <c r="F7" s="193"/>
-      <c r="G7" s="193"/>
-      <c r="H7" s="193"/>
-      <c r="I7" s="193"/>
-      <c r="J7" s="194"/>
+      <c r="D7" s="180"/>
+      <c r="E7" s="180"/>
+      <c r="F7" s="180"/>
+      <c r="G7" s="180"/>
+      <c r="H7" s="180"/>
+      <c r="I7" s="180"/>
+      <c r="J7" s="181"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3352,25 +3373,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="195" t="s">
+      <c r="G8" s="182" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="197"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="184"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="S3:Z3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3381,7 +3402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B20B11-9266-4E5E-A2B3-3496A1A10C3B}">
   <dimension ref="B1:Q35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20:H23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -3396,25 +3419,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="225" t="s">
+      <c r="B2" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="227"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="206"/>
       <c r="H2" s="174" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="225" t="s">
+      <c r="J2" s="204" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="226"/>
-      <c r="L2" s="226"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="205"/>
       <c r="M2" s="174" t="s">
         <v>112</v>
       </c>
@@ -3479,7 +3502,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="206" t="s">
+      <c r="H4" s="207" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3525,7 +3548,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="205"/>
+      <c r="H5" s="208"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3569,25 +3592,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="209" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="208" t="s">
+      <c r="J6" s="210" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="217" t="s">
+      <c r="K6" s="212" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="214" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="219" t="s">
+      <c r="M6" s="222" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="222" t="s">
+      <c r="N6" s="216" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3615,15 +3638,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
+      <c r="H7" s="209"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="208"/>
-      <c r="K7" s="217"/>
+      <c r="J7" s="210"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="214"/>
-      <c r="M7" s="220"/>
-      <c r="N7" s="222"/>
+      <c r="M7" s="223"/>
+      <c r="N7" s="216"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3649,15 +3672,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
+      <c r="H8" s="209"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="208"/>
-      <c r="K8" s="217"/>
+      <c r="J8" s="210"/>
+      <c r="K8" s="212"/>
       <c r="L8" s="214"/>
-      <c r="M8" s="220"/>
-      <c r="N8" s="222"/>
+      <c r="M8" s="223"/>
+      <c r="N8" s="216"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3683,15 +3706,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
+      <c r="H9" s="209"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="208"/>
-      <c r="K9" s="217"/>
+      <c r="J9" s="210"/>
+      <c r="K9" s="212"/>
       <c r="L9" s="214"/>
-      <c r="M9" s="220"/>
-      <c r="N9" s="222"/>
+      <c r="M9" s="223"/>
+      <c r="N9" s="216"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3717,15 +3740,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="209"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="208"/>
-      <c r="K10" s="217"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="212"/>
       <c r="L10" s="214"/>
-      <c r="M10" s="220"/>
-      <c r="N10" s="222"/>
+      <c r="M10" s="223"/>
+      <c r="N10" s="216"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3751,15 +3774,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="205"/>
+      <c r="H11" s="208"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="209"/>
-      <c r="K11" s="218"/>
+      <c r="J11" s="211"/>
+      <c r="K11" s="213"/>
       <c r="L11" s="215"/>
-      <c r="M11" s="221"/>
-      <c r="N11" s="223"/>
+      <c r="M11" s="224"/>
+      <c r="N11" s="217"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3785,25 +3808,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="206" t="s">
+      <c r="H12" s="207" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="207" t="s">
+      <c r="J12" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="216" t="s">
+      <c r="K12" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="213" t="s">
+      <c r="L12" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="206" t="s">
+      <c r="M12" s="207" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="224" t="s">
+      <c r="N12" s="221" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3831,15 +3854,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
+      <c r="H13" s="209"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="208"/>
-      <c r="K13" s="217"/>
+      <c r="J13" s="210"/>
+      <c r="K13" s="212"/>
       <c r="L13" s="214"/>
-      <c r="M13" s="204"/>
-      <c r="N13" s="222"/>
+      <c r="M13" s="209"/>
+      <c r="N13" s="216"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3865,15 +3888,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="209"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="208"/>
-      <c r="K14" s="217"/>
+      <c r="J14" s="210"/>
+      <c r="K14" s="212"/>
       <c r="L14" s="214"/>
-      <c r="M14" s="204"/>
-      <c r="N14" s="222"/>
+      <c r="M14" s="209"/>
+      <c r="N14" s="216"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3899,15 +3922,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="205"/>
+      <c r="H15" s="208"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="209"/>
-      <c r="K15" s="218"/>
+      <c r="J15" s="211"/>
+      <c r="K15" s="213"/>
       <c r="L15" s="215"/>
-      <c r="M15" s="205"/>
-      <c r="N15" s="223"/>
+      <c r="M15" s="208"/>
+      <c r="N15" s="217"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3933,22 +3956,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="206" t="s">
+      <c r="H16" s="207" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="207" t="s">
+      <c r="J16" s="218" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="210" t="s">
+      <c r="K16" s="225" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="213" t="s">
+      <c r="L16" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="206" t="s">
+      <c r="M16" s="207" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -3979,14 +4002,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="209"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="208"/>
-      <c r="K17" s="211"/>
+      <c r="J17" s="210"/>
+      <c r="K17" s="226"/>
       <c r="L17" s="214"/>
-      <c r="M17" s="204"/>
+      <c r="M17" s="209"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4015,14 +4038,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
+      <c r="H18" s="209"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="208"/>
-      <c r="K18" s="211"/>
+      <c r="J18" s="210"/>
+      <c r="K18" s="226"/>
       <c r="L18" s="214"/>
-      <c r="M18" s="204"/>
+      <c r="M18" s="209"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4051,14 +4074,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="205"/>
+      <c r="H19" s="208"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="209"/>
-      <c r="K19" s="212"/>
+      <c r="J19" s="211"/>
+      <c r="K19" s="227"/>
       <c r="L19" s="215"/>
-      <c r="M19" s="205"/>
+      <c r="M19" s="208"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4088,22 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="206" t="s">
+      <c r="H20" s="207" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="207" t="s">
+      <c r="J20" s="218" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="216" t="s">
+      <c r="K20" s="219" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="213" t="s">
+      <c r="L20" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="219" t="s">
+      <c r="M20" s="222" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4134,14 +4157,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="204"/>
+      <c r="H21" s="209"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="208"/>
-      <c r="K21" s="217"/>
+      <c r="J21" s="210"/>
+      <c r="K21" s="212"/>
       <c r="L21" s="214"/>
-      <c r="M21" s="220"/>
+      <c r="M21" s="223"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4170,14 +4193,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="204"/>
+      <c r="H22" s="209"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="208"/>
-      <c r="K22" s="217"/>
+      <c r="J22" s="210"/>
+      <c r="K22" s="212"/>
       <c r="L22" s="214"/>
-      <c r="M22" s="220"/>
+      <c r="M22" s="223"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4206,14 +4229,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="205"/>
+      <c r="H23" s="208"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="209"/>
-      <c r="K23" s="218"/>
+      <c r="J23" s="211"/>
+      <c r="K23" s="213"/>
       <c r="L23" s="215"/>
-      <c r="M23" s="221"/>
+      <c r="M23" s="224"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4242,7 +4265,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="206" t="s">
+      <c r="H24" s="207" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4288,7 +4311,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="209"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4332,7 +4355,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
+      <c r="H26" s="209"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4364,7 +4387,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="205"/>
+      <c r="H27" s="208"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4396,7 +4419,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="206" t="s">
+      <c r="H28" s="207" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4442,7 +4465,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="209"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4486,7 +4509,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="209"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4530,7 +4553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="205"/>
+      <c r="H31" s="208"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4562,7 +4585,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="209" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4609,7 +4632,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="209"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4654,7 +4677,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="205"/>
+      <c r="H34" s="208"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4711,17 +4734,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="M20:M23"/>
     <mergeCell ref="N6:N11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
@@ -4730,19 +4755,17 @@
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
     <mergeCell ref="M6:M11"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4753,7 +4776,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD788E61-AC5A-4E7F-9536-02553AF94143}">
   <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16:L19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4767,25 +4792,25 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="225" t="s">
+      <c r="B2" s="204" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="226"/>
-      <c r="F2" s="226"/>
-      <c r="G2" s="227"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="205"/>
+      <c r="F2" s="205"/>
+      <c r="G2" s="206"/>
       <c r="H2" s="174" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="174" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="225" t="s">
+      <c r="J2" s="204" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="226"/>
-      <c r="L2" s="226"/>
+      <c r="K2" s="205"/>
+      <c r="L2" s="205"/>
       <c r="M2" s="174" t="s">
         <v>33</v>
       </c>
@@ -4846,7 +4871,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="206" t="s">
+      <c r="H4" s="207" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4858,8 +4883,8 @@
       <c r="K4" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="170" t="s">
-        <v>3</v>
+      <c r="L4" s="67" t="s">
+        <v>85</v>
       </c>
       <c r="M4" s="76" t="s">
         <v>116</v>
@@ -4889,7 +4914,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="205"/>
+      <c r="H5" s="208"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4900,7 +4925,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="64" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="M5" s="45" t="s">
         <v>117</v>
@@ -4930,22 +4955,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="204" t="s">
+      <c r="H6" s="209" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="65" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="208" t="s">
+      <c r="I6" s="260"/>
+      <c r="J6" s="210" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="217" t="s">
+      <c r="K6" s="212" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="214" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="222" t="s">
+      <c r="M6" s="216" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4973,12 +4996,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="204"/>
-      <c r="I7" s="236"/>
-      <c r="J7" s="208"/>
-      <c r="K7" s="217"/>
+      <c r="H7" s="209"/>
+      <c r="I7" s="71" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="210"/>
+      <c r="K7" s="212"/>
       <c r="L7" s="214"/>
-      <c r="M7" s="222"/>
+      <c r="M7" s="216"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5004,12 +5029,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="204"/>
-      <c r="I8" s="238"/>
-      <c r="J8" s="208"/>
-      <c r="K8" s="217"/>
+      <c r="H8" s="209"/>
+      <c r="I8" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="210"/>
+      <c r="K8" s="212"/>
       <c r="L8" s="214"/>
-      <c r="M8" s="222"/>
+      <c r="M8" s="216"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5035,12 +5062,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="204"/>
-      <c r="I9" s="248"/>
-      <c r="J9" s="208"/>
-      <c r="K9" s="217"/>
+      <c r="H9" s="209"/>
+      <c r="I9" s="260"/>
+      <c r="J9" s="210"/>
+      <c r="K9" s="212"/>
       <c r="L9" s="214"/>
-      <c r="M9" s="222"/>
+      <c r="M9" s="216"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5066,14 +5093,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="204"/>
+      <c r="H10" s="209"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="208"/>
-      <c r="K10" s="217"/>
+      <c r="J10" s="210"/>
+      <c r="K10" s="212"/>
       <c r="L10" s="214"/>
-      <c r="M10" s="222"/>
+      <c r="M10" s="216"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5099,12 +5126,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="205"/>
+      <c r="H11" s="208"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="209"/>
-      <c r="K11" s="218"/>
+      <c r="J11" s="211"/>
+      <c r="K11" s="213"/>
       <c r="L11" s="215"/>
-      <c r="M11" s="223"/>
+      <c r="M11" s="217"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5130,22 +5157,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="206" t="s">
+      <c r="H12" s="207" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="207" t="s">
+      <c r="J12" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="216" t="s">
+      <c r="K12" s="219" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="213" t="s">
+      <c r="L12" s="220" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="224" t="s">
+      <c r="M12" s="221" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5173,12 +5200,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="204"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="208"/>
-      <c r="K13" s="217"/>
+      <c r="H13" s="209"/>
+      <c r="I13" s="258" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="210"/>
+      <c r="K13" s="212"/>
       <c r="L13" s="214"/>
-      <c r="M13" s="222"/>
+      <c r="M13" s="216"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5204,12 +5233,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="204"/>
+      <c r="H14" s="209"/>
       <c r="I14" s="105"/>
-      <c r="J14" s="208"/>
-      <c r="K14" s="217"/>
+      <c r="J14" s="210"/>
+      <c r="K14" s="212"/>
       <c r="L14" s="214"/>
-      <c r="M14" s="222"/>
+      <c r="M14" s="216"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5235,12 +5264,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="205"/>
+      <c r="H15" s="208"/>
       <c r="I15" s="105"/>
-      <c r="J15" s="209"/>
-      <c r="K15" s="218"/>
+      <c r="J15" s="211"/>
+      <c r="K15" s="213"/>
       <c r="L15" s="215"/>
-      <c r="M15" s="223"/>
+      <c r="M15" s="217"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5266,19 +5295,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="206" t="s">
+      <c r="H16" s="207" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="207" t="s">
+      <c r="J16" s="218" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="210" t="s">
+      <c r="K16" s="225" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="213" t="s">
+      <c r="L16" s="220" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5309,12 +5338,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="204"/>
+      <c r="H17" s="209"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="208"/>
-      <c r="K17" s="211"/>
+      <c r="J17" s="210"/>
+      <c r="K17" s="226"/>
       <c r="L17" s="214"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
@@ -5344,12 +5373,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="204"/>
-      <c r="I18" s="236"/>
-      <c r="J18" s="208"/>
-      <c r="K18" s="211"/>
+      <c r="H18" s="209"/>
+      <c r="I18" s="228"/>
+      <c r="J18" s="210"/>
+      <c r="K18" s="226"/>
       <c r="L18" s="214"/>
-      <c r="M18" s="236"/>
+      <c r="M18" s="228"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5375,12 +5404,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="205"/>
-      <c r="I19" s="237"/>
-      <c r="J19" s="209"/>
-      <c r="K19" s="212"/>
+      <c r="H19" s="208"/>
+      <c r="I19" s="229"/>
+      <c r="J19" s="211"/>
+      <c r="K19" s="227"/>
       <c r="L19" s="215"/>
-      <c r="M19" s="237"/>
+      <c r="M19" s="229"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5407,12 +5436,24 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="239"/>
-      <c r="I20" s="238"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="243"/>
-      <c r="L20" s="246"/>
-      <c r="M20" s="238"/>
+      <c r="H20" s="270" t="s">
+        <v>179</v>
+      </c>
+      <c r="I20" s="269" t="s">
+        <v>119</v>
+      </c>
+      <c r="J20" s="67" t="s">
+        <v>181</v>
+      </c>
+      <c r="K20" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="170" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="268" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B21" s="82">
@@ -5438,12 +5479,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="238"/>
-      <c r="I21" s="238"/>
-      <c r="J21" s="241"/>
-      <c r="K21" s="244"/>
-      <c r="L21" s="247"/>
-      <c r="M21" s="238"/>
+      <c r="H21" s="271"/>
+      <c r="I21" s="259"/>
+      <c r="J21" s="262"/>
+      <c r="K21" s="264"/>
+      <c r="L21" s="266"/>
+      <c r="M21" s="259"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
@@ -5469,12 +5510,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="238"/>
-      <c r="I22" s="238"/>
-      <c r="J22" s="241"/>
-      <c r="K22" s="244"/>
-      <c r="L22" s="247"/>
-      <c r="M22" s="238"/>
+      <c r="H22" s="271"/>
+      <c r="I22" s="259"/>
+      <c r="J22" s="262"/>
+      <c r="K22" s="264"/>
+      <c r="L22" s="266"/>
+      <c r="M22" s="259"/>
     </row>
     <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
@@ -5500,12 +5541,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="237"/>
-      <c r="I23" s="237"/>
-      <c r="J23" s="242"/>
-      <c r="K23" s="245"/>
-      <c r="L23" s="233"/>
-      <c r="M23" s="237"/>
+      <c r="H23" s="272"/>
+      <c r="I23" s="261"/>
+      <c r="J23" s="263"/>
+      <c r="K23" s="265"/>
+      <c r="L23" s="267"/>
+      <c r="M23" s="261"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
@@ -5531,7 +5572,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="206" t="s">
+      <c r="H24" s="207" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5574,7 +5615,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="204"/>
+      <c r="H25" s="209"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5615,12 +5656,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="204"/>
-      <c r="I26" s="236"/>
-      <c r="J26" s="228"/>
-      <c r="K26" s="230"/>
-      <c r="L26" s="232"/>
-      <c r="M26" s="234"/>
+      <c r="H26" s="209"/>
+      <c r="I26" s="228"/>
+      <c r="J26" s="231"/>
+      <c r="K26" s="233"/>
+      <c r="L26" s="235"/>
+      <c r="M26" s="236"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5646,12 +5687,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="205"/>
-      <c r="I27" s="237"/>
-      <c r="J27" s="229"/>
-      <c r="K27" s="231"/>
-      <c r="L27" s="233"/>
-      <c r="M27" s="235"/>
+      <c r="H27" s="208"/>
+      <c r="I27" s="229"/>
+      <c r="J27" s="232"/>
+      <c r="K27" s="234"/>
+      <c r="L27" s="230"/>
+      <c r="M27" s="237"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5677,7 +5718,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="206" t="s">
+      <c r="H28" s="207" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5720,7 +5761,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="204"/>
+      <c r="H29" s="209"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5761,7 +5802,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="204"/>
+      <c r="H30" s="209"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5802,7 +5843,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="205"/>
+      <c r="H31" s="208"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5833,7 +5874,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="204" t="s">
+      <c r="H32" s="209" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5877,7 +5918,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="204"/>
+      <c r="H33" s="209"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5919,7 +5960,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="205"/>
+      <c r="H34" s="208"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -5981,44 +6022,38 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
+  <mergeCells count="31">
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="J26:J27"/>
     <mergeCell ref="M6:M11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
     <mergeCell ref="K12:K15"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="I20:I23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6029,7 +6064,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4182B34D-1176-43D9-83DE-D8E7EA5C96ED}">
   <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6038,12 +6075,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="225" t="s">
+      <c r="B2" s="204" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="226"/>
-      <c r="D2" s="226"/>
-      <c r="E2" s="227"/>
+      <c r="C2" s="205"/>
+      <c r="D2" s="205"/>
+      <c r="E2" s="206"/>
       <c r="F2" s="174" t="s">
         <v>32</v>
       </c>
@@ -6250,24 +6287,24 @@
       <c r="B2" s="174" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="258" t="s">
+      <c r="C2" s="247" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="259"/>
-      <c r="E2" s="259"/>
-      <c r="F2" s="259"/>
-      <c r="G2" s="259"/>
-      <c r="H2" s="259"/>
-      <c r="I2" s="259"/>
-      <c r="J2" s="259"/>
-      <c r="K2" s="259"/>
-      <c r="L2" s="259"/>
-      <c r="M2" s="259"/>
-      <c r="N2" s="259"/>
-      <c r="O2" s="259"/>
-      <c r="P2" s="259"/>
-      <c r="Q2" s="259"/>
-      <c r="R2" s="260"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="248"/>
+      <c r="F2" s="248"/>
+      <c r="G2" s="248"/>
+      <c r="H2" s="248"/>
+      <c r="I2" s="248"/>
+      <c r="J2" s="248"/>
+      <c r="K2" s="248"/>
+      <c r="L2" s="248"/>
+      <c r="M2" s="248"/>
+      <c r="N2" s="248"/>
+      <c r="O2" s="248"/>
+      <c r="P2" s="248"/>
+      <c r="Q2" s="248"/>
+      <c r="R2" s="249"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="175"/>
@@ -6341,13 +6378,13 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="252" t="s">
+      <c r="N4" s="241" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="252"/>
-      <c r="P4" s="252"/>
-      <c r="Q4" s="252"/>
-      <c r="R4" s="253"/>
+      <c r="O4" s="241"/>
+      <c r="P4" s="241"/>
+      <c r="Q4" s="241"/>
+      <c r="R4" s="242"/>
     </row>
     <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
@@ -6361,16 +6398,16 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="254" t="s">
+      <c r="K5" s="243" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="250"/>
-      <c r="M5" s="250"/>
-      <c r="N5" s="250"/>
-      <c r="O5" s="250"/>
-      <c r="P5" s="250"/>
-      <c r="Q5" s="250"/>
-      <c r="R5" s="251"/>
+      <c r="L5" s="239"/>
+      <c r="M5" s="239"/>
+      <c r="N5" s="239"/>
+      <c r="O5" s="239"/>
+      <c r="P5" s="239"/>
+      <c r="Q5" s="239"/>
+      <c r="R5" s="240"/>
     </row>
     <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
@@ -6384,16 +6421,16 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="254" t="s">
+      <c r="K6" s="243" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="250"/>
-      <c r="M6" s="250"/>
-      <c r="N6" s="250"/>
-      <c r="O6" s="250"/>
-      <c r="P6" s="250"/>
-      <c r="Q6" s="250"/>
-      <c r="R6" s="251"/>
+      <c r="L6" s="239"/>
+      <c r="M6" s="239"/>
+      <c r="N6" s="239"/>
+      <c r="O6" s="239"/>
+      <c r="P6" s="239"/>
+      <c r="Q6" s="239"/>
+      <c r="R6" s="240"/>
     </row>
     <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
@@ -6407,39 +6444,39 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="255" t="s">
+      <c r="K7" s="244" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="256"/>
-      <c r="M7" s="256"/>
-      <c r="N7" s="256"/>
-      <c r="O7" s="256"/>
-      <c r="P7" s="256"/>
-      <c r="Q7" s="256"/>
-      <c r="R7" s="257"/>
+      <c r="L7" s="245"/>
+      <c r="M7" s="245"/>
+      <c r="N7" s="245"/>
+      <c r="O7" s="245"/>
+      <c r="P7" s="245"/>
+      <c r="Q7" s="245"/>
+      <c r="R7" s="246"/>
     </row>
     <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="249" t="s">
+      <c r="C8" s="238" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="250"/>
-      <c r="E8" s="250"/>
-      <c r="F8" s="250"/>
-      <c r="G8" s="250"/>
-      <c r="H8" s="250"/>
-      <c r="I8" s="250"/>
-      <c r="J8" s="250"/>
-      <c r="K8" s="250"/>
-      <c r="L8" s="250"/>
-      <c r="M8" s="250"/>
-      <c r="N8" s="250"/>
-      <c r="O8" s="250"/>
-      <c r="P8" s="250"/>
-      <c r="Q8" s="250"/>
-      <c r="R8" s="251"/>
+      <c r="D8" s="239"/>
+      <c r="E8" s="239"/>
+      <c r="F8" s="239"/>
+      <c r="G8" s="239"/>
+      <c r="H8" s="239"/>
+      <c r="I8" s="239"/>
+      <c r="J8" s="239"/>
+      <c r="K8" s="239"/>
+      <c r="L8" s="239"/>
+      <c r="M8" s="239"/>
+      <c r="N8" s="239"/>
+      <c r="O8" s="239"/>
+      <c r="P8" s="239"/>
+      <c r="Q8" s="239"/>
+      <c r="R8" s="240"/>
     </row>
     <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
@@ -6487,7 +6524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27FF78FE-3CCF-4749-B213-A95B9184CAE3}">
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="B17:D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -6651,10 +6690,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="261" t="s">
+      <c r="B2" s="250" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="262"/>
+      <c r="C2" s="251"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6671,7 +6710,7 @@
       <c r="C4" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="263" t="s">
+      <c r="D4" s="252" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6680,21 +6719,21 @@
       <c r="C5" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="264"/>
+      <c r="D5" s="253"/>
     </row>
     <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="265"/>
+      <c r="D6" s="254"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="145"/>
-      <c r="D7" s="266" t="s">
+      <c r="D7" s="255" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6703,14 +6742,14 @@
         <v>142</v>
       </c>
       <c r="C8" s="146"/>
-      <c r="D8" s="267"/>
+      <c r="D8" s="256"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
       <c r="C9" s="146"/>
-      <c r="D9" s="267"/>
+      <c r="D9" s="256"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
@@ -6719,7 +6758,7 @@
       <c r="C10" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="267"/>
+      <c r="D10" s="256"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
@@ -6728,7 +6767,7 @@
       <c r="C11" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="267"/>
+      <c r="D11" s="256"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6738,7 +6777,7 @@
       <c r="C12" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="268"/>
+      <c r="D12" s="257"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
added opcode decoder, memory read unit
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF430FE-B514-48F9-B41E-98C7F88969A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAB9820-1F92-44F9-914C-085480A8E1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -1951,6 +1951,42 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1975,6 +2011,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2011,44 +2086,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2059,91 +2158,16 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2152,6 +2176,27 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2211,51 +2256,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2611,19 +2611,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="171" t="s">
+      <c r="B2" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="173"/>
-      <c r="G2" s="176" t="s">
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="185"/>
+      <c r="G2" s="188" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="177"/>
-      <c r="I2" s="178"/>
-      <c r="J2" s="174" t="s">
+      <c r="H2" s="189"/>
+      <c r="I2" s="190"/>
+      <c r="J2" s="186" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       <c r="I3" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="175"/>
+      <c r="J3" s="187"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
@@ -3258,23 +3258,23 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="188" t="s">
+      <c r="C3" s="213" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="189"/>
-      <c r="E3" s="189"/>
-      <c r="F3" s="189"/>
-      <c r="G3" s="190"/>
-      <c r="H3" s="185" t="s">
+      <c r="D3" s="214"/>
+      <c r="E3" s="214"/>
+      <c r="F3" s="214"/>
+      <c r="G3" s="215"/>
+      <c r="H3" s="210" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="186"/>
-      <c r="J3" s="187"/>
-      <c r="K3" s="185" t="s">
+      <c r="I3" s="211"/>
+      <c r="J3" s="212"/>
+      <c r="K3" s="210" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="186"/>
-      <c r="M3" s="186"/>
+      <c r="L3" s="211"/>
+      <c r="M3" s="211"/>
       <c r="N3" s="197" t="s">
         <v>95</v>
       </c>
@@ -3354,16 +3354,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="179" t="s">
+      <c r="C7" s="204" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="180"/>
-      <c r="E7" s="180"/>
-      <c r="F7" s="180"/>
-      <c r="G7" s="180"/>
-      <c r="H7" s="180"/>
-      <c r="I7" s="180"/>
-      <c r="J7" s="181"/>
+      <c r="D7" s="205"/>
+      <c r="E7" s="205"/>
+      <c r="F7" s="205"/>
+      <c r="G7" s="205"/>
+      <c r="H7" s="205"/>
+      <c r="I7" s="205"/>
+      <c r="J7" s="206"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3373,25 +3373,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="182" t="s">
+      <c r="G8" s="207" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="184"/>
+      <c r="H8" s="208"/>
+      <c r="I8" s="208"/>
+      <c r="J8" s="209"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3419,29 +3419,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="237" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="174" t="s">
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="174" t="s">
+      <c r="I2" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="204" t="s">
+      <c r="J2" s="237" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="205"/>
-      <c r="L2" s="205"/>
-      <c r="M2" s="174" t="s">
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="186" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="174" t="s">
+      <c r="N2" s="186" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3464,8 +3464,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -3475,8 +3475,8 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="175"/>
-      <c r="N3" s="175"/>
+      <c r="M3" s="187"/>
+      <c r="N3" s="187"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -3502,7 +3502,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="207" t="s">
+      <c r="H4" s="218" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3548,7 +3548,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="208"/>
+      <c r="H5" s="217"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3592,25 +3592,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="209" t="s">
+      <c r="H6" s="216" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="210" t="s">
+      <c r="J6" s="220" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="212" t="s">
+      <c r="K6" s="229" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="214" t="s">
+      <c r="L6" s="226" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="222" t="s">
+      <c r="M6" s="231" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="216" t="s">
+      <c r="N6" s="234" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3638,15 +3638,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="209"/>
+      <c r="H7" s="216"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="210"/>
-      <c r="K7" s="212"/>
-      <c r="L7" s="214"/>
-      <c r="M7" s="223"/>
-      <c r="N7" s="216"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="226"/>
+      <c r="M7" s="232"/>
+      <c r="N7" s="234"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3672,15 +3672,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="209"/>
+      <c r="H8" s="216"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="210"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="214"/>
-      <c r="M8" s="223"/>
-      <c r="N8" s="216"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="229"/>
+      <c r="L8" s="226"/>
+      <c r="M8" s="232"/>
+      <c r="N8" s="234"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3706,15 +3706,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="209"/>
+      <c r="H9" s="216"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="210"/>
-      <c r="K9" s="212"/>
-      <c r="L9" s="214"/>
-      <c r="M9" s="223"/>
-      <c r="N9" s="216"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="229"/>
+      <c r="L9" s="226"/>
+      <c r="M9" s="232"/>
+      <c r="N9" s="234"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3740,15 +3740,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="209"/>
+      <c r="H10" s="216"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="210"/>
-      <c r="K10" s="212"/>
-      <c r="L10" s="214"/>
-      <c r="M10" s="223"/>
-      <c r="N10" s="216"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="229"/>
+      <c r="L10" s="226"/>
+      <c r="M10" s="232"/>
+      <c r="N10" s="234"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3774,15 +3774,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="208"/>
+      <c r="H11" s="217"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="211"/>
-      <c r="K11" s="213"/>
-      <c r="L11" s="215"/>
-      <c r="M11" s="224"/>
-      <c r="N11" s="217"/>
+      <c r="J11" s="221"/>
+      <c r="K11" s="230"/>
+      <c r="L11" s="227"/>
+      <c r="M11" s="233"/>
+      <c r="N11" s="235"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3808,25 +3808,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="207" t="s">
+      <c r="H12" s="218" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="218" t="s">
+      <c r="J12" s="219" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="219" t="s">
+      <c r="K12" s="228" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="220" t="s">
+      <c r="L12" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="207" t="s">
+      <c r="M12" s="218" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="221" t="s">
+      <c r="N12" s="236" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3854,15 +3854,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="209"/>
+      <c r="H13" s="216"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="210"/>
-      <c r="K13" s="212"/>
-      <c r="L13" s="214"/>
-      <c r="M13" s="209"/>
-      <c r="N13" s="216"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="229"/>
+      <c r="L13" s="226"/>
+      <c r="M13" s="216"/>
+      <c r="N13" s="234"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3888,15 +3888,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="209"/>
+      <c r="H14" s="216"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="210"/>
-      <c r="K14" s="212"/>
-      <c r="L14" s="214"/>
-      <c r="M14" s="209"/>
-      <c r="N14" s="216"/>
+      <c r="J14" s="220"/>
+      <c r="K14" s="229"/>
+      <c r="L14" s="226"/>
+      <c r="M14" s="216"/>
+      <c r="N14" s="234"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3922,15 +3922,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="208"/>
+      <c r="H15" s="217"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="211"/>
-      <c r="K15" s="213"/>
-      <c r="L15" s="215"/>
-      <c r="M15" s="208"/>
-      <c r="N15" s="217"/>
+      <c r="J15" s="221"/>
+      <c r="K15" s="230"/>
+      <c r="L15" s="227"/>
+      <c r="M15" s="217"/>
+      <c r="N15" s="235"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3956,22 +3956,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="207" t="s">
+      <c r="H16" s="218" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="218" t="s">
+      <c r="J16" s="219" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="225" t="s">
+      <c r="K16" s="222" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="220" t="s">
+      <c r="L16" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="207" t="s">
+      <c r="M16" s="218" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -4002,14 +4002,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="209"/>
+      <c r="H17" s="216"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="210"/>
-      <c r="K17" s="226"/>
-      <c r="L17" s="214"/>
-      <c r="M17" s="209"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="223"/>
+      <c r="L17" s="226"/>
+      <c r="M17" s="216"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4038,14 +4038,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="209"/>
+      <c r="H18" s="216"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="210"/>
-      <c r="K18" s="226"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="209"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="223"/>
+      <c r="L18" s="226"/>
+      <c r="M18" s="216"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4074,14 +4074,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="208"/>
+      <c r="H19" s="217"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="211"/>
-      <c r="K19" s="227"/>
-      <c r="L19" s="215"/>
-      <c r="M19" s="208"/>
+      <c r="J19" s="221"/>
+      <c r="K19" s="224"/>
+      <c r="L19" s="227"/>
+      <c r="M19" s="217"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4111,22 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="207" t="s">
+      <c r="H20" s="218" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="218" t="s">
+      <c r="J20" s="219" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="219" t="s">
+      <c r="K20" s="228" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="220" t="s">
+      <c r="L20" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="222" t="s">
+      <c r="M20" s="231" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4157,14 +4157,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="209"/>
+      <c r="H21" s="216"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="210"/>
-      <c r="K21" s="212"/>
-      <c r="L21" s="214"/>
-      <c r="M21" s="223"/>
+      <c r="J21" s="220"/>
+      <c r="K21" s="229"/>
+      <c r="L21" s="226"/>
+      <c r="M21" s="232"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4193,14 +4193,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="209"/>
+      <c r="H22" s="216"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="210"/>
-      <c r="K22" s="212"/>
-      <c r="L22" s="214"/>
-      <c r="M22" s="223"/>
+      <c r="J22" s="220"/>
+      <c r="K22" s="229"/>
+      <c r="L22" s="226"/>
+      <c r="M22" s="232"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4229,14 +4229,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="208"/>
+      <c r="H23" s="217"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="211"/>
-      <c r="K23" s="213"/>
-      <c r="L23" s="215"/>
-      <c r="M23" s="224"/>
+      <c r="J23" s="221"/>
+      <c r="K23" s="230"/>
+      <c r="L23" s="227"/>
+      <c r="M23" s="233"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4265,7 +4265,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="207" t="s">
+      <c r="H24" s="218" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4311,7 +4311,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="209"/>
+      <c r="H25" s="216"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4355,7 +4355,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="209"/>
+      <c r="H26" s="216"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4387,7 +4387,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="208"/>
+      <c r="H27" s="217"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4419,7 +4419,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="207" t="s">
+      <c r="H28" s="218" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4465,7 +4465,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="209"/>
+      <c r="H29" s="216"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4509,7 +4509,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="209"/>
+      <c r="H30" s="216"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4553,7 +4553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="208"/>
+      <c r="H31" s="217"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4585,7 +4585,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="209" t="s">
+      <c r="H32" s="216" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4632,7 +4632,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="209"/>
+      <c r="H33" s="216"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4677,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="208"/>
+      <c r="H34" s="217"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4734,11 +4734,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4747,25 +4761,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4776,9 +4776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD788E61-AC5A-4E7F-9536-02553AF94143}">
   <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16:L19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4792,26 +4790,26 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="237" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="206"/>
-      <c r="H2" s="174" t="s">
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="238"/>
+      <c r="F2" s="238"/>
+      <c r="G2" s="239"/>
+      <c r="H2" s="186" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="174" t="s">
+      <c r="I2" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="204" t="s">
+      <c r="J2" s="237" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="205"/>
-      <c r="L2" s="205"/>
-      <c r="M2" s="174" t="s">
+      <c r="K2" s="238"/>
+      <c r="L2" s="238"/>
+      <c r="M2" s="186" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4834,8 +4832,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="175"/>
-      <c r="I3" s="175"/>
+      <c r="H3" s="187"/>
+      <c r="I3" s="187"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -4845,7 +4843,7 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="175"/>
+      <c r="M3" s="187"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -4871,7 +4869,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="207" t="s">
+      <c r="H4" s="218" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4914,7 +4912,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="208"/>
+      <c r="H5" s="217"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4955,20 +4953,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="209" t="s">
+      <c r="H6" s="216" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="260"/>
-      <c r="J6" s="210" t="s">
+      <c r="I6" s="173"/>
+      <c r="J6" s="220" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="212" t="s">
+      <c r="K6" s="229" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="214" t="s">
+      <c r="L6" s="226" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="216" t="s">
+      <c r="M6" s="234" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4996,14 +4994,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="209"/>
+      <c r="H7" s="216"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="210"/>
-      <c r="K7" s="212"/>
-      <c r="L7" s="214"/>
-      <c r="M7" s="216"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="226"/>
+      <c r="M7" s="234"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5029,14 +5027,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="209"/>
+      <c r="H8" s="216"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="210"/>
-      <c r="K8" s="212"/>
-      <c r="L8" s="214"/>
-      <c r="M8" s="216"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="229"/>
+      <c r="L8" s="226"/>
+      <c r="M8" s="234"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5062,12 +5060,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="209"/>
-      <c r="I9" s="260"/>
-      <c r="J9" s="210"/>
-      <c r="K9" s="212"/>
-      <c r="L9" s="214"/>
-      <c r="M9" s="216"/>
+      <c r="H9" s="216"/>
+      <c r="I9" s="173"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="229"/>
+      <c r="L9" s="226"/>
+      <c r="M9" s="234"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5093,14 +5091,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="209"/>
+      <c r="H10" s="216"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="210"/>
-      <c r="K10" s="212"/>
-      <c r="L10" s="214"/>
-      <c r="M10" s="216"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="229"/>
+      <c r="L10" s="226"/>
+      <c r="M10" s="234"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5126,12 +5124,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="208"/>
+      <c r="H11" s="217"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="211"/>
-      <c r="K11" s="213"/>
-      <c r="L11" s="215"/>
-      <c r="M11" s="217"/>
+      <c r="J11" s="221"/>
+      <c r="K11" s="230"/>
+      <c r="L11" s="227"/>
+      <c r="M11" s="235"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5157,22 +5155,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="207" t="s">
+      <c r="H12" s="218" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="218" t="s">
+      <c r="J12" s="219" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="219" t="s">
+      <c r="K12" s="228" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="220" t="s">
+      <c r="L12" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="221" t="s">
+      <c r="M12" s="236" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5200,14 +5198,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="209"/>
-      <c r="I13" s="258" t="s">
+      <c r="H13" s="216"/>
+      <c r="I13" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="210"/>
-      <c r="K13" s="212"/>
-      <c r="L13" s="214"/>
-      <c r="M13" s="216"/>
+      <c r="J13" s="220"/>
+      <c r="K13" s="229"/>
+      <c r="L13" s="226"/>
+      <c r="M13" s="234"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5233,12 +5231,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="209"/>
+      <c r="H14" s="216"/>
       <c r="I14" s="105"/>
-      <c r="J14" s="210"/>
-      <c r="K14" s="212"/>
-      <c r="L14" s="214"/>
-      <c r="M14" s="216"/>
+      <c r="J14" s="220"/>
+      <c r="K14" s="229"/>
+      <c r="L14" s="226"/>
+      <c r="M14" s="234"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5264,12 +5262,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="208"/>
+      <c r="H15" s="217"/>
       <c r="I15" s="105"/>
-      <c r="J15" s="211"/>
-      <c r="K15" s="213"/>
-      <c r="L15" s="215"/>
-      <c r="M15" s="217"/>
+      <c r="J15" s="221"/>
+      <c r="K15" s="230"/>
+      <c r="L15" s="227"/>
+      <c r="M15" s="235"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5295,19 +5293,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="207" t="s">
+      <c r="H16" s="218" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="218" t="s">
+      <c r="J16" s="219" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="225" t="s">
+      <c r="K16" s="222" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="220" t="s">
+      <c r="L16" s="225" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5338,13 +5336,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="209"/>
+      <c r="H17" s="216"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="210"/>
-      <c r="K17" s="226"/>
-      <c r="L17" s="214"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="223"/>
+      <c r="L17" s="226"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
       </c>
@@ -5373,12 +5371,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="209"/>
-      <c r="I18" s="228"/>
-      <c r="J18" s="210"/>
-      <c r="K18" s="226"/>
-      <c r="L18" s="214"/>
-      <c r="M18" s="228"/>
+      <c r="H18" s="216"/>
+      <c r="I18" s="246"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="223"/>
+      <c r="L18" s="226"/>
+      <c r="M18" s="246"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5404,12 +5402,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="208"/>
-      <c r="I19" s="229"/>
-      <c r="J19" s="211"/>
-      <c r="K19" s="227"/>
-      <c r="L19" s="215"/>
-      <c r="M19" s="229"/>
+      <c r="H19" s="217"/>
+      <c r="I19" s="247"/>
+      <c r="J19" s="221"/>
+      <c r="K19" s="224"/>
+      <c r="L19" s="227"/>
+      <c r="M19" s="247"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5436,10 +5434,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="270" t="s">
+      <c r="H20" s="248" t="s">
         <v>179</v>
       </c>
-      <c r="I20" s="269" t="s">
+      <c r="I20" s="182" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="67" t="s">
@@ -5451,7 +5449,7 @@
       <c r="L20" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="268" t="s">
+      <c r="M20" s="181" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5479,12 +5477,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="271"/>
-      <c r="I21" s="259"/>
-      <c r="J21" s="262"/>
-      <c r="K21" s="264"/>
-      <c r="L21" s="266"/>
-      <c r="M21" s="259"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="172"/>
+      <c r="J21" s="175"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="179"/>
+      <c r="M21" s="172"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
@@ -5510,12 +5508,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="271"/>
-      <c r="I22" s="259"/>
-      <c r="J22" s="262"/>
-      <c r="K22" s="264"/>
-      <c r="L22" s="266"/>
-      <c r="M22" s="259"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="172"/>
+      <c r="J22" s="175"/>
+      <c r="K22" s="177"/>
+      <c r="L22" s="179"/>
+      <c r="M22" s="172"/>
     </row>
     <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
@@ -5541,12 +5539,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="272"/>
-      <c r="I23" s="261"/>
-      <c r="J23" s="263"/>
-      <c r="K23" s="265"/>
-      <c r="L23" s="267"/>
-      <c r="M23" s="261"/>
+      <c r="H23" s="250"/>
+      <c r="I23" s="174"/>
+      <c r="J23" s="176"/>
+      <c r="K23" s="178"/>
+      <c r="L23" s="180"/>
+      <c r="M23" s="174"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
@@ -5572,7 +5570,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="207" t="s">
+      <c r="H24" s="218" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5615,7 +5613,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="209"/>
+      <c r="H25" s="216"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5656,12 +5654,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="209"/>
-      <c r="I26" s="228"/>
-      <c r="J26" s="231"/>
-      <c r="K26" s="233"/>
-      <c r="L26" s="235"/>
-      <c r="M26" s="236"/>
+      <c r="H26" s="216"/>
+      <c r="I26" s="246"/>
+      <c r="J26" s="251"/>
+      <c r="K26" s="240"/>
+      <c r="L26" s="242"/>
+      <c r="M26" s="244"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5687,12 +5685,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="208"/>
-      <c r="I27" s="229"/>
-      <c r="J27" s="232"/>
-      <c r="K27" s="234"/>
-      <c r="L27" s="230"/>
-      <c r="M27" s="237"/>
+      <c r="H27" s="217"/>
+      <c r="I27" s="247"/>
+      <c r="J27" s="252"/>
+      <c r="K27" s="241"/>
+      <c r="L27" s="243"/>
+      <c r="M27" s="245"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5718,7 +5716,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="207" t="s">
+      <c r="H28" s="218" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5761,7 +5759,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="209"/>
+      <c r="H29" s="216"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5802,7 +5800,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="209"/>
+      <c r="H30" s="216"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5843,7 +5841,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="208"/>
+      <c r="H31" s="217"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5874,7 +5872,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="209" t="s">
+      <c r="H32" s="216" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5918,7 +5916,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="209"/>
+      <c r="H33" s="216"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5960,7 +5958,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="208"/>
+      <c r="H34" s="217"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -6023,11 +6021,22 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="M18:M19"/>
@@ -6038,22 +6047,11 @@
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="H20:H23"/>
     <mergeCell ref="J26:J27"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H28:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6075,13 +6073,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="204" t="s">
+      <c r="B2" s="237" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="205"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="206"/>
-      <c r="F2" s="174" t="s">
+      <c r="C2" s="238"/>
+      <c r="D2" s="238"/>
+      <c r="E2" s="239"/>
+      <c r="F2" s="186" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6098,7 +6096,7 @@
       <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="175"/>
+      <c r="F3" s="187"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
@@ -6284,30 +6282,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="186" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="247" t="s">
+      <c r="C2" s="262" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="248"/>
-      <c r="E2" s="248"/>
-      <c r="F2" s="248"/>
-      <c r="G2" s="248"/>
-      <c r="H2" s="248"/>
-      <c r="I2" s="248"/>
-      <c r="J2" s="248"/>
-      <c r="K2" s="248"/>
-      <c r="L2" s="248"/>
-      <c r="M2" s="248"/>
-      <c r="N2" s="248"/>
-      <c r="O2" s="248"/>
-      <c r="P2" s="248"/>
-      <c r="Q2" s="248"/>
-      <c r="R2" s="249"/>
+      <c r="D2" s="263"/>
+      <c r="E2" s="263"/>
+      <c r="F2" s="263"/>
+      <c r="G2" s="263"/>
+      <c r="H2" s="263"/>
+      <c r="I2" s="263"/>
+      <c r="J2" s="263"/>
+      <c r="K2" s="263"/>
+      <c r="L2" s="263"/>
+      <c r="M2" s="263"/>
+      <c r="N2" s="263"/>
+      <c r="O2" s="263"/>
+      <c r="P2" s="263"/>
+      <c r="Q2" s="263"/>
+      <c r="R2" s="264"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="175"/>
+      <c r="B3" s="187"/>
       <c r="C3" s="118">
         <v>15</v>
       </c>
@@ -6378,13 +6376,13 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="241" t="s">
+      <c r="N4" s="256" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="241"/>
-      <c r="P4" s="241"/>
-      <c r="Q4" s="241"/>
-      <c r="R4" s="242"/>
+      <c r="O4" s="256"/>
+      <c r="P4" s="256"/>
+      <c r="Q4" s="256"/>
+      <c r="R4" s="257"/>
     </row>
     <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
@@ -6398,16 +6396,16 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="243" t="s">
+      <c r="K5" s="258" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="239"/>
-      <c r="M5" s="239"/>
-      <c r="N5" s="239"/>
-      <c r="O5" s="239"/>
-      <c r="P5" s="239"/>
-      <c r="Q5" s="239"/>
-      <c r="R5" s="240"/>
+      <c r="L5" s="254"/>
+      <c r="M5" s="254"/>
+      <c r="N5" s="254"/>
+      <c r="O5" s="254"/>
+      <c r="P5" s="254"/>
+      <c r="Q5" s="254"/>
+      <c r="R5" s="255"/>
     </row>
     <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
@@ -6421,16 +6419,16 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="243" t="s">
+      <c r="K6" s="258" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="239"/>
-      <c r="M6" s="239"/>
-      <c r="N6" s="239"/>
-      <c r="O6" s="239"/>
-      <c r="P6" s="239"/>
-      <c r="Q6" s="239"/>
-      <c r="R6" s="240"/>
+      <c r="L6" s="254"/>
+      <c r="M6" s="254"/>
+      <c r="N6" s="254"/>
+      <c r="O6" s="254"/>
+      <c r="P6" s="254"/>
+      <c r="Q6" s="254"/>
+      <c r="R6" s="255"/>
     </row>
     <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
@@ -6444,39 +6442,39 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="244" t="s">
+      <c r="K7" s="259" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="245"/>
-      <c r="M7" s="245"/>
-      <c r="N7" s="245"/>
-      <c r="O7" s="245"/>
-      <c r="P7" s="245"/>
-      <c r="Q7" s="245"/>
-      <c r="R7" s="246"/>
+      <c r="L7" s="260"/>
+      <c r="M7" s="260"/>
+      <c r="N7" s="260"/>
+      <c r="O7" s="260"/>
+      <c r="P7" s="260"/>
+      <c r="Q7" s="260"/>
+      <c r="R7" s="261"/>
     </row>
     <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="238" t="s">
+      <c r="C8" s="253" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="239"/>
-      <c r="E8" s="239"/>
-      <c r="F8" s="239"/>
-      <c r="G8" s="239"/>
-      <c r="H8" s="239"/>
-      <c r="I8" s="239"/>
-      <c r="J8" s="239"/>
-      <c r="K8" s="239"/>
-      <c r="L8" s="239"/>
-      <c r="M8" s="239"/>
-      <c r="N8" s="239"/>
-      <c r="O8" s="239"/>
-      <c r="P8" s="239"/>
-      <c r="Q8" s="239"/>
-      <c r="R8" s="240"/>
+      <c r="D8" s="254"/>
+      <c r="E8" s="254"/>
+      <c r="F8" s="254"/>
+      <c r="G8" s="254"/>
+      <c r="H8" s="254"/>
+      <c r="I8" s="254"/>
+      <c r="J8" s="254"/>
+      <c r="K8" s="254"/>
+      <c r="L8" s="254"/>
+      <c r="M8" s="254"/>
+      <c r="N8" s="254"/>
+      <c r="O8" s="254"/>
+      <c r="P8" s="254"/>
+      <c r="Q8" s="254"/>
+      <c r="R8" s="255"/>
     </row>
     <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
@@ -6525,7 +6523,7 @@
   <dimension ref="B1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="B17:D17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6690,10 +6688,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="250" t="s">
+      <c r="B2" s="265" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="251"/>
+      <c r="C2" s="266"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6710,7 +6708,7 @@
       <c r="C4" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="252" t="s">
+      <c r="D4" s="267" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6719,21 +6717,21 @@
       <c r="C5" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="253"/>
+      <c r="D5" s="268"/>
     </row>
     <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="254"/>
+      <c r="D6" s="269"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="145"/>
-      <c r="D7" s="255" t="s">
+      <c r="D7" s="270" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6742,14 +6740,14 @@
         <v>142</v>
       </c>
       <c r="C8" s="146"/>
-      <c r="D8" s="256"/>
+      <c r="D8" s="271"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
       <c r="C9" s="146"/>
-      <c r="D9" s="256"/>
+      <c r="D9" s="271"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
@@ -6758,7 +6756,7 @@
       <c r="C10" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="256"/>
+      <c r="D10" s="271"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
@@ -6767,7 +6765,7 @@
       <c r="C11" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="256"/>
+      <c r="D11" s="271"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6777,7 +6775,7 @@
       <c r="C12" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="257"/>
+      <c r="D12" s="272"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
prepared part order for peripherals
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAB9820-1F92-44F9-914C-085480A8E1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FA9720-7A4A-4358-B61B-559CADE1B023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -2011,6 +2011,42 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2050,94 +2086,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2146,17 +2128,56 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2175,27 +2196,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="64" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3258,73 +3258,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="213" t="s">
+      <c r="C3" s="200" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="214"/>
-      <c r="E3" s="214"/>
-      <c r="F3" s="214"/>
-      <c r="G3" s="215"/>
-      <c r="H3" s="210" t="s">
+      <c r="D3" s="201"/>
+      <c r="E3" s="201"/>
+      <c r="F3" s="201"/>
+      <c r="G3" s="202"/>
+      <c r="H3" s="197" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="211"/>
-      <c r="J3" s="212"/>
-      <c r="K3" s="210" t="s">
+      <c r="I3" s="198"/>
+      <c r="J3" s="199"/>
+      <c r="K3" s="197" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="211"/>
-      <c r="M3" s="211"/>
-      <c r="N3" s="197" t="s">
+      <c r="L3" s="198"/>
+      <c r="M3" s="198"/>
+      <c r="N3" s="209" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="198"/>
-      <c r="P3" s="199"/>
+      <c r="O3" s="210"/>
+      <c r="P3" s="211"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="191" t="s">
+      <c r="S3" s="203" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="192"/>
-      <c r="U3" s="192"/>
-      <c r="V3" s="192"/>
-      <c r="W3" s="192"/>
-      <c r="X3" s="192"/>
-      <c r="Y3" s="192"/>
-      <c r="Z3" s="193"/>
-      <c r="AA3" s="194" t="s">
+      <c r="T3" s="204"/>
+      <c r="U3" s="204"/>
+      <c r="V3" s="204"/>
+      <c r="W3" s="204"/>
+      <c r="X3" s="204"/>
+      <c r="Y3" s="204"/>
+      <c r="Z3" s="205"/>
+      <c r="AA3" s="206" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="195"/>
-      <c r="AC3" s="195"/>
-      <c r="AD3" s="195"/>
-      <c r="AE3" s="195"/>
-      <c r="AF3" s="195"/>
-      <c r="AG3" s="195"/>
-      <c r="AH3" s="196"/>
+      <c r="AB3" s="207"/>
+      <c r="AC3" s="207"/>
+      <c r="AD3" s="207"/>
+      <c r="AE3" s="207"/>
+      <c r="AF3" s="207"/>
+      <c r="AG3" s="207"/>
+      <c r="AH3" s="208"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="202" t="s">
+      <c r="B5" s="214" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="200" t="s">
+      <c r="C5" s="212" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="200"/>
-      <c r="E5" s="200"/>
-      <c r="F5" s="200"/>
-      <c r="G5" s="200"/>
-      <c r="H5" s="200"/>
-      <c r="I5" s="200"/>
-      <c r="J5" s="201"/>
+      <c r="D5" s="212"/>
+      <c r="E5" s="212"/>
+      <c r="F5" s="212"/>
+      <c r="G5" s="212"/>
+      <c r="H5" s="212"/>
+      <c r="I5" s="212"/>
+      <c r="J5" s="213"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="203"/>
+      <c r="B6" s="215"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3354,16 +3354,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="204" t="s">
+      <c r="C7" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="205"/>
-      <c r="E7" s="205"/>
-      <c r="F7" s="205"/>
-      <c r="G7" s="205"/>
-      <c r="H7" s="205"/>
-      <c r="I7" s="205"/>
-      <c r="J7" s="206"/>
+      <c r="D7" s="192"/>
+      <c r="E7" s="192"/>
+      <c r="F7" s="192"/>
+      <c r="G7" s="192"/>
+      <c r="H7" s="192"/>
+      <c r="I7" s="192"/>
+      <c r="J7" s="193"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3373,25 +3373,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="207" t="s">
+      <c r="G8" s="194" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="208"/>
-      <c r="I8" s="208"/>
-      <c r="J8" s="209"/>
+      <c r="H8" s="195"/>
+      <c r="I8" s="195"/>
+      <c r="J8" s="196"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="AA3:AH3"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="C7:J7"/>
     <mergeCell ref="G8:J8"/>
     <mergeCell ref="K3:M3"/>
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="C3:G3"/>
-    <mergeCell ref="S3:Z3"/>
-    <mergeCell ref="AA3:AH3"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3419,25 +3419,25 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="216" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="239"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="218"/>
       <c r="H2" s="186" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="237" t="s">
+      <c r="J2" s="216" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="238"/>
-      <c r="L2" s="238"/>
+      <c r="K2" s="217"/>
+      <c r="L2" s="217"/>
       <c r="M2" s="186" t="s">
         <v>112</v>
       </c>
@@ -3502,7 +3502,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="218" t="s">
+      <c r="H4" s="219" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3548,7 +3548,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="217"/>
+      <c r="H5" s="220"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3592,25 +3592,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="216" t="s">
+      <c r="H6" s="221" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="220" t="s">
+      <c r="J6" s="222" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="229" t="s">
+      <c r="K6" s="224" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="226" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="231" t="s">
+      <c r="M6" s="234" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="234" t="s">
+      <c r="N6" s="228" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3638,15 +3638,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="216"/>
+      <c r="H7" s="221"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="220"/>
-      <c r="K7" s="229"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="224"/>
       <c r="L7" s="226"/>
-      <c r="M7" s="232"/>
-      <c r="N7" s="234"/>
+      <c r="M7" s="235"/>
+      <c r="N7" s="228"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3672,15 +3672,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="216"/>
+      <c r="H8" s="221"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="220"/>
-      <c r="K8" s="229"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="224"/>
       <c r="L8" s="226"/>
-      <c r="M8" s="232"/>
-      <c r="N8" s="234"/>
+      <c r="M8" s="235"/>
+      <c r="N8" s="228"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3706,15 +3706,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="216"/>
+      <c r="H9" s="221"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="220"/>
-      <c r="K9" s="229"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="224"/>
       <c r="L9" s="226"/>
-      <c r="M9" s="232"/>
-      <c r="N9" s="234"/>
+      <c r="M9" s="235"/>
+      <c r="N9" s="228"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3740,15 +3740,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="216"/>
+      <c r="H10" s="221"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="220"/>
-      <c r="K10" s="229"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="224"/>
       <c r="L10" s="226"/>
-      <c r="M10" s="232"/>
-      <c r="N10" s="234"/>
+      <c r="M10" s="235"/>
+      <c r="N10" s="228"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3774,15 +3774,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="217"/>
+      <c r="H11" s="220"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="221"/>
-      <c r="K11" s="230"/>
+      <c r="J11" s="223"/>
+      <c r="K11" s="225"/>
       <c r="L11" s="227"/>
-      <c r="M11" s="233"/>
-      <c r="N11" s="235"/>
+      <c r="M11" s="236"/>
+      <c r="N11" s="229"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3808,25 +3808,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="218" t="s">
+      <c r="H12" s="219" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="219" t="s">
+      <c r="J12" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="228" t="s">
+      <c r="K12" s="231" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="225" t="s">
+      <c r="L12" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="218" t="s">
+      <c r="M12" s="219" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="236" t="s">
+      <c r="N12" s="233" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3854,15 +3854,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="216"/>
+      <c r="H13" s="221"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="229"/>
+      <c r="J13" s="222"/>
+      <c r="K13" s="224"/>
       <c r="L13" s="226"/>
-      <c r="M13" s="216"/>
-      <c r="N13" s="234"/>
+      <c r="M13" s="221"/>
+      <c r="N13" s="228"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3888,15 +3888,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="216"/>
+      <c r="H14" s="221"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="220"/>
-      <c r="K14" s="229"/>
+      <c r="J14" s="222"/>
+      <c r="K14" s="224"/>
       <c r="L14" s="226"/>
-      <c r="M14" s="216"/>
-      <c r="N14" s="234"/>
+      <c r="M14" s="221"/>
+      <c r="N14" s="228"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3922,15 +3922,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="217"/>
+      <c r="H15" s="220"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="221"/>
-      <c r="K15" s="230"/>
+      <c r="J15" s="223"/>
+      <c r="K15" s="225"/>
       <c r="L15" s="227"/>
-      <c r="M15" s="217"/>
-      <c r="N15" s="235"/>
+      <c r="M15" s="220"/>
+      <c r="N15" s="229"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3956,22 +3956,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="218" t="s">
+      <c r="H16" s="219" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="219" t="s">
+      <c r="J16" s="230" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="222" t="s">
+      <c r="K16" s="237" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="225" t="s">
+      <c r="L16" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="218" t="s">
+      <c r="M16" s="219" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -4002,14 +4002,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="216"/>
+      <c r="H17" s="221"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="220"/>
-      <c r="K17" s="223"/>
+      <c r="J17" s="222"/>
+      <c r="K17" s="238"/>
       <c r="L17" s="226"/>
-      <c r="M17" s="216"/>
+      <c r="M17" s="221"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4038,14 +4038,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="216"/>
+      <c r="H18" s="221"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="220"/>
-      <c r="K18" s="223"/>
+      <c r="J18" s="222"/>
+      <c r="K18" s="238"/>
       <c r="L18" s="226"/>
-      <c r="M18" s="216"/>
+      <c r="M18" s="221"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4074,14 +4074,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="217"/>
+      <c r="H19" s="220"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="221"/>
-      <c r="K19" s="224"/>
+      <c r="J19" s="223"/>
+      <c r="K19" s="239"/>
       <c r="L19" s="227"/>
-      <c r="M19" s="217"/>
+      <c r="M19" s="220"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4111,22 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="218" t="s">
+      <c r="H20" s="219" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="219" t="s">
+      <c r="J20" s="230" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="228" t="s">
+      <c r="K20" s="231" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="225" t="s">
+      <c r="L20" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="231" t="s">
+      <c r="M20" s="234" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4157,14 +4157,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="216"/>
+      <c r="H21" s="221"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="220"/>
-      <c r="K21" s="229"/>
+      <c r="J21" s="222"/>
+      <c r="K21" s="224"/>
       <c r="L21" s="226"/>
-      <c r="M21" s="232"/>
+      <c r="M21" s="235"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4193,14 +4193,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="216"/>
+      <c r="H22" s="221"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="220"/>
-      <c r="K22" s="229"/>
+      <c r="J22" s="222"/>
+      <c r="K22" s="224"/>
       <c r="L22" s="226"/>
-      <c r="M22" s="232"/>
+      <c r="M22" s="235"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4229,14 +4229,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="217"/>
+      <c r="H23" s="220"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="221"/>
-      <c r="K23" s="230"/>
+      <c r="J23" s="223"/>
+      <c r="K23" s="225"/>
       <c r="L23" s="227"/>
-      <c r="M23" s="233"/>
+      <c r="M23" s="236"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4265,7 +4265,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="218" t="s">
+      <c r="H24" s="219" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4311,7 +4311,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="216"/>
+      <c r="H25" s="221"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4355,7 +4355,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="216"/>
+      <c r="H26" s="221"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4387,7 +4387,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="217"/>
+      <c r="H27" s="220"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4419,7 +4419,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="218" t="s">
+      <c r="H28" s="219" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4465,7 +4465,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="216"/>
+      <c r="H29" s="221"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4509,7 +4509,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="216"/>
+      <c r="H30" s="221"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4553,7 +4553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="217"/>
+      <c r="H31" s="220"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4585,7 +4585,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="216" t="s">
+      <c r="H32" s="221" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4632,7 +4632,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="216"/>
+      <c r="H33" s="221"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4677,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="217"/>
+      <c r="H34" s="220"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4734,17 +4734,19 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="K16:K19"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M19"/>
+    <mergeCell ref="H20:H23"/>
+    <mergeCell ref="J20:J23"/>
+    <mergeCell ref="K20:K23"/>
+    <mergeCell ref="L20:L23"/>
+    <mergeCell ref="M20:M23"/>
     <mergeCell ref="N6:N11"/>
     <mergeCell ref="H12:H15"/>
     <mergeCell ref="J12:J15"/>
@@ -4753,19 +4755,17 @@
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
     <mergeCell ref="M6:M11"/>
-    <mergeCell ref="K16:K19"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M19"/>
-    <mergeCell ref="H20:H23"/>
-    <mergeCell ref="J20:J23"/>
-    <mergeCell ref="K20:K23"/>
-    <mergeCell ref="L20:L23"/>
-    <mergeCell ref="M20:M23"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4790,25 +4790,25 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="216" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="238"/>
-      <c r="F2" s="238"/>
-      <c r="G2" s="239"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="217"/>
+      <c r="G2" s="218"/>
       <c r="H2" s="186" t="s">
         <v>54</v>
       </c>
       <c r="I2" s="186" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="237" t="s">
+      <c r="J2" s="216" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="238"/>
-      <c r="L2" s="238"/>
+      <c r="K2" s="217"/>
+      <c r="L2" s="217"/>
       <c r="M2" s="186" t="s">
         <v>33</v>
       </c>
@@ -4869,7 +4869,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="218" t="s">
+      <c r="H4" s="219" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4912,7 +4912,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="217"/>
+      <c r="H5" s="220"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4953,20 +4953,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="216" t="s">
+      <c r="H6" s="221" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="173"/>
-      <c r="J6" s="220" t="s">
+      <c r="J6" s="222" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="229" t="s">
+      <c r="K6" s="224" t="s">
         <v>69</v>
       </c>
       <c r="L6" s="226" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="234" t="s">
+      <c r="M6" s="228" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4994,14 +4994,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="216"/>
+      <c r="H7" s="221"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="220"/>
-      <c r="K7" s="229"/>
+      <c r="J7" s="222"/>
+      <c r="K7" s="224"/>
       <c r="L7" s="226"/>
-      <c r="M7" s="234"/>
+      <c r="M7" s="228"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5027,14 +5027,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="216"/>
+      <c r="H8" s="221"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="220"/>
-      <c r="K8" s="229"/>
+      <c r="J8" s="222"/>
+      <c r="K8" s="224"/>
       <c r="L8" s="226"/>
-      <c r="M8" s="234"/>
+      <c r="M8" s="228"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5060,12 +5060,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="216"/>
+      <c r="H9" s="221"/>
       <c r="I9" s="173"/>
-      <c r="J9" s="220"/>
-      <c r="K9" s="229"/>
+      <c r="J9" s="222"/>
+      <c r="K9" s="224"/>
       <c r="L9" s="226"/>
-      <c r="M9" s="234"/>
+      <c r="M9" s="228"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5091,14 +5091,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="216"/>
+      <c r="H10" s="221"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="220"/>
-      <c r="K10" s="229"/>
+      <c r="J10" s="222"/>
+      <c r="K10" s="224"/>
       <c r="L10" s="226"/>
-      <c r="M10" s="234"/>
+      <c r="M10" s="228"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5124,12 +5124,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="217"/>
+      <c r="H11" s="220"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="221"/>
-      <c r="K11" s="230"/>
+      <c r="J11" s="223"/>
+      <c r="K11" s="225"/>
       <c r="L11" s="227"/>
-      <c r="M11" s="235"/>
+      <c r="M11" s="229"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5155,22 +5155,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="218" t="s">
+      <c r="H12" s="219" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="219" t="s">
+      <c r="J12" s="230" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="228" t="s">
+      <c r="K12" s="231" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="225" t="s">
+      <c r="L12" s="232" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="236" t="s">
+      <c r="M12" s="233" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5198,14 +5198,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="216"/>
+      <c r="H13" s="221"/>
       <c r="I13" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="220"/>
-      <c r="K13" s="229"/>
+      <c r="J13" s="222"/>
+      <c r="K13" s="224"/>
       <c r="L13" s="226"/>
-      <c r="M13" s="234"/>
+      <c r="M13" s="228"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5231,12 +5231,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="216"/>
+      <c r="H14" s="221"/>
       <c r="I14" s="105"/>
-      <c r="J14" s="220"/>
-      <c r="K14" s="229"/>
+      <c r="J14" s="222"/>
+      <c r="K14" s="224"/>
       <c r="L14" s="226"/>
-      <c r="M14" s="234"/>
+      <c r="M14" s="228"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5262,12 +5262,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="217"/>
+      <c r="H15" s="220"/>
       <c r="I15" s="105"/>
-      <c r="J15" s="221"/>
-      <c r="K15" s="230"/>
+      <c r="J15" s="223"/>
+      <c r="K15" s="225"/>
       <c r="L15" s="227"/>
-      <c r="M15" s="235"/>
+      <c r="M15" s="229"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5293,19 +5293,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="218" t="s">
+      <c r="H16" s="219" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="219" t="s">
+      <c r="J16" s="230" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="222" t="s">
+      <c r="K16" s="237" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="225" t="s">
+      <c r="L16" s="232" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5336,12 +5336,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="216"/>
+      <c r="H17" s="221"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="220"/>
-      <c r="K17" s="223"/>
+      <c r="J17" s="222"/>
+      <c r="K17" s="238"/>
       <c r="L17" s="226"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
@@ -5371,12 +5371,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="216"/>
-      <c r="I18" s="246"/>
-      <c r="J18" s="220"/>
-      <c r="K18" s="223"/>
+      <c r="H18" s="221"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="222"/>
+      <c r="K18" s="238"/>
       <c r="L18" s="226"/>
-      <c r="M18" s="246"/>
+      <c r="M18" s="240"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5402,12 +5402,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="217"/>
-      <c r="I19" s="247"/>
-      <c r="J19" s="221"/>
-      <c r="K19" s="224"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="241"/>
+      <c r="J19" s="223"/>
+      <c r="K19" s="239"/>
       <c r="L19" s="227"/>
-      <c r="M19" s="247"/>
+      <c r="M19" s="241"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5434,7 +5434,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="248" t="s">
+      <c r="H20" s="242" t="s">
         <v>179</v>
       </c>
       <c r="I20" s="182" t="s">
@@ -5477,7 +5477,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="249"/>
+      <c r="H21" s="243"/>
       <c r="I21" s="172"/>
       <c r="J21" s="175"/>
       <c r="K21" s="177"/>
@@ -5508,7 +5508,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="249"/>
+      <c r="H22" s="243"/>
       <c r="I22" s="172"/>
       <c r="J22" s="175"/>
       <c r="K22" s="177"/>
@@ -5539,7 +5539,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="250"/>
+      <c r="H23" s="244"/>
       <c r="I23" s="174"/>
       <c r="J23" s="176"/>
       <c r="K23" s="178"/>
@@ -5570,7 +5570,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="218" t="s">
+      <c r="H24" s="219" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5613,7 +5613,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="216"/>
+      <c r="H25" s="221"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5654,12 +5654,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="216"/>
-      <c r="I26" s="246"/>
-      <c r="J26" s="251"/>
-      <c r="K26" s="240"/>
-      <c r="L26" s="242"/>
-      <c r="M26" s="244"/>
+      <c r="H26" s="221"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="245"/>
+      <c r="K26" s="247"/>
+      <c r="L26" s="249"/>
+      <c r="M26" s="251"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5685,12 +5685,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="217"/>
-      <c r="I27" s="247"/>
-      <c r="J27" s="252"/>
-      <c r="K27" s="241"/>
-      <c r="L27" s="243"/>
-      <c r="M27" s="245"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="241"/>
+      <c r="J27" s="246"/>
+      <c r="K27" s="248"/>
+      <c r="L27" s="250"/>
+      <c r="M27" s="252"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5716,7 +5716,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="218" t="s">
+      <c r="H28" s="219" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5759,7 +5759,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="216"/>
+      <c r="H29" s="221"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5800,7 +5800,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="216"/>
+      <c r="H30" s="221"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5841,7 +5841,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="217"/>
+      <c r="H31" s="220"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5872,7 +5872,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="216" t="s">
+      <c r="H32" s="221" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5916,7 +5916,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="216"/>
+      <c r="H33" s="221"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5958,7 +5958,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="217"/>
+      <c r="H34" s="220"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -6021,22 +6021,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="M18:M19"/>
@@ -6052,6 +6036,22 @@
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="H28:H31"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6073,12 +6073,12 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="216" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="239"/>
+      <c r="C2" s="217"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="218"/>
       <c r="F2" s="186" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
updated order estimate, fixed minor schematic opcode oopsies
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FA9720-7A4A-4358-B61B-559CADE1B023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E438F04A-2EF9-4FAC-B9C8-6B01D22417BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="182">
   <si>
     <t>MODE B</t>
   </si>
@@ -1951,9 +1951,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2256,6 +2253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2611,19 +2611,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="183" t="s">
+      <c r="B2" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="184"/>
-      <c r="F2" s="185"/>
-      <c r="G2" s="188" t="s">
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="187" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="189"/>
-      <c r="I2" s="190"/>
-      <c r="J2" s="186" t="s">
+      <c r="H2" s="188"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="185" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       <c r="I3" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="187"/>
+      <c r="J3" s="186"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
@@ -3258,73 +3258,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="200" t="s">
+      <c r="C3" s="199" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="201"/>
-      <c r="E3" s="201"/>
-      <c r="F3" s="201"/>
-      <c r="G3" s="202"/>
-      <c r="H3" s="197" t="s">
+      <c r="D3" s="200"/>
+      <c r="E3" s="200"/>
+      <c r="F3" s="200"/>
+      <c r="G3" s="201"/>
+      <c r="H3" s="196" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="198"/>
-      <c r="J3" s="199"/>
-      <c r="K3" s="197" t="s">
+      <c r="I3" s="197"/>
+      <c r="J3" s="198"/>
+      <c r="K3" s="196" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="198"/>
-      <c r="M3" s="198"/>
-      <c r="N3" s="209" t="s">
+      <c r="L3" s="197"/>
+      <c r="M3" s="197"/>
+      <c r="N3" s="208" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="210"/>
-      <c r="P3" s="211"/>
+      <c r="O3" s="209"/>
+      <c r="P3" s="210"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="203" t="s">
+      <c r="S3" s="202" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="204"/>
-      <c r="U3" s="204"/>
-      <c r="V3" s="204"/>
-      <c r="W3" s="204"/>
-      <c r="X3" s="204"/>
-      <c r="Y3" s="204"/>
-      <c r="Z3" s="205"/>
-      <c r="AA3" s="206" t="s">
+      <c r="T3" s="203"/>
+      <c r="U3" s="203"/>
+      <c r="V3" s="203"/>
+      <c r="W3" s="203"/>
+      <c r="X3" s="203"/>
+      <c r="Y3" s="203"/>
+      <c r="Z3" s="204"/>
+      <c r="AA3" s="205" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="207"/>
-      <c r="AC3" s="207"/>
-      <c r="AD3" s="207"/>
-      <c r="AE3" s="207"/>
-      <c r="AF3" s="207"/>
-      <c r="AG3" s="207"/>
-      <c r="AH3" s="208"/>
+      <c r="AB3" s="206"/>
+      <c r="AC3" s="206"/>
+      <c r="AD3" s="206"/>
+      <c r="AE3" s="206"/>
+      <c r="AF3" s="206"/>
+      <c r="AG3" s="206"/>
+      <c r="AH3" s="207"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="214" t="s">
+      <c r="B5" s="213" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="212" t="s">
+      <c r="C5" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="212"/>
-      <c r="E5" s="212"/>
-      <c r="F5" s="212"/>
-      <c r="G5" s="212"/>
-      <c r="H5" s="212"/>
-      <c r="I5" s="212"/>
-      <c r="J5" s="213"/>
+      <c r="D5" s="211"/>
+      <c r="E5" s="211"/>
+      <c r="F5" s="211"/>
+      <c r="G5" s="211"/>
+      <c r="H5" s="211"/>
+      <c r="I5" s="211"/>
+      <c r="J5" s="212"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="215"/>
+      <c r="B6" s="214"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3354,16 +3354,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="191" t="s">
+      <c r="C7" s="190" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="192"/>
-      <c r="E7" s="192"/>
-      <c r="F7" s="192"/>
-      <c r="G7" s="192"/>
-      <c r="H7" s="192"/>
-      <c r="I7" s="192"/>
-      <c r="J7" s="193"/>
+      <c r="D7" s="191"/>
+      <c r="E7" s="191"/>
+      <c r="F7" s="191"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="191"/>
+      <c r="I7" s="191"/>
+      <c r="J7" s="192"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3373,12 +3373,12 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="194" t="s">
+      <c r="G8" s="193" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="195"/>
-      <c r="I8" s="195"/>
-      <c r="J8" s="196"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="194"/>
+      <c r="J8" s="195"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3419,29 +3419,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="215" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="186" t="s">
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="185" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="186" t="s">
+      <c r="I2" s="185" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="216" t="s">
+      <c r="J2" s="215" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="217"/>
-      <c r="L2" s="217"/>
-      <c r="M2" s="186" t="s">
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="185" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="186" t="s">
+      <c r="N2" s="185" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3464,8 +3464,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -3475,8 +3475,8 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="187"/>
-      <c r="N3" s="187"/>
+      <c r="M3" s="186"/>
+      <c r="N3" s="186"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -3502,7 +3502,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="219" t="s">
+      <c r="H4" s="218" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3548,7 +3548,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="220"/>
+      <c r="H5" s="219"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3592,25 +3592,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="221" t="s">
+      <c r="H6" s="220" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="222" t="s">
+      <c r="J6" s="221" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="224" t="s">
+      <c r="K6" s="223" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="226" t="s">
+      <c r="L6" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="234" t="s">
+      <c r="M6" s="233" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="228" t="s">
+      <c r="N6" s="227" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3638,15 +3638,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="221"/>
+      <c r="H7" s="220"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="222"/>
-      <c r="K7" s="224"/>
-      <c r="L7" s="226"/>
-      <c r="M7" s="235"/>
-      <c r="N7" s="228"/>
+      <c r="J7" s="221"/>
+      <c r="K7" s="223"/>
+      <c r="L7" s="225"/>
+      <c r="M7" s="234"/>
+      <c r="N7" s="227"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3672,15 +3672,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="221"/>
+      <c r="H8" s="220"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="222"/>
-      <c r="K8" s="224"/>
-      <c r="L8" s="226"/>
-      <c r="M8" s="235"/>
-      <c r="N8" s="228"/>
+      <c r="J8" s="221"/>
+      <c r="K8" s="223"/>
+      <c r="L8" s="225"/>
+      <c r="M8" s="234"/>
+      <c r="N8" s="227"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3706,15 +3706,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="221"/>
+      <c r="H9" s="220"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="222"/>
-      <c r="K9" s="224"/>
-      <c r="L9" s="226"/>
-      <c r="M9" s="235"/>
-      <c r="N9" s="228"/>
+      <c r="J9" s="221"/>
+      <c r="K9" s="223"/>
+      <c r="L9" s="225"/>
+      <c r="M9" s="234"/>
+      <c r="N9" s="227"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3740,15 +3740,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="221"/>
+      <c r="H10" s="220"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="222"/>
-      <c r="K10" s="224"/>
-      <c r="L10" s="226"/>
-      <c r="M10" s="235"/>
-      <c r="N10" s="228"/>
+      <c r="J10" s="221"/>
+      <c r="K10" s="223"/>
+      <c r="L10" s="225"/>
+      <c r="M10" s="234"/>
+      <c r="N10" s="227"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3774,15 +3774,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="220"/>
+      <c r="H11" s="219"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="223"/>
-      <c r="K11" s="225"/>
-      <c r="L11" s="227"/>
-      <c r="M11" s="236"/>
-      <c r="N11" s="229"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="224"/>
+      <c r="L11" s="226"/>
+      <c r="M11" s="235"/>
+      <c r="N11" s="228"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3808,25 +3808,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="219" t="s">
+      <c r="H12" s="218" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="230" t="s">
+      <c r="J12" s="229" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="231" t="s">
+      <c r="K12" s="230" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="232" t="s">
+      <c r="L12" s="231" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="219" t="s">
+      <c r="M12" s="218" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="233" t="s">
+      <c r="N12" s="232" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3854,15 +3854,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="221"/>
+      <c r="H13" s="220"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="222"/>
-      <c r="K13" s="224"/>
-      <c r="L13" s="226"/>
-      <c r="M13" s="221"/>
-      <c r="N13" s="228"/>
+      <c r="J13" s="221"/>
+      <c r="K13" s="223"/>
+      <c r="L13" s="225"/>
+      <c r="M13" s="220"/>
+      <c r="N13" s="227"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3888,15 +3888,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="221"/>
+      <c r="H14" s="220"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="222"/>
-      <c r="K14" s="224"/>
-      <c r="L14" s="226"/>
-      <c r="M14" s="221"/>
-      <c r="N14" s="228"/>
+      <c r="J14" s="221"/>
+      <c r="K14" s="223"/>
+      <c r="L14" s="225"/>
+      <c r="M14" s="220"/>
+      <c r="N14" s="227"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3922,15 +3922,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="220"/>
+      <c r="H15" s="219"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="223"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="227"/>
-      <c r="M15" s="220"/>
-      <c r="N15" s="229"/>
+      <c r="J15" s="222"/>
+      <c r="K15" s="224"/>
+      <c r="L15" s="226"/>
+      <c r="M15" s="219"/>
+      <c r="N15" s="228"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3956,22 +3956,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="219" t="s">
+      <c r="H16" s="218" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="230" t="s">
+      <c r="J16" s="229" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="237" t="s">
+      <c r="K16" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="232" t="s">
+      <c r="L16" s="231" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="219" t="s">
+      <c r="M16" s="218" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -4002,14 +4002,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="221"/>
+      <c r="H17" s="220"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="222"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="226"/>
-      <c r="M17" s="221"/>
+      <c r="J17" s="221"/>
+      <c r="K17" s="237"/>
+      <c r="L17" s="225"/>
+      <c r="M17" s="220"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4038,14 +4038,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="221"/>
+      <c r="H18" s="220"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="222"/>
-      <c r="K18" s="238"/>
-      <c r="L18" s="226"/>
-      <c r="M18" s="221"/>
+      <c r="J18" s="221"/>
+      <c r="K18" s="237"/>
+      <c r="L18" s="225"/>
+      <c r="M18" s="220"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4074,14 +4074,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="220"/>
+      <c r="H19" s="219"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="223"/>
-      <c r="K19" s="239"/>
-      <c r="L19" s="227"/>
-      <c r="M19" s="220"/>
+      <c r="J19" s="222"/>
+      <c r="K19" s="238"/>
+      <c r="L19" s="226"/>
+      <c r="M19" s="219"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4111,22 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="219" t="s">
+      <c r="H20" s="218" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="230" t="s">
+      <c r="J20" s="229" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="231" t="s">
+      <c r="K20" s="230" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="232" t="s">
+      <c r="L20" s="231" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="234" t="s">
+      <c r="M20" s="233" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4157,14 +4157,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="221"/>
+      <c r="H21" s="220"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="222"/>
-      <c r="K21" s="224"/>
-      <c r="L21" s="226"/>
-      <c r="M21" s="235"/>
+      <c r="J21" s="221"/>
+      <c r="K21" s="223"/>
+      <c r="L21" s="225"/>
+      <c r="M21" s="234"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4193,14 +4193,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="221"/>
+      <c r="H22" s="220"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="222"/>
-      <c r="K22" s="224"/>
-      <c r="L22" s="226"/>
-      <c r="M22" s="235"/>
+      <c r="J22" s="221"/>
+      <c r="K22" s="223"/>
+      <c r="L22" s="225"/>
+      <c r="M22" s="234"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4229,14 +4229,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="220"/>
+      <c r="H23" s="219"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="223"/>
-      <c r="K23" s="225"/>
-      <c r="L23" s="227"/>
-      <c r="M23" s="236"/>
+      <c r="J23" s="222"/>
+      <c r="K23" s="224"/>
+      <c r="L23" s="226"/>
+      <c r="M23" s="235"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4265,7 +4265,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="219" t="s">
+      <c r="H24" s="218" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4311,7 +4311,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="221"/>
+      <c r="H25" s="220"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4355,7 +4355,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="221"/>
+      <c r="H26" s="220"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4387,7 +4387,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="220"/>
+      <c r="H27" s="219"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4419,7 +4419,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="219" t="s">
+      <c r="H28" s="218" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4465,7 +4465,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="221"/>
+      <c r="H29" s="220"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4509,7 +4509,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="221"/>
+      <c r="H30" s="220"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4553,7 +4553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="220"/>
+      <c r="H31" s="219"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4585,7 +4585,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="221" t="s">
+      <c r="H32" s="220" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4632,7 +4632,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="221"/>
+      <c r="H33" s="220"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4677,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="220"/>
+      <c r="H34" s="219"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4790,26 +4790,26 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="215" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="218"/>
-      <c r="H2" s="186" t="s">
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="216"/>
+      <c r="F2" s="216"/>
+      <c r="G2" s="217"/>
+      <c r="H2" s="185" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="186" t="s">
+      <c r="I2" s="185" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="216" t="s">
+      <c r="J2" s="215" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="217"/>
-      <c r="L2" s="217"/>
-      <c r="M2" s="186" t="s">
+      <c r="K2" s="216"/>
+      <c r="L2" s="216"/>
+      <c r="M2" s="185" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4832,8 +4832,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="187"/>
-      <c r="I3" s="187"/>
+      <c r="H3" s="186"/>
+      <c r="I3" s="186"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="187"/>
+      <c r="M3" s="186"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -4869,7 +4869,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="219" t="s">
+      <c r="H4" s="218" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4912,7 +4912,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="220"/>
+      <c r="H5" s="219"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4953,20 +4953,20 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="221" t="s">
+      <c r="H6" s="220" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="173"/>
-      <c r="J6" s="222" t="s">
+      <c r="I6" s="172"/>
+      <c r="J6" s="221" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="224" t="s">
+      <c r="K6" s="223" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="226" t="s">
+      <c r="L6" s="225" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="228" t="s">
+      <c r="M6" s="227" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4994,14 +4994,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="221"/>
+      <c r="H7" s="220"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="222"/>
-      <c r="K7" s="224"/>
-      <c r="L7" s="226"/>
-      <c r="M7" s="228"/>
+      <c r="J7" s="221"/>
+      <c r="K7" s="223"/>
+      <c r="L7" s="225"/>
+      <c r="M7" s="227"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5027,14 +5027,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="221"/>
+      <c r="H8" s="220"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="222"/>
-      <c r="K8" s="224"/>
-      <c r="L8" s="226"/>
-      <c r="M8" s="228"/>
+      <c r="J8" s="221"/>
+      <c r="K8" s="223"/>
+      <c r="L8" s="225"/>
+      <c r="M8" s="227"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5060,12 +5060,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="221"/>
-      <c r="I9" s="173"/>
-      <c r="J9" s="222"/>
-      <c r="K9" s="224"/>
-      <c r="L9" s="226"/>
-      <c r="M9" s="228"/>
+      <c r="H9" s="220"/>
+      <c r="I9" s="172"/>
+      <c r="J9" s="221"/>
+      <c r="K9" s="223"/>
+      <c r="L9" s="225"/>
+      <c r="M9" s="227"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5091,14 +5091,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="221"/>
+      <c r="H10" s="220"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="222"/>
-      <c r="K10" s="224"/>
-      <c r="L10" s="226"/>
-      <c r="M10" s="228"/>
+      <c r="J10" s="221"/>
+      <c r="K10" s="223"/>
+      <c r="L10" s="225"/>
+      <c r="M10" s="227"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5124,12 +5124,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="220"/>
+      <c r="H11" s="219"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="223"/>
-      <c r="K11" s="225"/>
-      <c r="L11" s="227"/>
-      <c r="M11" s="229"/>
+      <c r="J11" s="222"/>
+      <c r="K11" s="224"/>
+      <c r="L11" s="226"/>
+      <c r="M11" s="228"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5155,22 +5155,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="219" t="s">
+      <c r="H12" s="218" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="230" t="s">
+      <c r="J12" s="229" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="231" t="s">
+      <c r="K12" s="230" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="232" t="s">
+      <c r="L12" s="231" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="233" t="s">
+      <c r="M12" s="232" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5198,14 +5198,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="221"/>
-      <c r="I13" s="171" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="222"/>
-      <c r="K13" s="224"/>
-      <c r="L13" s="226"/>
-      <c r="M13" s="228"/>
+      <c r="H13" s="220"/>
+      <c r="I13" s="239"/>
+      <c r="J13" s="221"/>
+      <c r="K13" s="223"/>
+      <c r="L13" s="225"/>
+      <c r="M13" s="227"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5231,12 +5229,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="221"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="222"/>
-      <c r="K14" s="224"/>
-      <c r="L14" s="226"/>
-      <c r="M14" s="228"/>
+      <c r="H14" s="220"/>
+      <c r="I14" s="272"/>
+      <c r="J14" s="221"/>
+      <c r="K14" s="223"/>
+      <c r="L14" s="225"/>
+      <c r="M14" s="227"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5262,12 +5260,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="220"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="223"/>
-      <c r="K15" s="225"/>
-      <c r="L15" s="227"/>
-      <c r="M15" s="229"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="240"/>
+      <c r="J15" s="222"/>
+      <c r="K15" s="224"/>
+      <c r="L15" s="226"/>
+      <c r="M15" s="228"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5293,19 +5291,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="219" t="s">
+      <c r="H16" s="218" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="230" t="s">
+      <c r="J16" s="229" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="237" t="s">
+      <c r="K16" s="236" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="232" t="s">
+      <c r="L16" s="231" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5336,13 +5334,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="221"/>
+      <c r="H17" s="220"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="222"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="226"/>
+      <c r="J17" s="221"/>
+      <c r="K17" s="237"/>
+      <c r="L17" s="225"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
       </c>
@@ -5371,12 +5369,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="221"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="222"/>
-      <c r="K18" s="238"/>
-      <c r="L18" s="226"/>
-      <c r="M18" s="240"/>
+      <c r="H18" s="220"/>
+      <c r="I18" s="239"/>
+      <c r="J18" s="221"/>
+      <c r="K18" s="237"/>
+      <c r="L18" s="225"/>
+      <c r="M18" s="239"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5402,12 +5400,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="220"/>
-      <c r="I19" s="241"/>
-      <c r="J19" s="223"/>
-      <c r="K19" s="239"/>
-      <c r="L19" s="227"/>
-      <c r="M19" s="241"/>
+      <c r="H19" s="219"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="222"/>
+      <c r="K19" s="238"/>
+      <c r="L19" s="226"/>
+      <c r="M19" s="240"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5434,10 +5432,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="242" t="s">
+      <c r="H20" s="241" t="s">
         <v>179</v>
       </c>
-      <c r="I20" s="182" t="s">
+      <c r="I20" s="181" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="67" t="s">
@@ -5449,7 +5447,7 @@
       <c r="L20" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="181" t="s">
+      <c r="M20" s="180" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5477,12 +5475,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="243"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="175"/>
-      <c r="K21" s="177"/>
-      <c r="L21" s="179"/>
-      <c r="M21" s="172"/>
+      <c r="H21" s="242"/>
+      <c r="I21" s="171"/>
+      <c r="J21" s="174"/>
+      <c r="K21" s="176"/>
+      <c r="L21" s="178"/>
+      <c r="M21" s="171"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B22" s="82">
@@ -5508,12 +5506,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="243"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="175"/>
-      <c r="K22" s="177"/>
-      <c r="L22" s="179"/>
-      <c r="M22" s="172"/>
+      <c r="H22" s="242"/>
+      <c r="I22" s="171"/>
+      <c r="J22" s="174"/>
+      <c r="K22" s="176"/>
+      <c r="L22" s="178"/>
+      <c r="M22" s="171"/>
     </row>
     <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B23" s="82">
@@ -5539,12 +5537,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="244"/>
-      <c r="I23" s="174"/>
-      <c r="J23" s="176"/>
-      <c r="K23" s="178"/>
-      <c r="L23" s="180"/>
-      <c r="M23" s="174"/>
+      <c r="H23" s="243"/>
+      <c r="I23" s="173"/>
+      <c r="J23" s="175"/>
+      <c r="K23" s="177"/>
+      <c r="L23" s="179"/>
+      <c r="M23" s="173"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
@@ -5570,7 +5568,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="219" t="s">
+      <c r="H24" s="218" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5613,7 +5611,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="221"/>
+      <c r="H25" s="220"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5654,12 +5652,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="221"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="245"/>
-      <c r="K26" s="247"/>
-      <c r="L26" s="249"/>
-      <c r="M26" s="251"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="239"/>
+      <c r="J26" s="244"/>
+      <c r="K26" s="246"/>
+      <c r="L26" s="248"/>
+      <c r="M26" s="250"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5685,12 +5683,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="220"/>
-      <c r="I27" s="241"/>
-      <c r="J27" s="246"/>
-      <c r="K27" s="248"/>
-      <c r="L27" s="250"/>
-      <c r="M27" s="252"/>
+      <c r="H27" s="219"/>
+      <c r="I27" s="240"/>
+      <c r="J27" s="245"/>
+      <c r="K27" s="247"/>
+      <c r="L27" s="249"/>
+      <c r="M27" s="251"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5716,7 +5714,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="219" t="s">
+      <c r="H28" s="218" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5759,7 +5757,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="221"/>
+      <c r="H29" s="220"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5800,7 +5798,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="221"/>
+      <c r="H30" s="220"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5841,7 +5839,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="220"/>
+      <c r="H31" s="219"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5872,7 +5870,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="221" t="s">
+      <c r="H32" s="220" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5916,7 +5914,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="221"/>
+      <c r="H33" s="220"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5958,7 +5956,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="220"/>
+      <c r="H34" s="219"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -6020,7 +6018,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="M18:M19"/>
@@ -6042,6 +6040,7 @@
     <mergeCell ref="K12:K15"/>
     <mergeCell ref="L12:L15"/>
     <mergeCell ref="M12:M15"/>
+    <mergeCell ref="I13:I15"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="H6:H11"/>
     <mergeCell ref="J6:J11"/>
@@ -6073,13 +6072,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="216" t="s">
+      <c r="B2" s="215" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="218"/>
-      <c r="F2" s="186" t="s">
+      <c r="C2" s="216"/>
+      <c r="D2" s="216"/>
+      <c r="E2" s="217"/>
+      <c r="F2" s="185" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6096,7 +6095,7 @@
       <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="187"/>
+      <c r="F3" s="186"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
@@ -6282,30 +6281,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="185" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="262" t="s">
+      <c r="C2" s="261" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="263"/>
-      <c r="E2" s="263"/>
-      <c r="F2" s="263"/>
-      <c r="G2" s="263"/>
-      <c r="H2" s="263"/>
-      <c r="I2" s="263"/>
-      <c r="J2" s="263"/>
-      <c r="K2" s="263"/>
-      <c r="L2" s="263"/>
-      <c r="M2" s="263"/>
-      <c r="N2" s="263"/>
-      <c r="O2" s="263"/>
-      <c r="P2" s="263"/>
-      <c r="Q2" s="263"/>
-      <c r="R2" s="264"/>
+      <c r="D2" s="262"/>
+      <c r="E2" s="262"/>
+      <c r="F2" s="262"/>
+      <c r="G2" s="262"/>
+      <c r="H2" s="262"/>
+      <c r="I2" s="262"/>
+      <c r="J2" s="262"/>
+      <c r="K2" s="262"/>
+      <c r="L2" s="262"/>
+      <c r="M2" s="262"/>
+      <c r="N2" s="262"/>
+      <c r="O2" s="262"/>
+      <c r="P2" s="262"/>
+      <c r="Q2" s="262"/>
+      <c r="R2" s="263"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="187"/>
+      <c r="B3" s="186"/>
       <c r="C3" s="118">
         <v>15</v>
       </c>
@@ -6376,13 +6375,13 @@
       <c r="M4" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="N4" s="256" t="s">
+      <c r="N4" s="255" t="s">
         <v>89</v>
       </c>
-      <c r="O4" s="256"/>
-      <c r="P4" s="256"/>
-      <c r="Q4" s="256"/>
-      <c r="R4" s="257"/>
+      <c r="O4" s="255"/>
+      <c r="P4" s="255"/>
+      <c r="Q4" s="255"/>
+      <c r="R4" s="256"/>
     </row>
     <row r="5" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="89" t="s">
@@ -6396,16 +6395,16 @@
       <c r="H5" s="157"/>
       <c r="I5" s="157"/>
       <c r="J5" s="158"/>
-      <c r="K5" s="258" t="s">
+      <c r="K5" s="257" t="s">
         <v>85</v>
       </c>
-      <c r="L5" s="254"/>
-      <c r="M5" s="254"/>
-      <c r="N5" s="254"/>
-      <c r="O5" s="254"/>
-      <c r="P5" s="254"/>
-      <c r="Q5" s="254"/>
-      <c r="R5" s="255"/>
+      <c r="L5" s="253"/>
+      <c r="M5" s="253"/>
+      <c r="N5" s="253"/>
+      <c r="O5" s="253"/>
+      <c r="P5" s="253"/>
+      <c r="Q5" s="253"/>
+      <c r="R5" s="254"/>
     </row>
     <row r="6" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="89" t="s">
@@ -6419,16 +6418,16 @@
       <c r="H6" s="157"/>
       <c r="I6" s="157"/>
       <c r="J6" s="158"/>
-      <c r="K6" s="258" t="s">
+      <c r="K6" s="257" t="s">
         <v>85</v>
       </c>
-      <c r="L6" s="254"/>
-      <c r="M6" s="254"/>
-      <c r="N6" s="254"/>
-      <c r="O6" s="254"/>
-      <c r="P6" s="254"/>
-      <c r="Q6" s="254"/>
-      <c r="R6" s="255"/>
+      <c r="L6" s="253"/>
+      <c r="M6" s="253"/>
+      <c r="N6" s="253"/>
+      <c r="O6" s="253"/>
+      <c r="P6" s="253"/>
+      <c r="Q6" s="253"/>
+      <c r="R6" s="254"/>
     </row>
     <row r="7" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="89" t="s">
@@ -6442,39 +6441,39 @@
       <c r="H7" s="159"/>
       <c r="I7" s="159"/>
       <c r="J7" s="159"/>
-      <c r="K7" s="259" t="s">
+      <c r="K7" s="258" t="s">
         <v>85</v>
       </c>
-      <c r="L7" s="260"/>
-      <c r="M7" s="260"/>
-      <c r="N7" s="260"/>
-      <c r="O7" s="260"/>
-      <c r="P7" s="260"/>
-      <c r="Q7" s="260"/>
-      <c r="R7" s="261"/>
+      <c r="L7" s="259"/>
+      <c r="M7" s="259"/>
+      <c r="N7" s="259"/>
+      <c r="O7" s="259"/>
+      <c r="P7" s="259"/>
+      <c r="Q7" s="259"/>
+      <c r="R7" s="260"/>
     </row>
     <row r="8" spans="2:18" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="C8" s="253" t="s">
+      <c r="C8" s="252" t="s">
         <v>150</v>
       </c>
-      <c r="D8" s="254"/>
-      <c r="E8" s="254"/>
-      <c r="F8" s="254"/>
-      <c r="G8" s="254"/>
-      <c r="H8" s="254"/>
-      <c r="I8" s="254"/>
-      <c r="J8" s="254"/>
-      <c r="K8" s="254"/>
-      <c r="L8" s="254"/>
-      <c r="M8" s="254"/>
-      <c r="N8" s="254"/>
-      <c r="O8" s="254"/>
-      <c r="P8" s="254"/>
-      <c r="Q8" s="254"/>
-      <c r="R8" s="255"/>
+      <c r="D8" s="253"/>
+      <c r="E8" s="253"/>
+      <c r="F8" s="253"/>
+      <c r="G8" s="253"/>
+      <c r="H8" s="253"/>
+      <c r="I8" s="253"/>
+      <c r="J8" s="253"/>
+      <c r="K8" s="253"/>
+      <c r="L8" s="253"/>
+      <c r="M8" s="253"/>
+      <c r="N8" s="253"/>
+      <c r="O8" s="253"/>
+      <c r="P8" s="253"/>
+      <c r="Q8" s="253"/>
+      <c r="R8" s="254"/>
     </row>
     <row r="9" spans="2:18" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="90" t="s">
@@ -6688,10 +6687,10 @@
   <sheetData>
     <row r="1" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="265" t="s">
+      <c r="B2" s="264" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="266"/>
+      <c r="C2" s="265"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="2:5" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
@@ -6708,7 +6707,7 @@
       <c r="C4" s="133" t="s">
         <v>143</v>
       </c>
-      <c r="D4" s="267" t="s">
+      <c r="D4" s="266" t="s">
         <v>148</v>
       </c>
     </row>
@@ -6717,21 +6716,21 @@
       <c r="C5" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="268"/>
+      <c r="D5" s="267"/>
     </row>
     <row r="6" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B6" s="136"/>
       <c r="C6" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="269"/>
+      <c r="D6" s="268"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="144" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="145"/>
-      <c r="D7" s="270" t="s">
+      <c r="D7" s="269" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6740,14 +6739,14 @@
         <v>142</v>
       </c>
       <c r="C8" s="146"/>
-      <c r="D8" s="271"/>
+      <c r="D8" s="270"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="41" t="s">
         <v>144</v>
       </c>
       <c r="C9" s="146"/>
-      <c r="D9" s="271"/>
+      <c r="D9" s="270"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="147" t="s">
@@ -6756,7 +6755,7 @@
       <c r="C10" s="148" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="271"/>
+      <c r="D10" s="270"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="41" t="s">
@@ -6765,7 +6764,7 @@
       <c r="C11" s="134" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="271"/>
+      <c r="D11" s="270"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -6775,7 +6774,7 @@
       <c r="C12" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="272"/>
+      <c r="D12" s="271"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
finished component placement (lite)
</commit_message>
<xml_diff>
--- a/ax08.xlsx
+++ b/ax08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olive\Desktop\pc project\rlpc\AX08-PC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E438F04A-2EF9-4FAC-B9C8-6B01D22417BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBABCF57-02F9-4BF2-804E-6FB406024E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{9E4BE3C4-600D-4A58-9D6E-A286F07640A8}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="182">
   <si>
     <t>MODE B</t>
   </si>
@@ -1954,9 +1954,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2008,6 +2005,45 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2044,44 +2080,68 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2092,69 +2152,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2194,6 +2191,9 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2254,7 +2254,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2611,19 +2611,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="183"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="187" t="s">
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="182"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="186" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="188"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="185" t="s">
+      <c r="H2" s="187"/>
+      <c r="I2" s="188"/>
+      <c r="J2" s="184" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2652,7 +2652,7 @@
       <c r="I3" s="51" t="s">
         <v>138</v>
       </c>
-      <c r="J3" s="186"/>
+      <c r="J3" s="185"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B4" s="107">
@@ -3258,73 +3258,73 @@
       </c>
     </row>
     <row r="3" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C3" s="199" t="s">
+      <c r="C3" s="211" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="200"/>
-      <c r="E3" s="200"/>
-      <c r="F3" s="200"/>
-      <c r="G3" s="201"/>
-      <c r="H3" s="196" t="s">
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="213"/>
+      <c r="H3" s="208" t="s">
         <v>97</v>
       </c>
-      <c r="I3" s="197"/>
-      <c r="J3" s="198"/>
-      <c r="K3" s="196" t="s">
+      <c r="I3" s="209"/>
+      <c r="J3" s="210"/>
+      <c r="K3" s="208" t="s">
         <v>96</v>
       </c>
-      <c r="L3" s="197"/>
-      <c r="M3" s="197"/>
-      <c r="N3" s="208" t="s">
+      <c r="L3" s="209"/>
+      <c r="M3" s="209"/>
+      <c r="N3" s="195" t="s">
         <v>95</v>
       </c>
-      <c r="O3" s="209"/>
-      <c r="P3" s="210"/>
+      <c r="O3" s="196"/>
+      <c r="P3" s="197"/>
       <c r="Q3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="R3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="S3" s="202" t="s">
+      <c r="S3" s="189" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="203"/>
-      <c r="U3" s="203"/>
-      <c r="V3" s="203"/>
-      <c r="W3" s="203"/>
-      <c r="X3" s="203"/>
-      <c r="Y3" s="203"/>
-      <c r="Z3" s="204"/>
-      <c r="AA3" s="205" t="s">
+      <c r="T3" s="190"/>
+      <c r="U3" s="190"/>
+      <c r="V3" s="190"/>
+      <c r="W3" s="190"/>
+      <c r="X3" s="190"/>
+      <c r="Y3" s="190"/>
+      <c r="Z3" s="191"/>
+      <c r="AA3" s="192" t="s">
         <v>29</v>
       </c>
-      <c r="AB3" s="206"/>
-      <c r="AC3" s="206"/>
-      <c r="AD3" s="206"/>
-      <c r="AE3" s="206"/>
-      <c r="AF3" s="206"/>
-      <c r="AG3" s="206"/>
-      <c r="AH3" s="207"/>
+      <c r="AB3" s="193"/>
+      <c r="AC3" s="193"/>
+      <c r="AD3" s="193"/>
+      <c r="AE3" s="193"/>
+      <c r="AF3" s="193"/>
+      <c r="AG3" s="193"/>
+      <c r="AH3" s="194"/>
     </row>
     <row r="4" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="5" spans="2:34" x14ac:dyDescent="0.45">
-      <c r="B5" s="213" t="s">
+      <c r="B5" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="211" t="s">
+      <c r="C5" s="198" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
-      <c r="H5" s="211"/>
-      <c r="I5" s="211"/>
-      <c r="J5" s="212"/>
+      <c r="D5" s="198"/>
+      <c r="E5" s="198"/>
+      <c r="F5" s="198"/>
+      <c r="G5" s="198"/>
+      <c r="H5" s="198"/>
+      <c r="I5" s="198"/>
+      <c r="J5" s="199"/>
     </row>
     <row r="6" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="214"/>
+      <c r="B6" s="201"/>
       <c r="C6" s="7">
         <v>7</v>
       </c>
@@ -3354,16 +3354,16 @@
       <c r="B7" s="9">
         <v>0</v>
       </c>
-      <c r="C7" s="190" t="s">
+      <c r="C7" s="202" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="191"/>
-      <c r="E7" s="191"/>
-      <c r="F7" s="191"/>
-      <c r="G7" s="191"/>
-      <c r="H7" s="191"/>
-      <c r="I7" s="191"/>
-      <c r="J7" s="192"/>
+      <c r="D7" s="203"/>
+      <c r="E7" s="203"/>
+      <c r="F7" s="203"/>
+      <c r="G7" s="203"/>
+      <c r="H7" s="203"/>
+      <c r="I7" s="203"/>
+      <c r="J7" s="204"/>
     </row>
     <row r="8" spans="2:34" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B8" s="6">
@@ -3373,25 +3373,25 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="193" t="s">
+      <c r="G8" s="205" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="194"/>
-      <c r="I8" s="194"/>
-      <c r="J8" s="195"/>
+      <c r="H8" s="206"/>
+      <c r="I8" s="206"/>
+      <c r="J8" s="207"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C3:G3"/>
     <mergeCell ref="S3:Z3"/>
     <mergeCell ref="AA3:AH3"/>
     <mergeCell ref="N3:P3"/>
     <mergeCell ref="C5:J5"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C3:G3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3419,29 +3419,29 @@
   <sheetData>
     <row r="1" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="235" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="185" t="s">
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="185" t="s">
+      <c r="I2" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="215" t="s">
+      <c r="J2" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="185" t="s">
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="184" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="185" t="s">
+      <c r="N2" s="184" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3464,8 +3464,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -3475,8 +3475,8 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="186"/>
-      <c r="N3" s="186"/>
+      <c r="M3" s="185"/>
+      <c r="N3" s="185"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -3502,7 +3502,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="218" t="s">
+      <c r="H4" s="216" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -3548,7 +3548,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="219"/>
+      <c r="H5" s="215"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -3592,25 +3592,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="220" t="s">
+      <c r="H6" s="214" t="s">
         <v>61</v>
       </c>
       <c r="I6" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="221" t="s">
+      <c r="J6" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="223" t="s">
+      <c r="K6" s="227" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="225" t="s">
+      <c r="L6" s="224" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="233" t="s">
+      <c r="M6" s="229" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="227" t="s">
+      <c r="N6" s="232" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3638,15 +3638,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="220"/>
+      <c r="H7" s="214"/>
       <c r="I7" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="221"/>
-      <c r="K7" s="223"/>
-      <c r="L7" s="225"/>
-      <c r="M7" s="234"/>
-      <c r="N7" s="227"/>
+      <c r="J7" s="218"/>
+      <c r="K7" s="227"/>
+      <c r="L7" s="224"/>
+      <c r="M7" s="230"/>
+      <c r="N7" s="232"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -3672,15 +3672,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
+      <c r="H8" s="214"/>
       <c r="I8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="221"/>
-      <c r="K8" s="223"/>
-      <c r="L8" s="225"/>
-      <c r="M8" s="234"/>
-      <c r="N8" s="227"/>
+      <c r="J8" s="218"/>
+      <c r="K8" s="227"/>
+      <c r="L8" s="224"/>
+      <c r="M8" s="230"/>
+      <c r="N8" s="232"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -3706,15 +3706,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="220"/>
+      <c r="H9" s="214"/>
       <c r="I9" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="221"/>
-      <c r="K9" s="223"/>
-      <c r="L9" s="225"/>
-      <c r="M9" s="234"/>
-      <c r="N9" s="227"/>
+      <c r="J9" s="218"/>
+      <c r="K9" s="227"/>
+      <c r="L9" s="224"/>
+      <c r="M9" s="230"/>
+      <c r="N9" s="232"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -3740,15 +3740,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="220"/>
+      <c r="H10" s="214"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="221"/>
-      <c r="K10" s="223"/>
-      <c r="L10" s="225"/>
-      <c r="M10" s="234"/>
-      <c r="N10" s="227"/>
+      <c r="J10" s="218"/>
+      <c r="K10" s="227"/>
+      <c r="L10" s="224"/>
+      <c r="M10" s="230"/>
+      <c r="N10" s="232"/>
     </row>
     <row r="11" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -3774,15 +3774,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="219"/>
+      <c r="H11" s="215"/>
       <c r="I11" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="222"/>
-      <c r="K11" s="224"/>
-      <c r="L11" s="226"/>
-      <c r="M11" s="235"/>
-      <c r="N11" s="228"/>
+      <c r="J11" s="219"/>
+      <c r="K11" s="228"/>
+      <c r="L11" s="225"/>
+      <c r="M11" s="231"/>
+      <c r="N11" s="233"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -3808,25 +3808,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="218" t="s">
+      <c r="H12" s="216" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="229" t="s">
+      <c r="J12" s="217" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="230" t="s">
+      <c r="K12" s="226" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="231" t="s">
+      <c r="L12" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="218" t="s">
+      <c r="M12" s="216" t="s">
         <v>114</v>
       </c>
-      <c r="N12" s="232" t="s">
+      <c r="N12" s="234" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3854,15 +3854,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="220"/>
+      <c r="H13" s="214"/>
       <c r="I13" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="221"/>
-      <c r="K13" s="223"/>
-      <c r="L13" s="225"/>
-      <c r="M13" s="220"/>
-      <c r="N13" s="227"/>
+      <c r="J13" s="218"/>
+      <c r="K13" s="227"/>
+      <c r="L13" s="224"/>
+      <c r="M13" s="214"/>
+      <c r="N13" s="232"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -3888,15 +3888,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="220"/>
+      <c r="H14" s="214"/>
       <c r="I14" s="91" t="s">
         <v>102</v>
       </c>
-      <c r="J14" s="221"/>
-      <c r="K14" s="223"/>
-      <c r="L14" s="225"/>
-      <c r="M14" s="220"/>
-      <c r="N14" s="227"/>
+      <c r="J14" s="218"/>
+      <c r="K14" s="227"/>
+      <c r="L14" s="224"/>
+      <c r="M14" s="214"/>
+      <c r="N14" s="232"/>
     </row>
     <row r="15" spans="2:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -3922,15 +3922,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="219"/>
+      <c r="H15" s="215"/>
       <c r="I15" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="J15" s="222"/>
-      <c r="K15" s="224"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="219"/>
-      <c r="N15" s="228"/>
+      <c r="J15" s="219"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="225"/>
+      <c r="M15" s="215"/>
+      <c r="N15" s="233"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -3956,22 +3956,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="218" t="s">
+      <c r="H16" s="216" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="229" t="s">
+      <c r="J16" s="217" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="236" t="s">
+      <c r="K16" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="231" t="s">
+      <c r="L16" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="M16" s="218" t="s">
+      <c r="M16" s="216" t="s">
         <v>114</v>
       </c>
       <c r="N16" s="76" t="s">
@@ -4002,14 +4002,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="220"/>
+      <c r="H17" s="214"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="221"/>
-      <c r="K17" s="237"/>
-      <c r="L17" s="225"/>
-      <c r="M17" s="220"/>
+      <c r="J17" s="218"/>
+      <c r="K17" s="221"/>
+      <c r="L17" s="224"/>
+      <c r="M17" s="214"/>
       <c r="N17" s="75" t="s">
         <v>105</v>
       </c>
@@ -4038,14 +4038,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="220"/>
+      <c r="H18" s="214"/>
       <c r="I18" s="71" t="s">
         <v>49</v>
       </c>
-      <c r="J18" s="221"/>
-      <c r="K18" s="237"/>
-      <c r="L18" s="225"/>
-      <c r="M18" s="220"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="221"/>
+      <c r="L18" s="224"/>
+      <c r="M18" s="214"/>
       <c r="N18" s="75" t="s">
         <v>107</v>
       </c>
@@ -4074,14 +4074,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="219"/>
+      <c r="H19" s="215"/>
       <c r="I19" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="222"/>
-      <c r="K19" s="238"/>
-      <c r="L19" s="226"/>
-      <c r="M19" s="219"/>
+      <c r="J19" s="219"/>
+      <c r="K19" s="222"/>
+      <c r="L19" s="225"/>
+      <c r="M19" s="215"/>
       <c r="N19" s="45" t="s">
         <v>108</v>
       </c>
@@ -4111,22 +4111,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="218" t="s">
+      <c r="H20" s="216" t="s">
         <v>57</v>
       </c>
       <c r="I20" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="J20" s="229" t="s">
+      <c r="J20" s="217" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="230" t="s">
+      <c r="K20" s="226" t="s">
         <v>18</v>
       </c>
-      <c r="L20" s="231" t="s">
+      <c r="L20" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="233" t="s">
+      <c r="M20" s="229" t="s">
         <v>113</v>
       </c>
       <c r="N20" s="42" t="s">
@@ -4157,14 +4157,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="220"/>
+      <c r="H21" s="214"/>
       <c r="I21" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="221"/>
-      <c r="K21" s="223"/>
-      <c r="L21" s="225"/>
-      <c r="M21" s="234"/>
+      <c r="J21" s="218"/>
+      <c r="K21" s="227"/>
+      <c r="L21" s="224"/>
+      <c r="M21" s="230"/>
       <c r="N21" s="75" t="s">
         <v>99</v>
       </c>
@@ -4193,14 +4193,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="220"/>
+      <c r="H22" s="214"/>
       <c r="I22" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="221"/>
-      <c r="K22" s="223"/>
-      <c r="L22" s="225"/>
-      <c r="M22" s="234"/>
+      <c r="J22" s="218"/>
+      <c r="K22" s="227"/>
+      <c r="L22" s="224"/>
+      <c r="M22" s="230"/>
       <c r="N22" s="75" t="s">
         <v>100</v>
       </c>
@@ -4229,14 +4229,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="219"/>
+      <c r="H23" s="215"/>
       <c r="I23" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="J23" s="222"/>
-      <c r="K23" s="224"/>
-      <c r="L23" s="226"/>
-      <c r="M23" s="235"/>
+      <c r="J23" s="219"/>
+      <c r="K23" s="228"/>
+      <c r="L23" s="225"/>
+      <c r="M23" s="231"/>
       <c r="N23" s="42" t="s">
         <v>101</v>
       </c>
@@ -4265,7 +4265,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="218" t="s">
+      <c r="H24" s="216" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -4311,7 +4311,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="220"/>
+      <c r="H25" s="214"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -4355,7 +4355,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="220"/>
+      <c r="H26" s="214"/>
       <c r="I26" s="105"/>
       <c r="J26" s="139"/>
       <c r="K26" s="140"/>
@@ -4387,7 +4387,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="219"/>
+      <c r="H27" s="215"/>
       <c r="I27" s="98"/>
       <c r="J27" s="136"/>
       <c r="K27" s="137"/>
@@ -4419,7 +4419,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="218" t="s">
+      <c r="H28" s="216" t="s">
         <v>60</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -4465,7 +4465,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="220"/>
+      <c r="H29" s="214"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -4509,7 +4509,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="220"/>
+      <c r="H30" s="214"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -4553,7 +4553,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="219"/>
+      <c r="H31" s="215"/>
       <c r="I31" s="92"/>
       <c r="J31" s="95"/>
       <c r="K31" s="96"/>
@@ -4585,7 +4585,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="220" t="s">
+      <c r="H32" s="214" t="s">
         <v>59</v>
       </c>
       <c r="I32" s="65" t="s">
@@ -4632,7 +4632,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="220"/>
+      <c r="H33" s="214"/>
       <c r="I33" s="71" t="s">
         <v>24</v>
       </c>
@@ -4677,7 +4677,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="219"/>
+      <c r="H34" s="215"/>
       <c r="I34" s="98"/>
       <c r="J34" s="95"/>
       <c r="K34" s="96"/>
@@ -4734,11 +4734,25 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H28:H31"/>
-    <mergeCell ref="H24:H27"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="N6:N11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="N12:N15"/>
+    <mergeCell ref="M6:M11"/>
     <mergeCell ref="K16:K19"/>
     <mergeCell ref="L16:L19"/>
     <mergeCell ref="M16:M19"/>
@@ -4747,25 +4761,11 @@
     <mergeCell ref="K20:K23"/>
     <mergeCell ref="L20:L23"/>
     <mergeCell ref="M20:M23"/>
-    <mergeCell ref="N6:N11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="N12:N15"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H28:H31"/>
+    <mergeCell ref="H24:H27"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="J16:J19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4790,26 +4790,26 @@
   <sheetData>
     <row r="1" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="235" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="185" t="s">
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="236"/>
+      <c r="F2" s="236"/>
+      <c r="G2" s="237"/>
+      <c r="H2" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="185" t="s">
+      <c r="I2" s="184" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="215" t="s">
+      <c r="J2" s="235" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="185" t="s">
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="184" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4832,8 +4832,8 @@
       <c r="G3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="186"/>
-      <c r="I3" s="186"/>
+      <c r="H3" s="185"/>
+      <c r="I3" s="185"/>
       <c r="J3" s="49" t="s">
         <v>3</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="L3" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="186"/>
+      <c r="M3" s="185"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B4" s="81">
@@ -4869,7 +4869,7 @@
         <f>_xlfn.BITAND($B4,1)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="218" t="s">
+      <c r="H4" s="216" t="s">
         <v>45</v>
       </c>
       <c r="I4" s="68" t="s">
@@ -4912,7 +4912,7 @@
         <f t="shared" ref="G5:G35" si="0">_xlfn.BITAND($B5,1)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="219"/>
+      <c r="H5" s="215"/>
       <c r="I5" s="43" t="s">
         <v>3</v>
       </c>
@@ -4953,20 +4953,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H6" s="220" t="s">
+      <c r="H6" s="214" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="172"/>
-      <c r="J6" s="221" t="s">
+      <c r="I6" s="91" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="218" t="s">
         <v>70</v>
       </c>
-      <c r="K6" s="223" t="s">
+      <c r="K6" s="227" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="225" t="s">
+      <c r="L6" s="224" t="s">
         <v>66</v>
       </c>
-      <c r="M6" s="227" t="s">
+      <c r="M6" s="232" t="s">
         <v>71</v>
       </c>
     </row>
@@ -4994,14 +4996,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H7" s="220"/>
-      <c r="I7" s="71" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="221"/>
-      <c r="K7" s="223"/>
-      <c r="L7" s="225"/>
-      <c r="M7" s="227"/>
+      <c r="H7" s="214"/>
+      <c r="I7" s="238"/>
+      <c r="J7" s="218"/>
+      <c r="K7" s="227"/>
+      <c r="L7" s="224"/>
+      <c r="M7" s="232"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B8" s="82">
@@ -5027,14 +5027,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H8" s="220"/>
-      <c r="I8" s="91" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="221"/>
-      <c r="K8" s="223"/>
-      <c r="L8" s="225"/>
-      <c r="M8" s="227"/>
+      <c r="H8" s="214"/>
+      <c r="I8" s="251"/>
+      <c r="J8" s="218"/>
+      <c r="K8" s="227"/>
+      <c r="L8" s="224"/>
+      <c r="M8" s="232"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B9" s="82">
@@ -5060,12 +5058,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H9" s="220"/>
-      <c r="I9" s="172"/>
-      <c r="J9" s="221"/>
-      <c r="K9" s="223"/>
-      <c r="L9" s="225"/>
-      <c r="M9" s="227"/>
+      <c r="H9" s="214"/>
+      <c r="I9" s="272"/>
+      <c r="J9" s="218"/>
+      <c r="K9" s="227"/>
+      <c r="L9" s="224"/>
+      <c r="M9" s="232"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B10" s="82">
@@ -5091,14 +5089,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H10" s="220"/>
+      <c r="H10" s="214"/>
       <c r="I10" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="J10" s="221"/>
-      <c r="K10" s="223"/>
-      <c r="L10" s="225"/>
-      <c r="M10" s="227"/>
+      <c r="J10" s="218"/>
+      <c r="K10" s="227"/>
+      <c r="L10" s="224"/>
+      <c r="M10" s="232"/>
     </row>
     <row r="11" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B11" s="83">
@@ -5124,12 +5122,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H11" s="219"/>
+      <c r="H11" s="215"/>
       <c r="I11" s="105"/>
-      <c r="J11" s="222"/>
-      <c r="K11" s="224"/>
-      <c r="L11" s="226"/>
-      <c r="M11" s="228"/>
+      <c r="J11" s="219"/>
+      <c r="K11" s="228"/>
+      <c r="L11" s="225"/>
+      <c r="M11" s="233"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B12" s="81">
@@ -5155,22 +5153,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H12" s="218" t="s">
+      <c r="H12" s="216" t="s">
         <v>55</v>
       </c>
       <c r="I12" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="229" t="s">
+      <c r="J12" s="217" t="s">
         <v>70</v>
       </c>
-      <c r="K12" s="230" t="s">
+      <c r="K12" s="226" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="231" t="s">
+      <c r="L12" s="223" t="s">
         <v>66</v>
       </c>
-      <c r="M12" s="232" t="s">
+      <c r="M12" s="234" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5198,12 +5196,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H13" s="220"/>
-      <c r="I13" s="239"/>
-      <c r="J13" s="221"/>
-      <c r="K13" s="223"/>
-      <c r="L13" s="225"/>
-      <c r="M13" s="227"/>
+      <c r="H13" s="214"/>
+      <c r="I13" s="238"/>
+      <c r="J13" s="218"/>
+      <c r="K13" s="227"/>
+      <c r="L13" s="224"/>
+      <c r="M13" s="232"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B14" s="82">
@@ -5229,12 +5227,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H14" s="220"/>
-      <c r="I14" s="272"/>
-      <c r="J14" s="221"/>
-      <c r="K14" s="223"/>
-      <c r="L14" s="225"/>
-      <c r="M14" s="227"/>
+      <c r="H14" s="214"/>
+      <c r="I14" s="251"/>
+      <c r="J14" s="218"/>
+      <c r="K14" s="227"/>
+      <c r="L14" s="224"/>
+      <c r="M14" s="232"/>
     </row>
     <row r="15" spans="2:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B15" s="83">
@@ -5260,12 +5258,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H15" s="219"/>
-      <c r="I15" s="240"/>
-      <c r="J15" s="222"/>
-      <c r="K15" s="224"/>
-      <c r="L15" s="226"/>
-      <c r="M15" s="228"/>
+      <c r="H15" s="215"/>
+      <c r="I15" s="239"/>
+      <c r="J15" s="219"/>
+      <c r="K15" s="228"/>
+      <c r="L15" s="225"/>
+      <c r="M15" s="233"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B16" s="81">
@@ -5291,19 +5289,19 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H16" s="218" t="s">
+      <c r="H16" s="216" t="s">
         <v>56</v>
       </c>
       <c r="I16" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="J16" s="229" t="s">
+      <c r="J16" s="217" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="236" t="s">
+      <c r="K16" s="220" t="s">
         <v>64</v>
       </c>
-      <c r="L16" s="231" t="s">
+      <c r="L16" s="223" t="s">
         <v>66</v>
       </c>
       <c r="M16" s="76" t="s">
@@ -5334,13 +5332,13 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H17" s="220"/>
+      <c r="H17" s="214"/>
       <c r="I17" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="221"/>
-      <c r="K17" s="237"/>
-      <c r="L17" s="225"/>
+      <c r="J17" s="218"/>
+      <c r="K17" s="221"/>
+      <c r="L17" s="224"/>
       <c r="M17" s="75" t="s">
         <v>105</v>
       </c>
@@ -5369,12 +5367,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H18" s="220"/>
-      <c r="I18" s="239"/>
-      <c r="J18" s="221"/>
-      <c r="K18" s="237"/>
-      <c r="L18" s="225"/>
-      <c r="M18" s="239"/>
+      <c r="H18" s="214"/>
+      <c r="I18" s="238"/>
+      <c r="J18" s="218"/>
+      <c r="K18" s="221"/>
+      <c r="L18" s="224"/>
+      <c r="M18" s="238"/>
     </row>
     <row r="19" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B19" s="83">
@@ -5400,12 +5398,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H19" s="219"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="222"/>
-      <c r="K19" s="238"/>
-      <c r="L19" s="226"/>
-      <c r="M19" s="240"/>
+      <c r="H19" s="215"/>
+      <c r="I19" s="239"/>
+      <c r="J19" s="219"/>
+      <c r="K19" s="222"/>
+      <c r="L19" s="225"/>
+      <c r="M19" s="239"/>
       <c r="O19" s="1"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.45">
@@ -5432,10 +5430,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="241" t="s">
+      <c r="H20" s="240" t="s">
         <v>179</v>
       </c>
-      <c r="I20" s="181" t="s">
+      <c r="I20" s="180" t="s">
         <v>119</v>
       </c>
       <c r="J20" s="67" t="s">
@@ -5447,7 +5445,7 @@
       <c r="L20" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="M20" s="180" t="s">
+      <c r="M20" s="179" t="s">
         <v>180</v>
       </c>
     </row>
@@ -5475,11 +5473,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H21" s="242"/>
+      <c r="H21" s="241"/>
       <c r="I21" s="171"/>
-      <c r="J21" s="174"/>
-      <c r="K21" s="176"/>
-      <c r="L21" s="178"/>
+      <c r="J21" s="173"/>
+      <c r="K21" s="175"/>
+      <c r="L21" s="177"/>
       <c r="M21" s="171"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.45">
@@ -5506,11 +5504,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H22" s="242"/>
+      <c r="H22" s="241"/>
       <c r="I22" s="171"/>
-      <c r="J22" s="174"/>
-      <c r="K22" s="176"/>
-      <c r="L22" s="178"/>
+      <c r="J22" s="173"/>
+      <c r="K22" s="175"/>
+      <c r="L22" s="177"/>
       <c r="M22" s="171"/>
     </row>
     <row r="23" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
@@ -5537,12 +5535,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H23" s="243"/>
-      <c r="I23" s="173"/>
-      <c r="J23" s="175"/>
-      <c r="K23" s="177"/>
-      <c r="L23" s="179"/>
-      <c r="M23" s="173"/>
+      <c r="H23" s="242"/>
+      <c r="I23" s="172"/>
+      <c r="J23" s="174"/>
+      <c r="K23" s="176"/>
+      <c r="L23" s="178"/>
+      <c r="M23" s="172"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B24" s="81">
@@ -5568,7 +5566,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H24" s="218" t="s">
+      <c r="H24" s="216" t="s">
         <v>58</v>
       </c>
       <c r="I24" s="65" t="s">
@@ -5611,7 +5609,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H25" s="220"/>
+      <c r="H25" s="214"/>
       <c r="I25" s="71" t="s">
         <v>46</v>
       </c>
@@ -5652,12 +5650,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="220"/>
-      <c r="I26" s="239"/>
-      <c r="J26" s="244"/>
-      <c r="K26" s="246"/>
-      <c r="L26" s="248"/>
-      <c r="M26" s="250"/>
+      <c r="H26" s="214"/>
+      <c r="I26" s="238"/>
+      <c r="J26" s="243"/>
+      <c r="K26" s="245"/>
+      <c r="L26" s="247"/>
+      <c r="M26" s="249"/>
     </row>
     <row r="27" spans="2:16" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B27" s="83">
@@ -5683,12 +5681,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H27" s="219"/>
-      <c r="I27" s="240"/>
-      <c r="J27" s="245"/>
-      <c r="K27" s="247"/>
-      <c r="L27" s="249"/>
-      <c r="M27" s="251"/>
+      <c r="H27" s="215"/>
+      <c r="I27" s="239"/>
+      <c r="J27" s="244"/>
+      <c r="K27" s="246"/>
+      <c r="L27" s="248"/>
+      <c r="M27" s="250"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.45">
       <c r="B28" s="81">
@@ -5714,7 +5712,7 @@
         <f>_xlfn.BITAND($B28,1)</f>
         <v>0</v>
       </c>
-      <c r="H28" s="218" t="s">
+      <c r="H28" s="216" t="s">
         <v>167</v>
       </c>
       <c r="I28" s="38" t="s">
@@ -5757,7 +5755,7 @@
         <f>_xlfn.BITAND($B29,1)</f>
         <v>1</v>
       </c>
-      <c r="H29" s="220"/>
+      <c r="H29" s="214"/>
       <c r="I29" s="71" t="s">
         <v>52</v>
       </c>
@@ -5798,7 +5796,7 @@
         <f>_xlfn.BITAND($B30,1)</f>
         <v>0</v>
       </c>
-      <c r="H30" s="220"/>
+      <c r="H30" s="214"/>
       <c r="I30" s="71" t="s">
         <v>53</v>
       </c>
@@ -5839,7 +5837,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H31" s="219"/>
+      <c r="H31" s="215"/>
       <c r="I31" s="92"/>
       <c r="J31" s="166"/>
       <c r="K31" s="167"/>
@@ -5870,7 +5868,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H32" s="220" t="s">
+      <c r="H32" s="214" t="s">
         <v>168</v>
       </c>
       <c r="I32" s="38" t="s">
@@ -5914,7 +5912,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="H33" s="220"/>
+      <c r="H33" s="214"/>
       <c r="I33" s="71" t="s">
         <v>52</v>
       </c>
@@ -5956,7 +5954,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="219"/>
+      <c r="H34" s="215"/>
       <c r="I34" s="71" t="s">
         <v>53</v>
       </c>
@@ -6018,7 +6016,25 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H11"/>
+    <mergeCell ref="J6:J11"/>
+    <mergeCell ref="K6:K11"/>
+    <mergeCell ref="L6:L11"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="M6:M11"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="M12:M15"/>
+    <mergeCell ref="I13:I15"/>
     <mergeCell ref="H32:H34"/>
     <mergeCell ref="I18:I19"/>
     <mergeCell ref="M18:M19"/>
@@ -6034,23 +6050,6 @@
     <mergeCell ref="M26:M27"/>
     <mergeCell ref="H24:H27"/>
     <mergeCell ref="H28:H31"/>
-    <mergeCell ref="M6:M11"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="M12:M15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H11"/>
-    <mergeCell ref="J6:J11"/>
-    <mergeCell ref="K6:K11"/>
-    <mergeCell ref="L6:L11"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6072,13 +6071,13 @@
   <sheetData>
     <row r="1" spans="2:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:6" x14ac:dyDescent="0.45">
-      <c r="B2" s="215" t="s">
+      <c r="B2" s="235" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="185" t="s">
+      <c r="C2" s="236"/>
+      <c r="D2" s="236"/>
+      <c r="E2" s="237"/>
+      <c r="F2" s="184" t="s">
         <v>32</v>
       </c>
     </row>
@@ -6095,7 +6094,7 @@
       <c r="E3" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="186"/>
+      <c r="F3" s="185"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B4" s="13">
@@ -6281,7 +6280,7 @@
   <sheetData>
     <row r="1" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="184" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="261" t="s">
@@ -6304,7 +6303,7 @@
       <c r="R2" s="263"/>
     </row>
     <row r="3" spans="2:18" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="186"/>
+      <c r="B3" s="185"/>
       <c r="C3" s="118">
         <v>15</v>
       </c>

</xml_diff>